<commit_message>
Data tagged for P4
</commit_message>
<xml_diff>
--- a/Data/exp2-consolidated.xlsx
+++ b/Data/exp2-consolidated.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3143" uniqueCount="1032">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4007" uniqueCount="1245">
   <si>
     <t>Ticks</t>
   </si>
@@ -3112,6 +3112,645 @@
   </si>
   <si>
     <t>0.0558</t>
+  </si>
+  <si>
+    <t>635138256417378553</t>
+  </si>
+  <si>
+    <t>22034.2603</t>
+  </si>
+  <si>
+    <t>635138256587538286</t>
+  </si>
+  <si>
+    <t>14670.8392</t>
+  </si>
+  <si>
+    <t>635138256685303878</t>
+  </si>
+  <si>
+    <t>7768.4444</t>
+  </si>
+  <si>
+    <t>635138256832742311</t>
+  </si>
+  <si>
+    <t>11811.6756</t>
+  </si>
+  <si>
+    <t>635138256980580766</t>
+  </si>
+  <si>
+    <t>10979.628</t>
+  </si>
+  <si>
+    <t>635138257137779758</t>
+  </si>
+  <si>
+    <t>13451.7694</t>
+  </si>
+  <si>
+    <t>635138257262016864</t>
+  </si>
+  <si>
+    <t>10907.6239</t>
+  </si>
+  <si>
+    <t>635138257383693823</t>
+  </si>
+  <si>
+    <t>9971.5703</t>
+  </si>
+  <si>
+    <t>635138257474739031</t>
+  </si>
+  <si>
+    <t>8000.4576</t>
+  </si>
+  <si>
+    <t>635138257725093350</t>
+  </si>
+  <si>
+    <t>24314.3907</t>
+  </si>
+  <si>
+    <t>635138258039011305</t>
+  </si>
+  <si>
+    <t>26639.5237</t>
+  </si>
+  <si>
+    <t>635138258225171953</t>
+  </si>
+  <si>
+    <t>16427.9396</t>
+  </si>
+  <si>
+    <t>635138258381210878</t>
+  </si>
+  <si>
+    <t>12731.7282</t>
+  </si>
+  <si>
+    <t>635138258555860867</t>
+  </si>
+  <si>
+    <t>15144.8662</t>
+  </si>
+  <si>
+    <t>635138258741121464</t>
+  </si>
+  <si>
+    <t>16674.9538</t>
+  </si>
+  <si>
+    <t>635138258899520523</t>
+  </si>
+  <si>
+    <t>14026.8022</t>
+  </si>
+  <si>
+    <t>635138259039768545</t>
+  </si>
+  <si>
+    <t>12263.7014</t>
+  </si>
+  <si>
+    <t>635138259299803418</t>
+  </si>
+  <si>
+    <t>16184.9257</t>
+  </si>
+  <si>
+    <t>635138259450482037</t>
+  </si>
+  <si>
+    <t>6515.3727</t>
+  </si>
+  <si>
+    <t>635138259612801321</t>
+  </si>
+  <si>
+    <t>10275.5878</t>
+  </si>
+  <si>
+    <t>635138259987402747</t>
+  </si>
+  <si>
+    <t>8346.4774</t>
+  </si>
+  <si>
+    <t>635138260067277315</t>
+  </si>
+  <si>
+    <t>5396.3086</t>
+  </si>
+  <si>
+    <t>635138260150182057</t>
+  </si>
+  <si>
+    <t>4930.282</t>
+  </si>
+  <si>
+    <t>635138260224606314</t>
+  </si>
+  <si>
+    <t>5560.318</t>
+  </si>
+  <si>
+    <t>635138260278959423</t>
+  </si>
+  <si>
+    <t>3435.1965</t>
+  </si>
+  <si>
+    <t>635138260362574205</t>
+  </si>
+  <si>
+    <t>6249.3574</t>
+  </si>
+  <si>
+    <t>635138260497111900</t>
+  </si>
+  <si>
+    <t>11102.635</t>
+  </si>
+  <si>
+    <t>635138260657551077</t>
+  </si>
+  <si>
+    <t>13659.7813</t>
+  </si>
+  <si>
+    <t>635138260865712983</t>
+  </si>
+  <si>
+    <t>12935.7399</t>
+  </si>
+  <si>
+    <t>635138260982309652</t>
+  </si>
+  <si>
+    <t>7996.4574</t>
+  </si>
+  <si>
+    <t>635138261090225825</t>
+  </si>
+  <si>
+    <t>8875.5077</t>
+  </si>
+  <si>
+    <t>635138261232153942</t>
+  </si>
+  <si>
+    <t>11288.6456</t>
+  </si>
+  <si>
+    <t>635138261402623693</t>
+  </si>
+  <si>
+    <t>635138261669668967</t>
+  </si>
+  <si>
+    <t>22700.2984</t>
+  </si>
+  <si>
+    <t>635138262209819862</t>
+  </si>
+  <si>
+    <t>44695.5565</t>
+  </si>
+  <si>
+    <t>635138262478305218</t>
+  </si>
+  <si>
+    <t>18376.051</t>
+  </si>
+  <si>
+    <t>635138262712898636</t>
+  </si>
+  <si>
+    <t>10015.5728</t>
+  </si>
+  <si>
+    <t>635138262806934015</t>
+  </si>
+  <si>
+    <t>6259.358</t>
+  </si>
+  <si>
+    <t>635138262898379245</t>
+  </si>
+  <si>
+    <t>5607.3207</t>
+  </si>
+  <si>
+    <t>635138262999655038</t>
+  </si>
+  <si>
+    <t>7231.4136</t>
+  </si>
+  <si>
+    <t>635138263070979117</t>
+  </si>
+  <si>
+    <t>4843.277</t>
+  </si>
+  <si>
+    <t>635138263174945064</t>
+  </si>
+  <si>
+    <t>5552.3176</t>
+  </si>
+  <si>
+    <t>635138263251099420</t>
+  </si>
+  <si>
+    <t>5620.3215</t>
+  </si>
+  <si>
+    <t>635138263350415100</t>
+  </si>
+  <si>
+    <t>7718.4415</t>
+  </si>
+  <si>
+    <t>635138263438130117</t>
+  </si>
+  <si>
+    <t>6475.3704</t>
+  </si>
+  <si>
+    <t>635138264197913574</t>
+  </si>
+  <si>
+    <t>15561.8901</t>
+  </si>
+  <si>
+    <t>635138264401805236</t>
+  </si>
+  <si>
+    <t>6535.3738</t>
+  </si>
+  <si>
+    <t>635138264483209892</t>
+  </si>
+  <si>
+    <t>3576.2045</t>
+  </si>
+  <si>
+    <t>635138264536882962</t>
+  </si>
+  <si>
+    <t>3579.2047</t>
+  </si>
+  <si>
+    <t>635138264615437455</t>
+  </si>
+  <si>
+    <t>4390.2511</t>
+  </si>
+  <si>
+    <t>635138264709482834</t>
+  </si>
+  <si>
+    <t>5955.3406</t>
+  </si>
+  <si>
+    <t>635138264801968124</t>
+  </si>
+  <si>
+    <t>5164.2954</t>
+  </si>
+  <si>
+    <t>635138264871402096</t>
+  </si>
+  <si>
+    <t>4963.2839</t>
+  </si>
+  <si>
+    <t>635138264938405928</t>
+  </si>
+  <si>
+    <t>4396.2515</t>
+  </si>
+  <si>
+    <t>635138265356039815</t>
+  </si>
+  <si>
+    <t>39575.2636</t>
+  </si>
+  <si>
+    <t>635138265552161033</t>
+  </si>
+  <si>
+    <t>5152.2947</t>
+  </si>
+  <si>
+    <t>635138265652796789</t>
+  </si>
+  <si>
+    <t>635138265754402600</t>
+  </si>
+  <si>
+    <t>6872.393</t>
+  </si>
+  <si>
+    <t>635138265853758283</t>
+  </si>
+  <si>
+    <t>6420.3672</t>
+  </si>
+  <si>
+    <t>635138265937273060</t>
+  </si>
+  <si>
+    <t>6243.3571</t>
+  </si>
+  <si>
+    <t>635138266014067452</t>
+  </si>
+  <si>
+    <t>5503.3147</t>
+  </si>
+  <si>
+    <t>635138266136114433</t>
+  </si>
+  <si>
+    <t>8219.4701</t>
+  </si>
+  <si>
+    <t>635138266219519203</t>
+  </si>
+  <si>
+    <t>5505.3148</t>
+  </si>
+  <si>
+    <t>635138266510715859</t>
+  </si>
+  <si>
+    <t>5984.3423</t>
+  </si>
+  <si>
+    <t>635138266590870444</t>
+  </si>
+  <si>
+    <t>5431.3107</t>
+  </si>
+  <si>
+    <t>635138266657474253</t>
+  </si>
+  <si>
+    <t>4310.2465</t>
+  </si>
+  <si>
+    <t>635138266746749359</t>
+  </si>
+  <si>
+    <t>6445.3686</t>
+  </si>
+  <si>
+    <t>635138266804512663</t>
+  </si>
+  <si>
+    <t>4473.2558</t>
+  </si>
+  <si>
+    <t>635138266877706850</t>
+  </si>
+  <si>
+    <t>5715.3269</t>
+  </si>
+  <si>
+    <t>635138266943110590</t>
+  </si>
+  <si>
+    <t>4056.232</t>
+  </si>
+  <si>
+    <t>635138267019144939</t>
+  </si>
+  <si>
+    <t>6036.3452</t>
+  </si>
+  <si>
+    <t>635138267079628399</t>
+  </si>
+  <si>
+    <t>635138267364264679</t>
+  </si>
+  <si>
+    <t>635138268004221283</t>
+  </si>
+  <si>
+    <t>9747.5576</t>
+  </si>
+  <si>
+    <t>635138268089746174</t>
+  </si>
+  <si>
+    <t>5976.3418</t>
+  </si>
+  <si>
+    <t>635138268193262095</t>
+  </si>
+  <si>
+    <t>7771.4445</t>
+  </si>
+  <si>
+    <t>635138268285497371</t>
+  </si>
+  <si>
+    <t>6755.3864</t>
+  </si>
+  <si>
+    <t>635138268375942544</t>
+  </si>
+  <si>
+    <t>6104.3492</t>
+  </si>
+  <si>
+    <t>635138268469437891</t>
+  </si>
+  <si>
+    <t>7261.4153</t>
+  </si>
+  <si>
+    <t>635138268554982784</t>
+  </si>
+  <si>
+    <t>6396.3658</t>
+  </si>
+  <si>
+    <t>635138268629897069</t>
+  </si>
+  <si>
+    <t>5567.3184</t>
+  </si>
+  <si>
+    <t>635138268682260064</t>
+  </si>
+  <si>
+    <t>3644.2084</t>
+  </si>
+  <si>
+    <t>635138268763174692</t>
+  </si>
+  <si>
+    <t>3635.2079</t>
+  </si>
+  <si>
+    <t>635138268811857477</t>
+  </si>
+  <si>
+    <t>3594.2056</t>
+  </si>
+  <si>
+    <t>635138268887771819</t>
+  </si>
+  <si>
+    <t>3615.2068</t>
+  </si>
+  <si>
+    <t>635138268974416775</t>
+  </si>
+  <si>
+    <t>4380.2506</t>
+  </si>
+  <si>
+    <t>635138269053031271</t>
+  </si>
+  <si>
+    <t>5509.3151</t>
+  </si>
+  <si>
+    <t>635138269104974242</t>
+  </si>
+  <si>
+    <t>3164.181</t>
+  </si>
+  <si>
+    <t>635138269153257004</t>
+  </si>
+  <si>
+    <t>3620.2071</t>
+  </si>
+  <si>
+    <t>635138269215330554</t>
+  </si>
+  <si>
+    <t>3871.2214</t>
+  </si>
+  <si>
+    <t>635138269445733732</t>
+  </si>
+  <si>
+    <t>20736.186</t>
+  </si>
+  <si>
+    <t>635138269570770884</t>
+  </si>
+  <si>
+    <t>6822.3902</t>
+  </si>
+  <si>
+    <t>635138269652685569</t>
+  </si>
+  <si>
+    <t>6779.3877</t>
+  </si>
+  <si>
+    <t>635138269747651001</t>
+  </si>
+  <si>
+    <t>6916.3956</t>
+  </si>
+  <si>
+    <t>635138269839486254</t>
+  </si>
+  <si>
+    <t>7015.4013</t>
+  </si>
+  <si>
+    <t>635138269934461686</t>
+  </si>
+  <si>
+    <t>6511.3724</t>
+  </si>
+  <si>
+    <t>635138270088850517</t>
+  </si>
+  <si>
+    <t>13114.7502</t>
+  </si>
+  <si>
+    <t>635138270212527590</t>
+  </si>
+  <si>
+    <t>10031.5737</t>
+  </si>
+  <si>
+    <t>635138270308283067</t>
+  </si>
+  <si>
+    <t>8055.4607</t>
+  </si>
+  <si>
+    <t>635138270453481372</t>
+  </si>
+  <si>
+    <t>13055.7467</t>
+  </si>
+  <si>
+    <t>635138270595379488</t>
+  </si>
+  <si>
+    <t>9329.5336</t>
+  </si>
+  <si>
+    <t>635138270703765688</t>
+  </si>
+  <si>
+    <t>7880.4508</t>
+  </si>
+  <si>
+    <t>635138270782520192</t>
+  </si>
+  <si>
+    <t>6339.3626</t>
+  </si>
+  <si>
+    <t>635138270834203148</t>
+  </si>
+  <si>
+    <t>3022.1728</t>
+  </si>
+  <si>
+    <t>635138270869805185</t>
+  </si>
+  <si>
+    <t>2184.125</t>
+  </si>
+  <si>
+    <t>635138270919278014</t>
+  </si>
+  <si>
+    <t>2935.1679</t>
+  </si>
+  <si>
+    <t>635138270989212014</t>
+  </si>
+  <si>
+    <t>5241.2998</t>
+  </si>
+  <si>
+    <t>635138271034084581</t>
+  </si>
+  <si>
+    <t>2993.1712</t>
+  </si>
+  <si>
+    <t>P4</t>
   </si>
 </sst>
 </file>
@@ -3119,7 +3758,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -3153,8 +3792,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3458,10 +4097,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L325"/>
+  <dimension ref="A1:L433"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15820,6 +16459,4110 @@
         <v>0</v>
       </c>
       <c r="L325" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A326" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B326" s="1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C326" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D326" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E326" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F326" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G326" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H326" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="I326">
+        <v>2.63E-2</v>
+      </c>
+      <c r="J326">
+        <v>0.42620000000000002</v>
+      </c>
+      <c r="K326">
+        <v>1.6922999999999999</v>
+      </c>
+      <c r="L326">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A327" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B327" s="1" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C327" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D327" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E327" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F327" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G327" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H327" s="1" t="s">
+        <v>1035</v>
+      </c>
+      <c r="I327">
+        <v>0.14130000000000001</v>
+      </c>
+      <c r="J327">
+        <v>0.7056</v>
+      </c>
+      <c r="K327">
+        <v>1.6079000000000001</v>
+      </c>
+      <c r="L327">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A328" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B328" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C328" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D328" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E328" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F328" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G328" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H328" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="I328">
+        <v>9.1600000000000001E-2</v>
+      </c>
+      <c r="J328">
+        <v>0.59789999999999999</v>
+      </c>
+      <c r="K328">
+        <v>1.9328000000000001</v>
+      </c>
+      <c r="L328">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A329" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B329" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C329" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D329" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E329" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F329" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G329" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H329" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="I329">
+        <v>1.95E-2</v>
+      </c>
+      <c r="J329">
+        <v>0.73640000000000005</v>
+      </c>
+      <c r="K329">
+        <v>1.4302999999999999</v>
+      </c>
+      <c r="L329">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A330" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B330" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C330" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D330" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E330" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F330" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G330" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H330" s="1" t="s">
+        <v>1041</v>
+      </c>
+      <c r="I330">
+        <v>0</v>
+      </c>
+      <c r="J330">
+        <v>1.0306</v>
+      </c>
+      <c r="K330">
+        <v>1.9359</v>
+      </c>
+      <c r="L330">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A331" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B331" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C331" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D331" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E331" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F331" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G331" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H331" s="1" t="s">
+        <v>1043</v>
+      </c>
+      <c r="I331">
+        <v>0.1108</v>
+      </c>
+      <c r="J331">
+        <v>5.4615999999999998</v>
+      </c>
+      <c r="K331">
+        <v>1.6561999999999999</v>
+      </c>
+      <c r="L331">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A332" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B332" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C332" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D332" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E332" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F332" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G332" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H332" s="1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="I332">
+        <v>6.7199999999999996E-2</v>
+      </c>
+      <c r="J332">
+        <v>4.1077000000000004</v>
+      </c>
+      <c r="K332">
+        <v>1.4834000000000001</v>
+      </c>
+      <c r="L332">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="333" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A333" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B333" s="1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C333" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D333" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E333" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F333" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G333" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H333" s="1" t="s">
+        <v>1047</v>
+      </c>
+      <c r="I333">
+        <v>0.1168</v>
+      </c>
+      <c r="J333">
+        <v>2.5211999999999999</v>
+      </c>
+      <c r="K333">
+        <v>1.8210999999999999</v>
+      </c>
+      <c r="L333">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A334" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B334" s="1" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C334" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D334" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E334" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F334" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G334" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H334" s="1" t="s">
+        <v>1049</v>
+      </c>
+      <c r="I334">
+        <v>0.11020000000000001</v>
+      </c>
+      <c r="J334">
+        <v>2.5600000000000001E-2</v>
+      </c>
+      <c r="K334">
+        <v>2.7147000000000001</v>
+      </c>
+      <c r="L334">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A335" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B335" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C335" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D335" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E335" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F335" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G335" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H335" s="1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="I335">
+        <v>6.9699999999999998E-2</v>
+      </c>
+      <c r="J335">
+        <v>1.0147999999999999</v>
+      </c>
+      <c r="K335">
+        <v>1.4971000000000001</v>
+      </c>
+      <c r="L335">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A336" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B336" s="1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C336" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D336" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E336" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F336" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G336" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H336" s="1" t="s">
+        <v>1053</v>
+      </c>
+      <c r="I336">
+        <v>0.1444</v>
+      </c>
+      <c r="J336">
+        <v>0.15290000000000001</v>
+      </c>
+      <c r="K336">
+        <v>1.3391999999999999</v>
+      </c>
+      <c r="L336">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="337" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A337" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B337" s="1" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C337" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D337" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E337" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F337" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G337" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H337" s="1" t="s">
+        <v>1055</v>
+      </c>
+      <c r="I337">
+        <v>8.72E-2</v>
+      </c>
+      <c r="J337">
+        <v>0.64859999999999995</v>
+      </c>
+      <c r="K337">
+        <v>1.1444000000000001</v>
+      </c>
+      <c r="L337">
+        <v>1.2999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="338" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A338" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B338" s="1" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D338" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E338" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F338" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G338" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H338" s="1" t="s">
+        <v>1057</v>
+      </c>
+      <c r="I338">
+        <v>0</v>
+      </c>
+      <c r="J338">
+        <v>1.0926</v>
+      </c>
+      <c r="K338">
+        <v>1.3721000000000001</v>
+      </c>
+      <c r="L338">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A339" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B339" s="1" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C339" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D339" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E339" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F339" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G339" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H339" s="1" t="s">
+        <v>1059</v>
+      </c>
+      <c r="I339">
+        <v>7.7399999999999997E-2</v>
+      </c>
+      <c r="J339">
+        <v>0.60240000000000005</v>
+      </c>
+      <c r="K339">
+        <v>1.7454000000000001</v>
+      </c>
+      <c r="L339">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="340" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A340" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B340" s="1" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C340" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D340" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E340" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F340" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G340" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H340" s="1" t="s">
+        <v>1061</v>
+      </c>
+      <c r="I340">
+        <v>9.9599999999999994E-2</v>
+      </c>
+      <c r="J340">
+        <v>0.47549999999999998</v>
+      </c>
+      <c r="K340">
+        <v>1.2408999999999999</v>
+      </c>
+      <c r="L340">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="341" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A341" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B341" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C341" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D341" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E341" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F341" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G341" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H341" s="1" t="s">
+        <v>1063</v>
+      </c>
+      <c r="I341">
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="J341">
+        <v>0.2253</v>
+      </c>
+      <c r="K341">
+        <v>1.4361999999999999</v>
+      </c>
+      <c r="L341">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="342" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A342" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B342" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C342" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D342" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E342" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F342" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G342" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H342" s="1" t="s">
+        <v>1065</v>
+      </c>
+      <c r="I342">
+        <v>0.12379999999999999</v>
+      </c>
+      <c r="J342">
+        <v>0</v>
+      </c>
+      <c r="K342">
+        <v>1.5641</v>
+      </c>
+      <c r="L342">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="343" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A343" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B343" s="1" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C343" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D343" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E343" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F343" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G343" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H343" s="1" t="s">
+        <v>1067</v>
+      </c>
+      <c r="I343">
+        <v>0.17</v>
+      </c>
+      <c r="J343">
+        <v>0.8135</v>
+      </c>
+      <c r="K343">
+        <v>1.7242999999999999</v>
+      </c>
+      <c r="L343">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="344" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A344" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B344" s="1" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C344" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D344" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E344" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F344" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G344" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H344" s="1" t="s">
+        <v>1069</v>
+      </c>
+      <c r="I344">
+        <v>8.3799999999999999E-2</v>
+      </c>
+      <c r="J344">
+        <v>0.186</v>
+      </c>
+      <c r="K344">
+        <v>0</v>
+      </c>
+      <c r="L344">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="345" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A345" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B345" s="1" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C345" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D345" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E345" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F345" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G345" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H345" s="1" t="s">
+        <v>1071</v>
+      </c>
+      <c r="I345">
+        <v>9.5200000000000007E-2</v>
+      </c>
+      <c r="J345">
+        <v>1.4280999999999999</v>
+      </c>
+      <c r="K345">
+        <v>0</v>
+      </c>
+      <c r="L345">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="346" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A346" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B346" s="1" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C346" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D346" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E346" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F346" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G346" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H346" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="I346">
+        <v>0.1716</v>
+      </c>
+      <c r="J346">
+        <v>2.0718000000000001</v>
+      </c>
+      <c r="K346">
+        <v>0</v>
+      </c>
+      <c r="L346">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="347" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A347" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B347" s="1" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C347" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D347" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E347" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F347" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G347" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H347" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="I347">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="J347">
+        <v>3.1701000000000001</v>
+      </c>
+      <c r="K347">
+        <v>0</v>
+      </c>
+      <c r="L347">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="348" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A348" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B348" s="1" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C348" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D348" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E348" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F348" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G348" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H348" s="1" t="s">
+        <v>1077</v>
+      </c>
+      <c r="I348">
+        <v>0.11</v>
+      </c>
+      <c r="J348">
+        <v>0.31740000000000002</v>
+      </c>
+      <c r="K348">
+        <v>0</v>
+      </c>
+      <c r="L348">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="349" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A349" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B349" s="1" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C349" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D349" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E349" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F349" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G349" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H349" s="1" t="s">
+        <v>1079</v>
+      </c>
+      <c r="I349">
+        <v>0.21360000000000001</v>
+      </c>
+      <c r="J349">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="K349">
+        <v>0</v>
+      </c>
+      <c r="L349">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="350" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A350" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B350" s="1" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C350" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D350" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E350" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F350" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G350" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H350" s="1" t="s">
+        <v>1081</v>
+      </c>
+      <c r="I350">
+        <v>0.25609999999999999</v>
+      </c>
+      <c r="J350">
+        <v>2.6223999999999998</v>
+      </c>
+      <c r="K350">
+        <v>0</v>
+      </c>
+      <c r="L350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="351" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A351" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B351" s="1" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C351" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D351" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E351" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F351" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G351" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H351" s="1" t="s">
+        <v>1083</v>
+      </c>
+      <c r="I351">
+        <v>0.17169999999999999</v>
+      </c>
+      <c r="J351">
+        <v>1.0178</v>
+      </c>
+      <c r="K351">
+        <v>0</v>
+      </c>
+      <c r="L351">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="352" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A352" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B352" s="1" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C352" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D352" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E352" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F352" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G352" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H352" s="1" t="s">
+        <v>1085</v>
+      </c>
+      <c r="I352">
+        <v>9.4799999999999995E-2</v>
+      </c>
+      <c r="J352">
+        <v>3.7768999999999999</v>
+      </c>
+      <c r="K352">
+        <v>0</v>
+      </c>
+      <c r="L352">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="353" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A353" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B353" s="1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C353" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D353" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E353" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F353" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G353" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H353" s="1" t="s">
+        <v>1087</v>
+      </c>
+      <c r="I353">
+        <v>0.1711</v>
+      </c>
+      <c r="J353">
+        <v>0.8881</v>
+      </c>
+      <c r="K353">
+        <v>1.0054000000000001</v>
+      </c>
+      <c r="L353">
+        <v>6.5600000000000006E-2</v>
+      </c>
+    </row>
+    <row r="354" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A354" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B354" s="1" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C354" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D354" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E354" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F354" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G354" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H354" s="1" t="s">
+        <v>1089</v>
+      </c>
+      <c r="I354">
+        <v>4.1200000000000001E-2</v>
+      </c>
+      <c r="J354">
+        <v>0.71140000000000003</v>
+      </c>
+      <c r="K354">
+        <v>1.284</v>
+      </c>
+      <c r="L354">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="355" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A355" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B355" s="1" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C355" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D355" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E355" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F355" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G355" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H355" s="1" t="s">
+        <v>1091</v>
+      </c>
+      <c r="I355">
+        <v>0.1832</v>
+      </c>
+      <c r="J355">
+        <v>0.47960000000000003</v>
+      </c>
+      <c r="K355">
+        <v>1.2807999999999999</v>
+      </c>
+      <c r="L355">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="356" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A356" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B356" s="1" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C356" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D356" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E356" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F356" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G356" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H356" s="1" t="s">
+        <v>1093</v>
+      </c>
+      <c r="I356">
+        <v>0.37159999999999999</v>
+      </c>
+      <c r="J356">
+        <v>2.8003</v>
+      </c>
+      <c r="K356">
+        <v>1.4722</v>
+      </c>
+      <c r="L356">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="357" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A357" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B357" s="1" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C357" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D357" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E357" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F357" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G357" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H357" s="1" t="s">
+        <v>1095</v>
+      </c>
+      <c r="I357">
+        <v>8.1900000000000001E-2</v>
+      </c>
+      <c r="J357">
+        <v>1.3152999999999999</v>
+      </c>
+      <c r="K357">
+        <v>1.3479000000000001</v>
+      </c>
+      <c r="L357">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="358" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A358" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B358" s="1" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C358" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D358" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E358" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F358" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G358" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H358" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="I358">
+        <v>0.48220000000000002</v>
+      </c>
+      <c r="J358">
+        <v>3.9510000000000001</v>
+      </c>
+      <c r="K358">
+        <v>1.6936</v>
+      </c>
+      <c r="L358">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="359" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A359" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B359" s="1" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C359" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D359" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E359" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F359" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G359" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H359" s="1" t="s">
+        <v>1098</v>
+      </c>
+      <c r="I359">
+        <v>0.35210000000000002</v>
+      </c>
+      <c r="J359">
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="K359">
+        <v>1.3368</v>
+      </c>
+      <c r="L359">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="360" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A360" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B360" s="1" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C360" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D360" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E360" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F360" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G360" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H360" s="1" t="s">
+        <v>1100</v>
+      </c>
+      <c r="I360">
+        <v>0.1212</v>
+      </c>
+      <c r="J360">
+        <v>2.4529000000000001</v>
+      </c>
+      <c r="K360">
+        <v>1.3162</v>
+      </c>
+      <c r="L360">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="361" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A361" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B361" s="1" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C361" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D361" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E361" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F361" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G361" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H361" s="1" t="s">
+        <v>1102</v>
+      </c>
+      <c r="I361">
+        <v>0.25890000000000002</v>
+      </c>
+      <c r="J361">
+        <v>1.5586</v>
+      </c>
+      <c r="K361">
+        <v>1.1878</v>
+      </c>
+      <c r="L361">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="362" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A362" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B362" s="1" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C362" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D362" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E362" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F362" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G362" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H362" s="1" t="s">
+        <v>1104</v>
+      </c>
+      <c r="I362">
+        <v>0</v>
+      </c>
+      <c r="J362">
+        <v>1.206</v>
+      </c>
+      <c r="K362">
+        <v>0</v>
+      </c>
+      <c r="L362">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="363" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A363" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B363" s="1" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C363" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D363" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E363" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F363" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G363" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H363" s="1" t="s">
+        <v>1106</v>
+      </c>
+      <c r="I363">
+        <v>3.0499999999999999E-2</v>
+      </c>
+      <c r="J363">
+        <v>2.786</v>
+      </c>
+      <c r="K363">
+        <v>0</v>
+      </c>
+      <c r="L363">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="364" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A364" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B364" s="1" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C364" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D364" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E364" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F364" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G364" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H364" s="1" t="s">
+        <v>1108</v>
+      </c>
+      <c r="I364">
+        <v>0.14649999999999999</v>
+      </c>
+      <c r="J364">
+        <v>2.3319999999999999</v>
+      </c>
+      <c r="K364">
+        <v>0</v>
+      </c>
+      <c r="L364">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="365" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A365" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B365" s="1" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C365" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D365" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E365" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F365" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G365" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H365" s="1" t="s">
+        <v>1110</v>
+      </c>
+      <c r="I365">
+        <v>0.1222</v>
+      </c>
+      <c r="J365">
+        <v>1.0911999999999999</v>
+      </c>
+      <c r="K365">
+        <v>0</v>
+      </c>
+      <c r="L365">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="366" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A366" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B366" s="1" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C366" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D366" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E366" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F366" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G366" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H366" s="1" t="s">
+        <v>1112</v>
+      </c>
+      <c r="I366">
+        <v>6.7400000000000002E-2</v>
+      </c>
+      <c r="J366">
+        <v>0.48349999999999999</v>
+      </c>
+      <c r="K366">
+        <v>0</v>
+      </c>
+      <c r="L366">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="367" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A367" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B367" s="1" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C367" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D367" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E367" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F367" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G367" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H367" s="1" t="s">
+        <v>1114</v>
+      </c>
+      <c r="I367">
+        <v>0.1052</v>
+      </c>
+      <c r="J367">
+        <v>2.9767000000000001</v>
+      </c>
+      <c r="K367">
+        <v>0</v>
+      </c>
+      <c r="L367">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="368" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A368" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B368" s="1" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C368" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D368" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E368" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F368" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G368" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H368" s="1" t="s">
+        <v>1116</v>
+      </c>
+      <c r="I368">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="J368">
+        <v>3.145</v>
+      </c>
+      <c r="K368">
+        <v>0</v>
+      </c>
+      <c r="L368">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="369" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A369" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B369" s="1" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C369" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D369" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E369" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F369" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G369" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H369" s="1" t="s">
+        <v>1118</v>
+      </c>
+      <c r="I369">
+        <v>9.6600000000000005E-2</v>
+      </c>
+      <c r="J369">
+        <v>0.73140000000000005</v>
+      </c>
+      <c r="K369">
+        <v>0</v>
+      </c>
+      <c r="L369">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="370" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A370" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B370" s="1" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C370" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D370" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E370" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F370" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G370" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H370" s="1" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I370">
+        <v>0.15629999999999999</v>
+      </c>
+      <c r="J370">
+        <v>2.3504</v>
+      </c>
+      <c r="K370">
+        <v>0</v>
+      </c>
+      <c r="L370">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="371" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A371" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B371" s="1" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C371" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D371" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E371" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F371" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G371" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H371" s="1" t="s">
+        <v>1122</v>
+      </c>
+      <c r="I371">
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="J371">
+        <v>1.6800999999999999</v>
+      </c>
+      <c r="K371">
+        <v>0</v>
+      </c>
+      <c r="L371">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="372" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A372" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B372" s="1" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C372" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D372" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E372" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F372" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G372" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H372" s="1" t="s">
+        <v>1124</v>
+      </c>
+      <c r="I372">
+        <v>8.9800000000000005E-2</v>
+      </c>
+      <c r="J372">
+        <v>0.45540000000000003</v>
+      </c>
+      <c r="K372">
+        <v>0</v>
+      </c>
+      <c r="L372">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="373" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A373" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B373" s="1" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C373" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D373" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E373" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F373" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G373" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H373" s="1" t="s">
+        <v>1126</v>
+      </c>
+      <c r="I373">
+        <v>9.0700000000000003E-2</v>
+      </c>
+      <c r="J373">
+        <v>0.61880000000000002</v>
+      </c>
+      <c r="K373">
+        <v>0</v>
+      </c>
+      <c r="L373">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="374" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A374" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B374" s="1" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C374" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D374" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E374" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F374" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G374" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H374" s="1" t="s">
+        <v>1128</v>
+      </c>
+      <c r="I374">
+        <v>9.2399999999999996E-2</v>
+      </c>
+      <c r="J374">
+        <v>1.1572</v>
+      </c>
+      <c r="K374">
+        <v>0</v>
+      </c>
+      <c r="L374">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="375" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A375" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B375" s="1" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C375" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D375" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E375" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F375" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G375" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H375" s="1" t="s">
+        <v>1130</v>
+      </c>
+      <c r="I375">
+        <v>0.1103</v>
+      </c>
+      <c r="J375">
+        <v>1.0501</v>
+      </c>
+      <c r="K375">
+        <v>0</v>
+      </c>
+      <c r="L375">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="376" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A376" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B376" s="1" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C376" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D376" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E376" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F376" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G376" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H376" s="1" t="s">
+        <v>1132</v>
+      </c>
+      <c r="I376">
+        <v>0.12939999999999999</v>
+      </c>
+      <c r="J376">
+        <v>4.5904999999999996</v>
+      </c>
+      <c r="K376">
+        <v>0</v>
+      </c>
+      <c r="L376">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="377" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A377" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B377" s="1" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C377" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D377" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E377" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F377" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G377" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H377" s="1" t="s">
+        <v>1134</v>
+      </c>
+      <c r="I377">
+        <v>0.1036</v>
+      </c>
+      <c r="J377">
+        <v>3.0394000000000001</v>
+      </c>
+      <c r="K377">
+        <v>0</v>
+      </c>
+      <c r="L377">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="378" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A378" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B378" s="1" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C378" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D378" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E378" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F378" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G378" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H378" s="1" t="s">
+        <v>1136</v>
+      </c>
+      <c r="I378">
+        <v>9.8599999999999993E-2</v>
+      </c>
+      <c r="J378">
+        <v>0.58879999999999999</v>
+      </c>
+      <c r="K378">
+        <v>0</v>
+      </c>
+      <c r="L378">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="379" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A379" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B379" s="1" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C379" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D379" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E379" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F379" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G379" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H379" s="1" t="s">
+        <v>1138</v>
+      </c>
+      <c r="I379">
+        <v>6.4799999999999996E-2</v>
+      </c>
+      <c r="J379">
+        <v>2.1745999999999999</v>
+      </c>
+      <c r="K379">
+        <v>0</v>
+      </c>
+      <c r="L379">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="380" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A380" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B380" s="1" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C380" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D380" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E380" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F380" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G380" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H380" s="1" t="s">
+        <v>1140</v>
+      </c>
+      <c r="I380">
+        <v>0.2616</v>
+      </c>
+      <c r="J380">
+        <v>0</v>
+      </c>
+      <c r="K380">
+        <v>0</v>
+      </c>
+      <c r="L380">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="381" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A381" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B381" s="1" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C381" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D381" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E381" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F381" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G381" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H381" s="1" t="s">
+        <v>1142</v>
+      </c>
+      <c r="I381">
+        <v>0.122</v>
+      </c>
+      <c r="J381">
+        <v>2.3694999999999999</v>
+      </c>
+      <c r="K381">
+        <v>0</v>
+      </c>
+      <c r="L381">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="382" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A382" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B382" s="1" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C382" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D382" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E382" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F382" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G382" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H382" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="I382">
+        <v>0.1762</v>
+      </c>
+      <c r="J382">
+        <v>1.1088</v>
+      </c>
+      <c r="K382">
+        <v>0</v>
+      </c>
+      <c r="L382">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="383" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A383" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B383" s="1" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C383" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D383" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E383" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F383" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G383" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H383" s="1" t="s">
+        <v>1145</v>
+      </c>
+      <c r="I383">
+        <v>7.0099999999999996E-2</v>
+      </c>
+      <c r="J383">
+        <v>1.4202999999999999</v>
+      </c>
+      <c r="K383">
+        <v>0</v>
+      </c>
+      <c r="L383">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="384" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A384" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B384" s="1" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C384" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D384" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E384" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F384" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G384" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H384" s="1" t="s">
+        <v>1147</v>
+      </c>
+      <c r="I384">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="J384">
+        <v>1.9885999999999999</v>
+      </c>
+      <c r="K384">
+        <v>0</v>
+      </c>
+      <c r="L384">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="385" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A385" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B385" s="1" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C385" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D385" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E385" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F385" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G385" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H385" s="1" t="s">
+        <v>1149</v>
+      </c>
+      <c r="I385">
+        <v>7.5499999999999998E-2</v>
+      </c>
+      <c r="J385">
+        <v>0.77739999999999998</v>
+      </c>
+      <c r="K385">
+        <v>0</v>
+      </c>
+      <c r="L385">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="386" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A386" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B386" s="1" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C386" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D386" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E386" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F386" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G386" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H386" s="1" t="s">
+        <v>1151</v>
+      </c>
+      <c r="I386">
+        <v>5.6599999999999998E-2</v>
+      </c>
+      <c r="J386">
+        <v>1.8475999999999999</v>
+      </c>
+      <c r="K386">
+        <v>0</v>
+      </c>
+      <c r="L386">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="387" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A387" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B387" s="1" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C387" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D387" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E387" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F387" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G387" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H387" s="1" t="s">
+        <v>1153</v>
+      </c>
+      <c r="I387">
+        <v>6.5699999999999995E-2</v>
+      </c>
+      <c r="J387">
+        <v>1.3322000000000001</v>
+      </c>
+      <c r="K387">
+        <v>0</v>
+      </c>
+      <c r="L387">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="388" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A388" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B388" s="1" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C388" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D388" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E388" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F388" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G388" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H388" s="1" t="s">
+        <v>1155</v>
+      </c>
+      <c r="I388">
+        <v>0.21790000000000001</v>
+      </c>
+      <c r="J388">
+        <v>4.3510999999999997</v>
+      </c>
+      <c r="K388">
+        <v>0</v>
+      </c>
+      <c r="L388">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="389" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A389" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B389" s="1" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C389" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D389" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E389" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F389" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G389" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H389" s="1" t="s">
+        <v>1157</v>
+      </c>
+      <c r="I389">
+        <v>0.1109</v>
+      </c>
+      <c r="J389">
+        <v>0.82189999999999996</v>
+      </c>
+      <c r="K389">
+        <v>0</v>
+      </c>
+      <c r="L389">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="390" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A390" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B390" s="1" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C390" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D390" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E390" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F390" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G390" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H390" s="1" t="s">
+        <v>1159</v>
+      </c>
+      <c r="I390">
+        <v>8.0500000000000002E-2</v>
+      </c>
+      <c r="J390">
+        <v>1.7269000000000001</v>
+      </c>
+      <c r="K390">
+        <v>0</v>
+      </c>
+      <c r="L390">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="391" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A391" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B391" s="1" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C391" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D391" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E391" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F391" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G391" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H391" s="1" t="s">
+        <v>1161</v>
+      </c>
+      <c r="I391">
+        <v>0.1132</v>
+      </c>
+      <c r="J391">
+        <v>1.2332000000000001</v>
+      </c>
+      <c r="K391">
+        <v>0</v>
+      </c>
+      <c r="L391">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="392" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A392" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B392" s="1" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C392" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D392" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E392" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F392" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G392" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H392" s="1" t="s">
+        <v>1163</v>
+      </c>
+      <c r="I392">
+        <v>5.0799999999999998E-2</v>
+      </c>
+      <c r="J392">
+        <v>0.94040000000000001</v>
+      </c>
+      <c r="K392">
+        <v>0</v>
+      </c>
+      <c r="L392">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="393" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A393" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B393" s="1" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C393" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D393" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E393" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F393" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G393" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H393" s="1" t="s">
+        <v>1165</v>
+      </c>
+      <c r="I393">
+        <v>9.74E-2</v>
+      </c>
+      <c r="J393">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="K393">
+        <v>0</v>
+      </c>
+      <c r="L393">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="394" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A394" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B394" s="1" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C394" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D394" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E394" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F394" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G394" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H394" s="1" t="s">
+        <v>1167</v>
+      </c>
+      <c r="I394">
+        <v>7.2300000000000003E-2</v>
+      </c>
+      <c r="J394">
+        <v>0.80010000000000003</v>
+      </c>
+      <c r="K394">
+        <v>0</v>
+      </c>
+      <c r="L394">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="395" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A395" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B395" s="1" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C395" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D395" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E395" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F395" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G395" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H395" s="1" t="s">
+        <v>1169</v>
+      </c>
+      <c r="I395">
+        <v>5.6300000000000003E-2</v>
+      </c>
+      <c r="J395">
+        <v>2.2926000000000002</v>
+      </c>
+      <c r="K395">
+        <v>0</v>
+      </c>
+      <c r="L395">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="396" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A396" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B396" s="1" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C396" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D396" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E396" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F396" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G396" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H396" s="1" t="s">
+        <v>1171</v>
+      </c>
+      <c r="I396">
+        <v>6.4799999999999996E-2</v>
+      </c>
+      <c r="J396">
+        <v>1.643</v>
+      </c>
+      <c r="K396">
+        <v>0</v>
+      </c>
+      <c r="L396">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="397" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A397" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B397" s="1" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C397" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D397" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E397" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F397" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G397" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H397" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="I397">
+        <v>6.5199999999999994E-2</v>
+      </c>
+      <c r="J397">
+        <v>5.33E-2</v>
+      </c>
+      <c r="K397">
+        <v>0</v>
+      </c>
+      <c r="L397">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="398" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A398" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B398" s="1" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C398" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D398" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E398" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F398" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G398" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H398" s="1" t="s">
+        <v>1102</v>
+      </c>
+      <c r="I398">
+        <v>9.0800000000000006E-2</v>
+      </c>
+      <c r="J398">
+        <v>1.6312</v>
+      </c>
+      <c r="K398">
+        <v>1.3671</v>
+      </c>
+      <c r="L398">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="399" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A399" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B399" s="1" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C399" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D399" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E399" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F399" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G399" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H399" s="1" t="s">
+        <v>1175</v>
+      </c>
+      <c r="I399">
+        <v>0.14480000000000001</v>
+      </c>
+      <c r="J399">
+        <v>2.1507000000000001</v>
+      </c>
+      <c r="K399">
+        <v>1.3156000000000001</v>
+      </c>
+      <c r="L399">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="400" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A400" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B400" s="1" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C400" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D400" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E400" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F400" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G400" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H400" s="1" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I400">
+        <v>0.14419999999999999</v>
+      </c>
+      <c r="J400">
+        <v>1.1678999999999999</v>
+      </c>
+      <c r="K400">
+        <v>1.2214</v>
+      </c>
+      <c r="L400">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="401" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A401" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B401" s="1" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C401" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D401" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E401" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F401" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G401" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H401" s="1" t="s">
+        <v>1179</v>
+      </c>
+      <c r="I401">
+        <v>0.13550000000000001</v>
+      </c>
+      <c r="J401">
+        <v>2.3978000000000002</v>
+      </c>
+      <c r="K401">
+        <v>1.8312999999999999</v>
+      </c>
+      <c r="L401">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="402" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A402" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B402" s="1" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C402" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D402" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E402" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F402" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G402" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H402" s="1" t="s">
+        <v>1181</v>
+      </c>
+      <c r="I402">
+        <v>0.16789999999999999</v>
+      </c>
+      <c r="J402">
+        <v>2.1779999999999999</v>
+      </c>
+      <c r="K402">
+        <v>1.4773000000000001</v>
+      </c>
+      <c r="L402">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="403" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A403" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B403" s="1" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C403" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D403" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E403" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F403" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G403" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H403" s="1" t="s">
+        <v>1183</v>
+      </c>
+      <c r="I403">
+        <v>0.16850000000000001</v>
+      </c>
+      <c r="J403">
+        <v>0.23780000000000001</v>
+      </c>
+      <c r="K403">
+        <v>1.4160999999999999</v>
+      </c>
+      <c r="L403">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="404" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A404" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B404" s="1" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C404" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D404" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E404" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F404" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G404" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H404" s="1" t="s">
+        <v>1185</v>
+      </c>
+      <c r="I404">
+        <v>0.14030000000000001</v>
+      </c>
+      <c r="J404">
+        <v>1.1237999999999999</v>
+      </c>
+      <c r="K404">
+        <v>1.4279999999999999</v>
+      </c>
+      <c r="L404">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="405" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A405" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B405" s="1" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C405" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D405" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E405" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F405" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G405" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H405" s="1" t="s">
+        <v>1187</v>
+      </c>
+      <c r="I405">
+        <v>9.11E-2</v>
+      </c>
+      <c r="J405">
+        <v>0.53539999999999999</v>
+      </c>
+      <c r="K405">
+        <v>1.1948000000000001</v>
+      </c>
+      <c r="L405">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="406" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A406" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B406" s="1" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C406" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D406" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E406" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F406" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G406" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H406" s="1" t="s">
+        <v>1189</v>
+      </c>
+      <c r="I406">
+        <v>0.14380000000000001</v>
+      </c>
+      <c r="J406">
+        <v>3.9823</v>
+      </c>
+      <c r="K406">
+        <v>1.7808999999999999</v>
+      </c>
+      <c r="L406">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="407" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A407" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B407" s="1" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C407" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D407" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E407" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F407" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G407" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H407" s="1" t="s">
+        <v>1191</v>
+      </c>
+      <c r="I407">
+        <v>0.12709999999999999</v>
+      </c>
+      <c r="J407">
+        <v>0.46139999999999998</v>
+      </c>
+      <c r="K407">
+        <v>0</v>
+      </c>
+      <c r="L407">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="408" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A408" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B408" s="1" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C408" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D408" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E408" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F408" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G408" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H408" s="1" t="s">
+        <v>1193</v>
+      </c>
+      <c r="I408">
+        <v>9.01E-2</v>
+      </c>
+      <c r="J408">
+        <v>1.089</v>
+      </c>
+      <c r="K408">
+        <v>0</v>
+      </c>
+      <c r="L408">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="409" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A409" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B409" s="1" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C409" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D409" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E409" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F409" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G409" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H409" s="1" t="s">
+        <v>1195</v>
+      </c>
+      <c r="I409">
+        <v>0.1368</v>
+      </c>
+      <c r="J409">
+        <v>5.1200000000000002E-2</v>
+      </c>
+      <c r="K409">
+        <v>0</v>
+      </c>
+      <c r="L409">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="410" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A410" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B410" s="1" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C410" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D410" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E410" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F410" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G410" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H410" s="1" t="s">
+        <v>1197</v>
+      </c>
+      <c r="I410">
+        <v>0.115</v>
+      </c>
+      <c r="J410">
+        <v>0.1517</v>
+      </c>
+      <c r="K410">
+        <v>0</v>
+      </c>
+      <c r="L410">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="411" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A411" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B411" s="1" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C411" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D411" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E411" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F411" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G411" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H411" s="1" t="s">
+        <v>1199</v>
+      </c>
+      <c r="I411">
+        <v>0.15140000000000001</v>
+      </c>
+      <c r="J411">
+        <v>2.0722</v>
+      </c>
+      <c r="K411">
+        <v>0</v>
+      </c>
+      <c r="L411">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="412" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A412" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B412" s="1" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C412" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D412" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E412" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F412" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G412" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H412" s="1" t="s">
+        <v>1201</v>
+      </c>
+      <c r="I412">
+        <v>0.1134</v>
+      </c>
+      <c r="J412">
+        <v>2.1501999999999999</v>
+      </c>
+      <c r="K412">
+        <v>0</v>
+      </c>
+      <c r="L412">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="413" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A413" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B413" s="1" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C413" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D413" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E413" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F413" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G413" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H413" s="1" t="s">
+        <v>1203</v>
+      </c>
+      <c r="I413">
+        <v>5.0299999999999997E-2</v>
+      </c>
+      <c r="J413">
+        <v>0.64559999999999995</v>
+      </c>
+      <c r="K413">
+        <v>0</v>
+      </c>
+      <c r="L413">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="414" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A414" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B414" s="1" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C414" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D414" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E414" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F414" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G414" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H414" s="1" t="s">
+        <v>1205</v>
+      </c>
+      <c r="I414">
+        <v>9.0499999999999997E-2</v>
+      </c>
+      <c r="J414">
+        <v>0.7087</v>
+      </c>
+      <c r="K414">
+        <v>0</v>
+      </c>
+      <c r="L414">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="415" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A415" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B415" s="1" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C415" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D415" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E415" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F415" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G415" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H415" s="1" t="s">
+        <v>1207</v>
+      </c>
+      <c r="I415">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="J415">
+        <v>1.3285</v>
+      </c>
+      <c r="K415">
+        <v>0</v>
+      </c>
+      <c r="L415">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="416" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A416" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B416" s="1" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C416" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D416" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E416" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F416" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G416" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H416" s="1" t="s">
+        <v>1209</v>
+      </c>
+      <c r="I416">
+        <v>9.5899999999999999E-2</v>
+      </c>
+      <c r="J416">
+        <v>6.7939999999999996</v>
+      </c>
+      <c r="K416">
+        <v>6.4991000000000003</v>
+      </c>
+      <c r="L416">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="417" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A417" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B417" s="1" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C417" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D417" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E417" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F417" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G417" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H417" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="I417">
+        <v>0.20880000000000001</v>
+      </c>
+      <c r="J417">
+        <v>3.3809999999999998</v>
+      </c>
+      <c r="K417">
+        <v>1.9061999999999999</v>
+      </c>
+      <c r="L417">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="418" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A418" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B418" s="1" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C418" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D418" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E418" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F418" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G418" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H418" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="I418">
+        <v>7.3800000000000004E-2</v>
+      </c>
+      <c r="J418">
+        <v>2.6599999999999999E-2</v>
+      </c>
+      <c r="K418">
+        <v>1.7290000000000001</v>
+      </c>
+      <c r="L418">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="419" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A419" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B419" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C419" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D419" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E419" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F419" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G419" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H419" s="1" t="s">
+        <v>1215</v>
+      </c>
+      <c r="I419">
+        <v>0.17910000000000001</v>
+      </c>
+      <c r="J419">
+        <v>2.5103</v>
+      </c>
+      <c r="K419">
+        <v>1.8487</v>
+      </c>
+      <c r="L419">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="420" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A420" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B420" s="1" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C420" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D420" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E420" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F420" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G420" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H420" s="1" t="s">
+        <v>1217</v>
+      </c>
+      <c r="I420">
+        <v>0.18160000000000001</v>
+      </c>
+      <c r="J420">
+        <v>4.4736000000000002</v>
+      </c>
+      <c r="K420">
+        <v>1.8601000000000001</v>
+      </c>
+      <c r="L420">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="421" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A421" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B421" s="1" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C421" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D421" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E421" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F421" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G421" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H421" s="1" t="s">
+        <v>1219</v>
+      </c>
+      <c r="I421">
+        <v>0.13439999999999999</v>
+      </c>
+      <c r="J421">
+        <v>4.3704999999999998</v>
+      </c>
+      <c r="K421">
+        <v>1.6017999999999999</v>
+      </c>
+      <c r="L421">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="422" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A422" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B422" s="1" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C422" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D422" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E422" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F422" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G422" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H422" s="1" t="s">
+        <v>1221</v>
+      </c>
+      <c r="I422">
+        <v>3.56E-2</v>
+      </c>
+      <c r="J422">
+        <v>0.46189999999999998</v>
+      </c>
+      <c r="K422">
+        <v>1.8275999999999999</v>
+      </c>
+      <c r="L422">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="423" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A423" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B423" s="1" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C423" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D423" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E423" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F423" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G423" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H423" s="1" t="s">
+        <v>1223</v>
+      </c>
+      <c r="I423">
+        <v>0.10580000000000001</v>
+      </c>
+      <c r="J423">
+        <v>2.4935</v>
+      </c>
+      <c r="K423">
+        <v>1.3627</v>
+      </c>
+      <c r="L423">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="424" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A424" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B424" s="1" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C424" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D424" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E424" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F424" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G424" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H424" s="1" t="s">
+        <v>1225</v>
+      </c>
+      <c r="I424">
+        <v>7.0900000000000005E-2</v>
+      </c>
+      <c r="J424">
+        <v>0.3548</v>
+      </c>
+      <c r="K424">
+        <v>1.7261</v>
+      </c>
+      <c r="L424">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="425" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A425" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B425" s="1" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C425" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D425" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E425" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F425" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G425" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H425" s="1" t="s">
+        <v>1227</v>
+      </c>
+      <c r="I425">
+        <v>3.5499999999999997E-2</v>
+      </c>
+      <c r="J425">
+        <v>2.8902999999999999</v>
+      </c>
+      <c r="K425">
+        <v>3.9297</v>
+      </c>
+      <c r="L425">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="426" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A426" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B426" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C426" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D426" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E426" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F426" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G426" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H426" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="I426">
+        <v>0.1419</v>
+      </c>
+      <c r="J426">
+        <v>10.9442</v>
+      </c>
+      <c r="K426">
+        <v>3.7841999999999998</v>
+      </c>
+      <c r="L426">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="427" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A427" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B427" s="1" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C427" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D427" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E427" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F427" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G427" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H427" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="I427">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="J427">
+        <v>4.1052</v>
+      </c>
+      <c r="K427">
+        <v>2.7521</v>
+      </c>
+      <c r="L427">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="428" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A428" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B428" s="1" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C428" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D428" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E428" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F428" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G428" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H428" s="1" t="s">
+        <v>1233</v>
+      </c>
+      <c r="I428">
+        <v>7.8600000000000003E-2</v>
+      </c>
+      <c r="J428">
+        <v>3.7732999999999999</v>
+      </c>
+      <c r="K428">
+        <v>4.0366</v>
+      </c>
+      <c r="L428">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="429" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A429" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B429" s="1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C429" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D429" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E429" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F429" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G429" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H429" s="1" t="s">
+        <v>1235</v>
+      </c>
+      <c r="I429">
+        <v>9.4899999999999998E-2</v>
+      </c>
+      <c r="J429">
+        <v>0.13750000000000001</v>
+      </c>
+      <c r="K429">
+        <v>3.9352999999999998</v>
+      </c>
+      <c r="L429">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="430" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A430" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B430" s="1" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C430" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D430" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E430" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F430" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G430" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H430" s="1" t="s">
+        <v>1237</v>
+      </c>
+      <c r="I430">
+        <v>0.12939999999999999</v>
+      </c>
+      <c r="J430">
+        <v>2.8614999999999999</v>
+      </c>
+      <c r="K430">
+        <v>3.9247999999999998</v>
+      </c>
+      <c r="L430">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="431" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A431" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B431" s="1" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C431" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D431" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E431" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F431" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G431" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H431" s="1" t="s">
+        <v>1239</v>
+      </c>
+      <c r="I431">
+        <v>9.4899999999999998E-2</v>
+      </c>
+      <c r="J431">
+        <v>0.89990000000000003</v>
+      </c>
+      <c r="K431">
+        <v>3.8816000000000002</v>
+      </c>
+      <c r="L431">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="432" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A432" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B432" s="1" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C432" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D432" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E432" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F432" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G432" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H432" s="1" t="s">
+        <v>1241</v>
+      </c>
+      <c r="I432">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="J432">
+        <v>0.55989999999999995</v>
+      </c>
+      <c r="K432">
+        <v>3.8845999999999998</v>
+      </c>
+      <c r="L432">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="433" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A433" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B433" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C433" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D433" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E433" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F433" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G433" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H433" s="1" t="s">
+        <v>1243</v>
+      </c>
+      <c r="I433">
+        <v>6.3399999999999998E-2</v>
+      </c>
+      <c r="J433">
+        <v>3.1076000000000001</v>
+      </c>
+      <c r="K433">
+        <v>3.9386999999999999</v>
+      </c>
+      <c r="L433">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Trimming data for p8 9 and 10
</commit_message>
<xml_diff>
--- a/Data/exp2-consolidated.xlsx
+++ b/Data/exp2-consolidated.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5519" uniqueCount="1464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6059" uniqueCount="1573">
   <si>
     <t>Ticks</t>
   </si>
@@ -4408,6 +4408,333 @@
   </si>
   <si>
     <t>635139106003199947</t>
+  </si>
+  <si>
+    <t>635139750508296817</t>
+  </si>
+  <si>
+    <t>635139750571810450</t>
+  </si>
+  <si>
+    <t>635139750676216421</t>
+  </si>
+  <si>
+    <t>635139750738870005</t>
+  </si>
+  <si>
+    <t>635139750807973957</t>
+  </si>
+  <si>
+    <t>635139750869657486</t>
+  </si>
+  <si>
+    <t>635139750947451935</t>
+  </si>
+  <si>
+    <t>635139751126452173</t>
+  </si>
+  <si>
+    <t>635139751382726831</t>
+  </si>
+  <si>
+    <t>635139751528285157</t>
+  </si>
+  <si>
+    <t>635139751593808905</t>
+  </si>
+  <si>
+    <t>635139751615330136</t>
+  </si>
+  <si>
+    <t>635139751677853712</t>
+  </si>
+  <si>
+    <t>635139751697844855</t>
+  </si>
+  <si>
+    <t>635139751750047841</t>
+  </si>
+  <si>
+    <t>635139751832602563</t>
+  </si>
+  <si>
+    <t>635139751900046420</t>
+  </si>
+  <si>
+    <t>635139751924977846</t>
+  </si>
+  <si>
+    <t>635139752042884590</t>
+  </si>
+  <si>
+    <t>635139752067045972</t>
+  </si>
+  <si>
+    <t>635139752134159811</t>
+  </si>
+  <si>
+    <t>635139752209684131</t>
+  </si>
+  <si>
+    <t>635139752274017810</t>
+  </si>
+  <si>
+    <t>635139752334401264</t>
+  </si>
+  <si>
+    <t>635139752350482184</t>
+  </si>
+  <si>
+    <t>635139752423006332</t>
+  </si>
+  <si>
+    <t>635139752478839525</t>
+  </si>
+  <si>
+    <t>635139752543883246</t>
+  </si>
+  <si>
+    <t>635139752607476883</t>
+  </si>
+  <si>
+    <t>635139752622107720</t>
+  </si>
+  <si>
+    <t>635139752685401340</t>
+  </si>
+  <si>
+    <t>635139752698322079</t>
+  </si>
+  <si>
+    <t>635139752768876115</t>
+  </si>
+  <si>
+    <t>635139752785717078</t>
+  </si>
+  <si>
+    <t>635139752841720281</t>
+  </si>
+  <si>
+    <t>635139752900443640</t>
+  </si>
+  <si>
+    <t>635139753645276242</t>
+  </si>
+  <si>
+    <t>635139753839717363</t>
+  </si>
+  <si>
+    <t>635139754044349067</t>
+  </si>
+  <si>
+    <t>635139754181946938</t>
+  </si>
+  <si>
+    <t>635139754371827798</t>
+  </si>
+  <si>
+    <t>635139754592910443</t>
+  </si>
+  <si>
+    <t>635139754714957424</t>
+  </si>
+  <si>
+    <t>635139754851865255</t>
+  </si>
+  <si>
+    <t>635139755032865607</t>
+  </si>
+  <si>
+    <t>635139755532424181</t>
+  </si>
+  <si>
+    <t>635139755640580367</t>
+  </si>
+  <si>
+    <t>635139755751696722</t>
+  </si>
+  <si>
+    <t>635139755815140351</t>
+  </si>
+  <si>
+    <t>635139755867263332</t>
+  </si>
+  <si>
+    <t>635139755974739480</t>
+  </si>
+  <si>
+    <t>635139756063134535</t>
+  </si>
+  <si>
+    <t>635139756137898812</t>
+  </si>
+  <si>
+    <t>635139756247175062</t>
+  </si>
+  <si>
+    <t>635139756655458414</t>
+  </si>
+  <si>
+    <t>635139756739253207</t>
+  </si>
+  <si>
+    <t>635139756937974573</t>
+  </si>
+  <si>
+    <t>635139757100653878</t>
+  </si>
+  <si>
+    <t>635139757242621998</t>
+  </si>
+  <si>
+    <t>635139757454524118</t>
+  </si>
+  <si>
+    <t>635139757588811799</t>
+  </si>
+  <si>
+    <t>635139757684647281</t>
+  </si>
+  <si>
+    <t>635139757860167320</t>
+  </si>
+  <si>
+    <t>635139758178395521</t>
+  </si>
+  <si>
+    <t>635139758287641770</t>
+  </si>
+  <si>
+    <t>635139758365556226</t>
+  </si>
+  <si>
+    <t>635139758441960596</t>
+  </si>
+  <si>
+    <t>635139758482802933</t>
+  </si>
+  <si>
+    <t>635139758564957632</t>
+  </si>
+  <si>
+    <t>635139758667673507</t>
+  </si>
+  <si>
+    <t>635139758742717799</t>
+  </si>
+  <si>
+    <t>635139758820752262</t>
+  </si>
+  <si>
+    <t>635139759377834125</t>
+  </si>
+  <si>
+    <t>635139759497310959</t>
+  </si>
+  <si>
+    <t>635139759564474801</t>
+  </si>
+  <si>
+    <t>635139759674271081</t>
+  </si>
+  <si>
+    <t>635139759835750317</t>
+  </si>
+  <si>
+    <t>635139760000549743</t>
+  </si>
+  <si>
+    <t>635139760093345050</t>
+  </si>
+  <si>
+    <t>635139760267264998</t>
+  </si>
+  <si>
+    <t>635139760391342095</t>
+  </si>
+  <si>
+    <t>635139760448505364</t>
+  </si>
+  <si>
+    <t>635139760484787440</t>
+  </si>
+  <si>
+    <t>635139760571982427</t>
+  </si>
+  <si>
+    <t>635139760680338624</t>
+  </si>
+  <si>
+    <t>635139760720260908</t>
+  </si>
+  <si>
+    <t>635139760815666365</t>
+  </si>
+  <si>
+    <t>635139760853948554</t>
+  </si>
+  <si>
+    <t>635139760961984734</t>
+  </si>
+  <si>
+    <t>635139760996556711</t>
+  </si>
+  <si>
+    <t>635139761185017490</t>
+  </si>
+  <si>
+    <t>635139761233660273</t>
+  </si>
+  <si>
+    <t>635139761264542039</t>
+  </si>
+  <si>
+    <t>635139761294333743</t>
+  </si>
+  <si>
+    <t>635139761372598219</t>
+  </si>
+  <si>
+    <t>635139761472253919</t>
+  </si>
+  <si>
+    <t>635139761501215576</t>
+  </si>
+  <si>
+    <t>635139761585620404</t>
+  </si>
+  <si>
+    <t>635139761609761784</t>
+  </si>
+  <si>
+    <t>635139761762050495</t>
+  </si>
+  <si>
+    <t>635139761873276857</t>
+  </si>
+  <si>
+    <t>635139761977612824</t>
+  </si>
+  <si>
+    <t>635139762033576025</t>
+  </si>
+  <si>
+    <t>635139762052777123</t>
+  </si>
+  <si>
+    <t>635139762119610946</t>
+  </si>
+  <si>
+    <t>635139762168533744</t>
+  </si>
+  <si>
+    <t>635139762189494943</t>
+  </si>
+  <si>
+    <t>635139762246968230</t>
+  </si>
+  <si>
+    <t>P8</t>
   </si>
 </sst>
 </file>
@@ -4755,10 +5082,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L757"/>
+  <dimension ref="A1:L865"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A721" workbookViewId="0">
-      <selection activeCell="D746" sqref="D746"/>
+    <sheetView tabSelected="1" topLeftCell="A835" workbookViewId="0">
+      <selection activeCell="B867" sqref="B867"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33533,6 +33860,4110 @@
         <v>0</v>
       </c>
       <c r="L757">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="758" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A758" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B758" s="1" t="s">
+        <v>1464</v>
+      </c>
+      <c r="C758" t="s">
+        <v>74</v>
+      </c>
+      <c r="D758" t="s">
+        <v>13</v>
+      </c>
+      <c r="E758" t="s">
+        <v>14</v>
+      </c>
+      <c r="F758">
+        <v>0</v>
+      </c>
+      <c r="G758">
+        <v>0</v>
+      </c>
+      <c r="H758">
+        <v>10602.606400000001</v>
+      </c>
+      <c r="I758">
+        <v>7.5244999999999997</v>
+      </c>
+      <c r="J758">
+        <v>34.991999999999997</v>
+      </c>
+      <c r="K758">
+        <v>0</v>
+      </c>
+      <c r="L758">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="759" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A759" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B759" s="1" t="s">
+        <v>1465</v>
+      </c>
+      <c r="C759" t="s">
+        <v>74</v>
+      </c>
+      <c r="D759" t="s">
+        <v>13</v>
+      </c>
+      <c r="E759" t="s">
+        <v>14</v>
+      </c>
+      <c r="F759">
+        <v>0</v>
+      </c>
+      <c r="G759">
+        <v>1</v>
+      </c>
+      <c r="H759">
+        <v>1559.0891999999999</v>
+      </c>
+      <c r="I759">
+        <v>5.0854999999999997</v>
+      </c>
+      <c r="J759">
+        <v>37.515000000000001</v>
+      </c>
+      <c r="K759">
+        <v>0</v>
+      </c>
+      <c r="L759">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="760" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A760" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B760" s="1" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C760" t="s">
+        <v>74</v>
+      </c>
+      <c r="D760" t="s">
+        <v>13</v>
+      </c>
+      <c r="E760" t="s">
+        <v>14</v>
+      </c>
+      <c r="F760">
+        <v>0</v>
+      </c>
+      <c r="G760">
+        <v>2</v>
+      </c>
+      <c r="H760">
+        <v>9195.5259000000005</v>
+      </c>
+      <c r="I760">
+        <v>0.11020000000000001</v>
+      </c>
+      <c r="J760">
+        <v>1.2189000000000001</v>
+      </c>
+      <c r="K760">
+        <v>0</v>
+      </c>
+      <c r="L760">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="761" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A761" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B761" s="1" t="s">
+        <v>1467</v>
+      </c>
+      <c r="C761" t="s">
+        <v>74</v>
+      </c>
+      <c r="D761" t="s">
+        <v>13</v>
+      </c>
+      <c r="E761" t="s">
+        <v>14</v>
+      </c>
+      <c r="F761">
+        <v>1</v>
+      </c>
+      <c r="G761">
+        <v>0</v>
+      </c>
+      <c r="H761">
+        <v>5333.3050999999996</v>
+      </c>
+      <c r="I761">
+        <v>7.1369999999999996</v>
+      </c>
+      <c r="J761">
+        <v>31.8855</v>
+      </c>
+      <c r="K761">
+        <v>0</v>
+      </c>
+      <c r="L761">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="762" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A762" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B762" s="1" t="s">
+        <v>1468</v>
+      </c>
+      <c r="C762" t="s">
+        <v>74</v>
+      </c>
+      <c r="D762" t="s">
+        <v>13</v>
+      </c>
+      <c r="E762" t="s">
+        <v>14</v>
+      </c>
+      <c r="F762">
+        <v>1</v>
+      </c>
+      <c r="G762">
+        <v>1</v>
+      </c>
+      <c r="H762">
+        <v>6007.3436000000002</v>
+      </c>
+      <c r="I762">
+        <v>7.1482999999999999</v>
+      </c>
+      <c r="J762">
+        <v>35.731400000000001</v>
+      </c>
+      <c r="K762">
+        <v>0</v>
+      </c>
+      <c r="L762">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="763" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A763" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B763" s="1" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C763" t="s">
+        <v>74</v>
+      </c>
+      <c r="D763" t="s">
+        <v>13</v>
+      </c>
+      <c r="E763" t="s">
+        <v>14</v>
+      </c>
+      <c r="F763">
+        <v>1</v>
+      </c>
+      <c r="G763">
+        <v>2</v>
+      </c>
+      <c r="H763">
+        <v>5435.3109000000004</v>
+      </c>
+      <c r="I763">
+        <v>7.4399999999999994E-2</v>
+      </c>
+      <c r="J763">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="K763">
+        <v>0</v>
+      </c>
+      <c r="L763">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="764" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A764" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B764" s="1" t="s">
+        <v>1470</v>
+      </c>
+      <c r="C764" t="s">
+        <v>74</v>
+      </c>
+      <c r="D764" t="s">
+        <v>13</v>
+      </c>
+      <c r="E764" t="s">
+        <v>14</v>
+      </c>
+      <c r="F764">
+        <v>2</v>
+      </c>
+      <c r="G764">
+        <v>0</v>
+      </c>
+      <c r="H764">
+        <v>6319.3613999999998</v>
+      </c>
+      <c r="I764">
+        <v>6.0575999999999999</v>
+      </c>
+      <c r="J764">
+        <v>33.730699999999999</v>
+      </c>
+      <c r="K764">
+        <v>0</v>
+      </c>
+      <c r="L764">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="765" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A765" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B765" s="1" t="s">
+        <v>1471</v>
+      </c>
+      <c r="C765" t="s">
+        <v>74</v>
+      </c>
+      <c r="D765" t="s">
+        <v>13</v>
+      </c>
+      <c r="E765" t="s">
+        <v>14</v>
+      </c>
+      <c r="F765">
+        <v>2</v>
+      </c>
+      <c r="G765">
+        <v>1</v>
+      </c>
+      <c r="H765">
+        <v>17115.978899999998</v>
+      </c>
+      <c r="I765">
+        <v>0.15640000000000001</v>
+      </c>
+      <c r="J765">
+        <v>2.2774999999999999</v>
+      </c>
+      <c r="K765">
+        <v>0</v>
+      </c>
+      <c r="L765">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="766" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A766" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B766" s="1" t="s">
+        <v>1472</v>
+      </c>
+      <c r="C766" t="s">
+        <v>74</v>
+      </c>
+      <c r="D766" t="s">
+        <v>13</v>
+      </c>
+      <c r="E766" t="s">
+        <v>14</v>
+      </c>
+      <c r="F766">
+        <v>2</v>
+      </c>
+      <c r="G766">
+        <v>2</v>
+      </c>
+      <c r="H766">
+        <v>24107.378799999999</v>
+      </c>
+      <c r="I766">
+        <v>0.1024</v>
+      </c>
+      <c r="J766">
+        <v>1.3070999999999999</v>
+      </c>
+      <c r="K766">
+        <v>0</v>
+      </c>
+      <c r="L766">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="767" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A767" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B767" s="1" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C767" t="s">
+        <v>74</v>
+      </c>
+      <c r="D767" t="s">
+        <v>13</v>
+      </c>
+      <c r="E767" t="s">
+        <v>35</v>
+      </c>
+      <c r="F767">
+        <v>0</v>
+      </c>
+      <c r="G767">
+        <v>0</v>
+      </c>
+      <c r="H767">
+        <v>13646.7806</v>
+      </c>
+      <c r="I767">
+        <v>10.5154</v>
+      </c>
+      <c r="J767">
+        <v>30.888500000000001</v>
+      </c>
+      <c r="K767">
+        <v>0</v>
+      </c>
+      <c r="L767">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="768" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A768" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B768" s="1" t="s">
+        <v>1474</v>
+      </c>
+      <c r="C768" t="s">
+        <v>74</v>
+      </c>
+      <c r="D768" t="s">
+        <v>13</v>
+      </c>
+      <c r="E768" t="s">
+        <v>35</v>
+      </c>
+      <c r="F768">
+        <v>0</v>
+      </c>
+      <c r="G768">
+        <v>1</v>
+      </c>
+      <c r="H768">
+        <v>5252.3005000000003</v>
+      </c>
+      <c r="I768">
+        <v>0.30270000000000002</v>
+      </c>
+      <c r="J768">
+        <v>0.91849999999999998</v>
+      </c>
+      <c r="K768">
+        <v>0</v>
+      </c>
+      <c r="L768">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="769" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A769" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B769" s="1" t="s">
+        <v>1475</v>
+      </c>
+      <c r="C769" t="s">
+        <v>74</v>
+      </c>
+      <c r="D769" t="s">
+        <v>13</v>
+      </c>
+      <c r="E769" t="s">
+        <v>35</v>
+      </c>
+      <c r="F769">
+        <v>0</v>
+      </c>
+      <c r="G769">
+        <v>2</v>
+      </c>
+      <c r="H769">
+        <v>1244.0712000000001</v>
+      </c>
+      <c r="I769">
+        <v>0.433</v>
+      </c>
+      <c r="J769">
+        <v>0.5917</v>
+      </c>
+      <c r="K769">
+        <v>0</v>
+      </c>
+      <c r="L769">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="770" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A770" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B770" s="1" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C770" t="s">
+        <v>74</v>
+      </c>
+      <c r="D770" t="s">
+        <v>13</v>
+      </c>
+      <c r="E770" t="s">
+        <v>35</v>
+      </c>
+      <c r="F770">
+        <v>1</v>
+      </c>
+      <c r="G770">
+        <v>0</v>
+      </c>
+      <c r="H770">
+        <v>5420.3100999999997</v>
+      </c>
+      <c r="I770">
+        <v>0.185</v>
+      </c>
+      <c r="J770">
+        <v>0.96230000000000004</v>
+      </c>
+      <c r="K770">
+        <v>0</v>
+      </c>
+      <c r="L770">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="771" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A771" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B771" s="1" t="s">
+        <v>1477</v>
+      </c>
+      <c r="C771" t="s">
+        <v>74</v>
+      </c>
+      <c r="D771" t="s">
+        <v>13</v>
+      </c>
+      <c r="E771" t="s">
+        <v>35</v>
+      </c>
+      <c r="F771">
+        <v>1</v>
+      </c>
+      <c r="G771">
+        <v>1</v>
+      </c>
+      <c r="H771">
+        <v>1282.0733</v>
+      </c>
+      <c r="I771">
+        <v>0.28910000000000002</v>
+      </c>
+      <c r="J771">
+        <v>0.6734</v>
+      </c>
+      <c r="K771">
+        <v>0</v>
+      </c>
+      <c r="L771">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="772" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A772" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B772" s="1" t="s">
+        <v>1478</v>
+      </c>
+      <c r="C772" t="s">
+        <v>74</v>
+      </c>
+      <c r="D772" t="s">
+        <v>13</v>
+      </c>
+      <c r="E772" t="s">
+        <v>35</v>
+      </c>
+      <c r="F772">
+        <v>1</v>
+      </c>
+      <c r="G772">
+        <v>2</v>
+      </c>
+      <c r="H772">
+        <v>3340.1911</v>
+      </c>
+      <c r="I772">
+        <v>0.13120000000000001</v>
+      </c>
+      <c r="J772">
+        <v>0.35870000000000002</v>
+      </c>
+      <c r="K772">
+        <v>0</v>
+      </c>
+      <c r="L772">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="773" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A773" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B773" s="1" t="s">
+        <v>1479</v>
+      </c>
+      <c r="C773" t="s">
+        <v>74</v>
+      </c>
+      <c r="D773" t="s">
+        <v>13</v>
+      </c>
+      <c r="E773" t="s">
+        <v>35</v>
+      </c>
+      <c r="F773">
+        <v>2</v>
+      </c>
+      <c r="G773">
+        <v>0</v>
+      </c>
+      <c r="H773">
+        <v>6015.3441000000003</v>
+      </c>
+      <c r="I773">
+        <v>0.34329999999999999</v>
+      </c>
+      <c r="J773">
+        <v>0.40229999999999999</v>
+      </c>
+      <c r="K773">
+        <v>0</v>
+      </c>
+      <c r="L773">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="774" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A774" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B774" s="1" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C774" t="s">
+        <v>74</v>
+      </c>
+      <c r="D774" t="s">
+        <v>13</v>
+      </c>
+      <c r="E774" t="s">
+        <v>35</v>
+      </c>
+      <c r="F774">
+        <v>2</v>
+      </c>
+      <c r="G774">
+        <v>1</v>
+      </c>
+      <c r="H774">
+        <v>5644.3227999999999</v>
+      </c>
+      <c r="I774">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="J774">
+        <v>3.5448</v>
+      </c>
+      <c r="K774">
+        <v>0</v>
+      </c>
+      <c r="L774">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="775" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A775" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B775" s="1" t="s">
+        <v>1481</v>
+      </c>
+      <c r="C775" t="s">
+        <v>74</v>
+      </c>
+      <c r="D775" t="s">
+        <v>13</v>
+      </c>
+      <c r="E775" t="s">
+        <v>35</v>
+      </c>
+      <c r="F775">
+        <v>2</v>
+      </c>
+      <c r="G775">
+        <v>2</v>
+      </c>
+      <c r="H775">
+        <v>1794.1025999999999</v>
+      </c>
+      <c r="I775">
+        <v>0.27679999999999999</v>
+      </c>
+      <c r="J775">
+        <v>2.5712000000000002</v>
+      </c>
+      <c r="K775">
+        <v>0</v>
+      </c>
+      <c r="L775">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="776" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A776" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B776" s="1" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C776" t="s">
+        <v>74</v>
+      </c>
+      <c r="D776" t="s">
+        <v>13</v>
+      </c>
+      <c r="E776" t="s">
+        <v>55</v>
+      </c>
+      <c r="F776">
+        <v>0</v>
+      </c>
+      <c r="G776">
+        <v>0</v>
+      </c>
+      <c r="H776">
+        <v>11117.635899999999</v>
+      </c>
+      <c r="I776">
+        <v>0.1138</v>
+      </c>
+      <c r="J776">
+        <v>0.31419999999999998</v>
+      </c>
+      <c r="K776">
+        <v>0</v>
+      </c>
+      <c r="L776">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="777" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A777" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B777" s="1" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C777" t="s">
+        <v>74</v>
+      </c>
+      <c r="D777" t="s">
+        <v>13</v>
+      </c>
+      <c r="E777" t="s">
+        <v>55</v>
+      </c>
+      <c r="F777">
+        <v>0</v>
+      </c>
+      <c r="G777">
+        <v>1</v>
+      </c>
+      <c r="H777">
+        <v>1248.0714</v>
+      </c>
+      <c r="I777">
+        <v>0.1167</v>
+      </c>
+      <c r="J777">
+        <v>1.8426</v>
+      </c>
+      <c r="K777">
+        <v>0</v>
+      </c>
+      <c r="L777">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="778" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A778" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B778" s="1" t="s">
+        <v>1484</v>
+      </c>
+      <c r="C778" t="s">
+        <v>74</v>
+      </c>
+      <c r="D778" t="s">
+        <v>13</v>
+      </c>
+      <c r="E778" t="s">
+        <v>55</v>
+      </c>
+      <c r="F778">
+        <v>0</v>
+      </c>
+      <c r="G778">
+        <v>2</v>
+      </c>
+      <c r="H778">
+        <v>5851.3347000000003</v>
+      </c>
+      <c r="I778">
+        <v>8.4699999999999998E-2</v>
+      </c>
+      <c r="J778">
+        <v>0.96150000000000002</v>
+      </c>
+      <c r="K778">
+        <v>0</v>
+      </c>
+      <c r="L778">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="779" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A779" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B779" s="1" t="s">
+        <v>1485</v>
+      </c>
+      <c r="C779" t="s">
+        <v>74</v>
+      </c>
+      <c r="D779" t="s">
+        <v>13</v>
+      </c>
+      <c r="E779" t="s">
+        <v>55</v>
+      </c>
+      <c r="F779">
+        <v>1</v>
+      </c>
+      <c r="G779">
+        <v>0</v>
+      </c>
+      <c r="H779">
+        <v>6675.3818000000001</v>
+      </c>
+      <c r="I779">
+        <v>9.5100000000000004E-2</v>
+      </c>
+      <c r="J779">
+        <v>1.4672000000000001</v>
+      </c>
+      <c r="K779">
+        <v>0</v>
+      </c>
+      <c r="L779">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="780" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A780" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B780" s="1" t="s">
+        <v>1486</v>
+      </c>
+      <c r="C780" t="s">
+        <v>74</v>
+      </c>
+      <c r="D780" t="s">
+        <v>13</v>
+      </c>
+      <c r="E780" t="s">
+        <v>55</v>
+      </c>
+      <c r="F780">
+        <v>1</v>
+      </c>
+      <c r="G780">
+        <v>1</v>
+      </c>
+      <c r="H780">
+        <v>5621.3215</v>
+      </c>
+      <c r="I780">
+        <v>0.1031</v>
+      </c>
+      <c r="J780">
+        <v>3.0766</v>
+      </c>
+      <c r="K780">
+        <v>0</v>
+      </c>
+      <c r="L780">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="781" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A781" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B781" s="1" t="s">
+        <v>1487</v>
+      </c>
+      <c r="C781" t="s">
+        <v>74</v>
+      </c>
+      <c r="D781" t="s">
+        <v>13</v>
+      </c>
+      <c r="E781" t="s">
+        <v>55</v>
+      </c>
+      <c r="F781">
+        <v>1</v>
+      </c>
+      <c r="G781">
+        <v>2</v>
+      </c>
+      <c r="H781">
+        <v>5371.3072000000002</v>
+      </c>
+      <c r="I781">
+        <v>0.16370000000000001</v>
+      </c>
+      <c r="J781">
+        <v>0.8901</v>
+      </c>
+      <c r="K781">
+        <v>0</v>
+      </c>
+      <c r="L781">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="782" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A782" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B782" s="1" t="s">
+        <v>1488</v>
+      </c>
+      <c r="C782" t="s">
+        <v>74</v>
+      </c>
+      <c r="D782" t="s">
+        <v>13</v>
+      </c>
+      <c r="E782" t="s">
+        <v>55</v>
+      </c>
+      <c r="F782">
+        <v>2</v>
+      </c>
+      <c r="G782">
+        <v>0</v>
+      </c>
+      <c r="H782">
+        <v>739.04229999999995</v>
+      </c>
+      <c r="I782">
+        <v>7.4300000000000005E-2</v>
+      </c>
+      <c r="J782">
+        <v>0</v>
+      </c>
+      <c r="K782">
+        <v>0</v>
+      </c>
+      <c r="L782">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="783" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A783" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B783" s="1" t="s">
+        <v>1489</v>
+      </c>
+      <c r="C783" t="s">
+        <v>74</v>
+      </c>
+      <c r="D783" t="s">
+        <v>13</v>
+      </c>
+      <c r="E783" t="s">
+        <v>55</v>
+      </c>
+      <c r="F783">
+        <v>2</v>
+      </c>
+      <c r="G783">
+        <v>1</v>
+      </c>
+      <c r="H783">
+        <v>6484.3708999999999</v>
+      </c>
+      <c r="I783">
+        <v>0.1071</v>
+      </c>
+      <c r="J783">
+        <v>3.7734999999999999</v>
+      </c>
+      <c r="K783">
+        <v>0</v>
+      </c>
+      <c r="L783">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="784" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A784" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B784" s="1" t="s">
+        <v>1490</v>
+      </c>
+      <c r="C784" t="s">
+        <v>74</v>
+      </c>
+      <c r="D784" t="s">
+        <v>13</v>
+      </c>
+      <c r="E784" t="s">
+        <v>55</v>
+      </c>
+      <c r="F784">
+        <v>2</v>
+      </c>
+      <c r="G784">
+        <v>2</v>
+      </c>
+      <c r="H784">
+        <v>4787.2737999999999</v>
+      </c>
+      <c r="I784">
+        <v>0.13039999999999999</v>
+      </c>
+      <c r="J784">
+        <v>2.1642999999999999</v>
+      </c>
+      <c r="K784">
+        <v>0</v>
+      </c>
+      <c r="L784">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="785" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A785" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B785" s="1" t="s">
+        <v>1491</v>
+      </c>
+      <c r="C785" t="s">
+        <v>74</v>
+      </c>
+      <c r="D785" t="s">
+        <v>54</v>
+      </c>
+      <c r="E785" t="s">
+        <v>55</v>
+      </c>
+      <c r="F785">
+        <v>0</v>
+      </c>
+      <c r="G785">
+        <v>0</v>
+      </c>
+      <c r="H785">
+        <v>5699.326</v>
+      </c>
+      <c r="I785">
+        <v>9.7799999999999998E-2</v>
+      </c>
+      <c r="J785">
+        <v>1.8709</v>
+      </c>
+      <c r="K785">
+        <v>3.9075000000000002</v>
+      </c>
+      <c r="L785">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="786" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A786" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B786" s="1" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C786" t="s">
+        <v>74</v>
+      </c>
+      <c r="D786" t="s">
+        <v>54</v>
+      </c>
+      <c r="E786" t="s">
+        <v>55</v>
+      </c>
+      <c r="F786">
+        <v>0</v>
+      </c>
+      <c r="G786">
+        <v>1</v>
+      </c>
+      <c r="H786">
+        <v>5583.3193000000001</v>
+      </c>
+      <c r="I786">
+        <v>0.1138</v>
+      </c>
+      <c r="J786">
+        <v>0.93410000000000004</v>
+      </c>
+      <c r="K786">
+        <v>3.4866999999999999</v>
+      </c>
+      <c r="L786">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="787" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A787" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B787" s="1" t="s">
+        <v>1493</v>
+      </c>
+      <c r="C787" t="s">
+        <v>74</v>
+      </c>
+      <c r="D787" t="s">
+        <v>54</v>
+      </c>
+      <c r="E787" t="s">
+        <v>55</v>
+      </c>
+      <c r="F787">
+        <v>0</v>
+      </c>
+      <c r="G787">
+        <v>2</v>
+      </c>
+      <c r="H787">
+        <v>694.03970000000004</v>
+      </c>
+      <c r="I787">
+        <v>0.1069</v>
+      </c>
+      <c r="J787">
+        <v>1.4795</v>
+      </c>
+      <c r="K787">
+        <v>3.9609000000000001</v>
+      </c>
+      <c r="L787">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="788" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A788" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B788" s="1" t="s">
+        <v>1494</v>
+      </c>
+      <c r="C788" t="s">
+        <v>74</v>
+      </c>
+      <c r="D788" t="s">
+        <v>54</v>
+      </c>
+      <c r="E788" t="s">
+        <v>55</v>
+      </c>
+      <c r="F788">
+        <v>1</v>
+      </c>
+      <c r="G788">
+        <v>0</v>
+      </c>
+      <c r="H788">
+        <v>5615.3212000000003</v>
+      </c>
+      <c r="I788">
+        <v>0.1217</v>
+      </c>
+      <c r="J788">
+        <v>0.54720000000000002</v>
+      </c>
+      <c r="K788">
+        <v>3.863</v>
+      </c>
+      <c r="L788">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="789" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A789" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B789" s="1" t="s">
+        <v>1495</v>
+      </c>
+      <c r="C789" t="s">
+        <v>74</v>
+      </c>
+      <c r="D789" t="s">
+        <v>54</v>
+      </c>
+      <c r="E789" t="s">
+        <v>55</v>
+      </c>
+      <c r="F789">
+        <v>1</v>
+      </c>
+      <c r="G789">
+        <v>1</v>
+      </c>
+      <c r="H789">
+        <v>556.03179999999998</v>
+      </c>
+      <c r="I789">
+        <v>8.5900000000000004E-2</v>
+      </c>
+      <c r="J789">
+        <v>1.9068000000000001</v>
+      </c>
+      <c r="K789">
+        <v>3.9613999999999998</v>
+      </c>
+      <c r="L789">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="790" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A790" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B790" s="1" t="s">
+        <v>1496</v>
+      </c>
+      <c r="C790" t="s">
+        <v>74</v>
+      </c>
+      <c r="D790" t="s">
+        <v>54</v>
+      </c>
+      <c r="E790" t="s">
+        <v>55</v>
+      </c>
+      <c r="F790">
+        <v>1</v>
+      </c>
+      <c r="G790">
+        <v>2</v>
+      </c>
+      <c r="H790">
+        <v>6379.3648999999996</v>
+      </c>
+      <c r="I790">
+        <v>0.1067</v>
+      </c>
+      <c r="J790">
+        <v>1.7677</v>
+      </c>
+      <c r="K790">
+        <v>3.9331999999999998</v>
+      </c>
+      <c r="L790">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="791" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A791" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B791" s="1" t="s">
+        <v>1497</v>
+      </c>
+      <c r="C791" t="s">
+        <v>74</v>
+      </c>
+      <c r="D791" t="s">
+        <v>54</v>
+      </c>
+      <c r="E791" t="s">
+        <v>55</v>
+      </c>
+      <c r="F791">
+        <v>2</v>
+      </c>
+      <c r="G791">
+        <v>0</v>
+      </c>
+      <c r="H791">
+        <v>887.05070000000001</v>
+      </c>
+      <c r="I791">
+        <v>0.1212</v>
+      </c>
+      <c r="J791">
+        <v>0.81079999999999997</v>
+      </c>
+      <c r="K791">
+        <v>4.0761000000000003</v>
+      </c>
+      <c r="L791">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="792" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A792" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B792" s="1" t="s">
+        <v>1498</v>
+      </c>
+      <c r="C792" t="s">
+        <v>74</v>
+      </c>
+      <c r="D792" t="s">
+        <v>54</v>
+      </c>
+      <c r="E792" t="s">
+        <v>55</v>
+      </c>
+      <c r="F792">
+        <v>2</v>
+      </c>
+      <c r="G792">
+        <v>1</v>
+      </c>
+      <c r="H792">
+        <v>4831.2763000000004</v>
+      </c>
+      <c r="I792">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="J792">
+        <v>0.1646</v>
+      </c>
+      <c r="K792">
+        <v>3.8311999999999999</v>
+      </c>
+      <c r="L792">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="793" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A793" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B793" s="1" t="s">
+        <v>1499</v>
+      </c>
+      <c r="C793" t="s">
+        <v>74</v>
+      </c>
+      <c r="D793" t="s">
+        <v>54</v>
+      </c>
+      <c r="E793" t="s">
+        <v>55</v>
+      </c>
+      <c r="F793">
+        <v>2</v>
+      </c>
+      <c r="G793">
+        <v>2</v>
+      </c>
+      <c r="H793">
+        <v>5076.2903999999999</v>
+      </c>
+      <c r="I793">
+        <v>8.5800000000000001E-2</v>
+      </c>
+      <c r="J793">
+        <v>0.41830000000000001</v>
+      </c>
+      <c r="K793">
+        <v>3.9483000000000001</v>
+      </c>
+      <c r="L793">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="794" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A794" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B794" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="C794" t="s">
+        <v>13</v>
+      </c>
+      <c r="D794" t="s">
+        <v>54</v>
+      </c>
+      <c r="E794" t="s">
+        <v>35</v>
+      </c>
+      <c r="F794">
+        <v>0</v>
+      </c>
+      <c r="G794">
+        <v>0</v>
+      </c>
+      <c r="H794">
+        <v>73692.214999999997</v>
+      </c>
+      <c r="I794">
+        <v>0.1832</v>
+      </c>
+      <c r="J794">
+        <v>2.383</v>
+      </c>
+      <c r="K794">
+        <v>1.5795999999999999</v>
+      </c>
+      <c r="L794">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="795" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A795" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B795" s="1" t="s">
+        <v>1501</v>
+      </c>
+      <c r="C795" t="s">
+        <v>13</v>
+      </c>
+      <c r="D795" t="s">
+        <v>54</v>
+      </c>
+      <c r="E795" t="s">
+        <v>35</v>
+      </c>
+      <c r="F795">
+        <v>0</v>
+      </c>
+      <c r="G795">
+        <v>1</v>
+      </c>
+      <c r="H795">
+        <v>17067.976200000001</v>
+      </c>
+      <c r="I795">
+        <v>0.25390000000000001</v>
+      </c>
+      <c r="J795">
+        <v>1.7085999999999999</v>
+      </c>
+      <c r="K795">
+        <v>1.6960999999999999</v>
+      </c>
+      <c r="L795">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="796" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A796" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B796" s="1" t="s">
+        <v>1502</v>
+      </c>
+      <c r="C796" t="s">
+        <v>13</v>
+      </c>
+      <c r="D796" t="s">
+        <v>54</v>
+      </c>
+      <c r="E796" t="s">
+        <v>35</v>
+      </c>
+      <c r="F796">
+        <v>0</v>
+      </c>
+      <c r="G796">
+        <v>2</v>
+      </c>
+      <c r="H796">
+        <v>18047.032200000001</v>
+      </c>
+      <c r="I796">
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="J796">
+        <v>2.1918000000000002</v>
+      </c>
+      <c r="K796">
+        <v>1.4381999999999999</v>
+      </c>
+      <c r="L796">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="797" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A797" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B797" s="1" t="s">
+        <v>1503</v>
+      </c>
+      <c r="C797" t="s">
+        <v>13</v>
+      </c>
+      <c r="D797" t="s">
+        <v>54</v>
+      </c>
+      <c r="E797" t="s">
+        <v>35</v>
+      </c>
+      <c r="F797">
+        <v>1</v>
+      </c>
+      <c r="G797">
+        <v>0</v>
+      </c>
+      <c r="H797">
+        <v>11859.678400000001</v>
+      </c>
+      <c r="I797">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="J797">
+        <v>2.8008000000000002</v>
+      </c>
+      <c r="K797">
+        <v>1.4148000000000001</v>
+      </c>
+      <c r="L797">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="798" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A798" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B798" s="1" t="s">
+        <v>1504</v>
+      </c>
+      <c r="C798" t="s">
+        <v>13</v>
+      </c>
+      <c r="D798" t="s">
+        <v>54</v>
+      </c>
+      <c r="E798" t="s">
+        <v>35</v>
+      </c>
+      <c r="F798">
+        <v>1</v>
+      </c>
+      <c r="G798">
+        <v>1</v>
+      </c>
+      <c r="H798">
+        <v>17804.0183</v>
+      </c>
+      <c r="I798">
+        <v>0.20930000000000001</v>
+      </c>
+      <c r="J798">
+        <v>0.64690000000000003</v>
+      </c>
+      <c r="K798">
+        <v>1.6062000000000001</v>
+      </c>
+      <c r="L798">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="799" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A799" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B799" s="1" t="s">
+        <v>1505</v>
+      </c>
+      <c r="C799" t="s">
+        <v>13</v>
+      </c>
+      <c r="D799" t="s">
+        <v>54</v>
+      </c>
+      <c r="E799" t="s">
+        <v>35</v>
+      </c>
+      <c r="F799">
+        <v>1</v>
+      </c>
+      <c r="G799">
+        <v>2</v>
+      </c>
+      <c r="H799">
+        <v>21187.211800000001</v>
+      </c>
+      <c r="I799">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="J799">
+        <v>2.9695</v>
+      </c>
+      <c r="K799">
+        <v>1.4342999999999999</v>
+      </c>
+      <c r="L799">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="800" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A800" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B800" s="1" t="s">
+        <v>1506</v>
+      </c>
+      <c r="C800" t="s">
+        <v>13</v>
+      </c>
+      <c r="D800" t="s">
+        <v>54</v>
+      </c>
+      <c r="E800" t="s">
+        <v>35</v>
+      </c>
+      <c r="F800">
+        <v>2</v>
+      </c>
+      <c r="G800">
+        <v>0</v>
+      </c>
+      <c r="H800">
+        <v>10272.5875</v>
+      </c>
+      <c r="I800">
+        <v>0.36009999999999998</v>
+      </c>
+      <c r="J800">
+        <v>0.40639999999999998</v>
+      </c>
+      <c r="K800">
+        <v>1.7219</v>
+      </c>
+      <c r="L800">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="801" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A801" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B801" s="1" t="s">
+        <v>1507</v>
+      </c>
+      <c r="C801" t="s">
+        <v>13</v>
+      </c>
+      <c r="D801" t="s">
+        <v>54</v>
+      </c>
+      <c r="E801" t="s">
+        <v>35</v>
+      </c>
+      <c r="F801">
+        <v>2</v>
+      </c>
+      <c r="G801">
+        <v>1</v>
+      </c>
+      <c r="H801">
+        <v>12506.715399999999</v>
+      </c>
+      <c r="I801">
+        <v>0.24030000000000001</v>
+      </c>
+      <c r="J801">
+        <v>0.88370000000000004</v>
+      </c>
+      <c r="K801">
+        <v>1.4084000000000001</v>
+      </c>
+      <c r="L801">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="802" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A802" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B802" s="1" t="s">
+        <v>1508</v>
+      </c>
+      <c r="C802" t="s">
+        <v>13</v>
+      </c>
+      <c r="D802" t="s">
+        <v>54</v>
+      </c>
+      <c r="E802" t="s">
+        <v>35</v>
+      </c>
+      <c r="F802">
+        <v>2</v>
+      </c>
+      <c r="G802">
+        <v>2</v>
+      </c>
+      <c r="H802">
+        <v>16795.960599999999</v>
+      </c>
+      <c r="I802">
+        <v>6.2300000000000001E-2</v>
+      </c>
+      <c r="J802">
+        <v>4.3380000000000001</v>
+      </c>
+      <c r="K802">
+        <v>1.5105999999999999</v>
+      </c>
+      <c r="L802">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="803" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A803" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B803" s="1" t="s">
+        <v>1509</v>
+      </c>
+      <c r="C803" t="s">
+        <v>74</v>
+      </c>
+      <c r="D803" t="s">
+        <v>54</v>
+      </c>
+      <c r="E803" t="s">
+        <v>14</v>
+      </c>
+      <c r="F803">
+        <v>0</v>
+      </c>
+      <c r="G803">
+        <v>0</v>
+      </c>
+      <c r="H803">
+        <v>37240.130100000002</v>
+      </c>
+      <c r="I803">
+        <v>0.16020000000000001</v>
+      </c>
+      <c r="J803">
+        <v>2.0642999999999998</v>
+      </c>
+      <c r="K803">
+        <v>1.2758</v>
+      </c>
+      <c r="L803">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="804" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A804" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B804" s="1" t="s">
+        <v>1510</v>
+      </c>
+      <c r="C804" t="s">
+        <v>74</v>
+      </c>
+      <c r="D804" t="s">
+        <v>54</v>
+      </c>
+      <c r="E804" t="s">
+        <v>14</v>
+      </c>
+      <c r="F804">
+        <v>0</v>
+      </c>
+      <c r="G804">
+        <v>1</v>
+      </c>
+      <c r="H804">
+        <v>9431.5395000000008</v>
+      </c>
+      <c r="I804">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="J804">
+        <v>0.42380000000000001</v>
+      </c>
+      <c r="K804">
+        <v>1.214</v>
+      </c>
+      <c r="L804">
+        <v>4.5400000000000003E-2</v>
+      </c>
+    </row>
+    <row r="805" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A805" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B805" s="1" t="s">
+        <v>1511</v>
+      </c>
+      <c r="C805" t="s">
+        <v>74</v>
+      </c>
+      <c r="D805" t="s">
+        <v>54</v>
+      </c>
+      <c r="E805" t="s">
+        <v>14</v>
+      </c>
+      <c r="F805">
+        <v>0</v>
+      </c>
+      <c r="G805">
+        <v>2</v>
+      </c>
+      <c r="H805">
+        <v>9603.5493000000006</v>
+      </c>
+      <c r="I805">
+        <v>0.12570000000000001</v>
+      </c>
+      <c r="J805">
+        <v>4.87E-2</v>
+      </c>
+      <c r="K805">
+        <v>1.2457</v>
+      </c>
+      <c r="L805">
+        <v>5.04E-2</v>
+      </c>
+    </row>
+    <row r="806" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A806" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B806" s="1" t="s">
+        <v>1512</v>
+      </c>
+      <c r="C806" t="s">
+        <v>74</v>
+      </c>
+      <c r="D806" t="s">
+        <v>54</v>
+      </c>
+      <c r="E806" t="s">
+        <v>14</v>
+      </c>
+      <c r="F806">
+        <v>1</v>
+      </c>
+      <c r="G806">
+        <v>0</v>
+      </c>
+      <c r="H806">
+        <v>5212.2981</v>
+      </c>
+      <c r="I806">
+        <v>9.1800000000000007E-2</v>
+      </c>
+      <c r="J806">
+        <v>0</v>
+      </c>
+      <c r="K806">
+        <v>1.2856000000000001</v>
+      </c>
+      <c r="L806">
+        <v>4.6600000000000003E-2</v>
+      </c>
+    </row>
+    <row r="807" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A807" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B807" s="1" t="s">
+        <v>1513</v>
+      </c>
+      <c r="C807" t="s">
+        <v>74</v>
+      </c>
+      <c r="D807" t="s">
+        <v>54</v>
+      </c>
+      <c r="E807" t="s">
+        <v>14</v>
+      </c>
+      <c r="F807">
+        <v>1</v>
+      </c>
+      <c r="G807">
+        <v>1</v>
+      </c>
+      <c r="H807">
+        <v>4260.2435999999998</v>
+      </c>
+      <c r="I807">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="J807">
+        <v>0.64480000000000004</v>
+      </c>
+      <c r="K807">
+        <v>1.2431000000000001</v>
+      </c>
+      <c r="L807">
+        <v>4.87E-2</v>
+      </c>
+    </row>
+    <row r="808" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A808" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B808" s="1" t="s">
+        <v>1514</v>
+      </c>
+      <c r="C808" t="s">
+        <v>74</v>
+      </c>
+      <c r="D808" t="s">
+        <v>54</v>
+      </c>
+      <c r="E808" t="s">
+        <v>14</v>
+      </c>
+      <c r="F808">
+        <v>1</v>
+      </c>
+      <c r="G808">
+        <v>2</v>
+      </c>
+      <c r="H808">
+        <v>9843.5630999999994</v>
+      </c>
+      <c r="I808">
+        <v>0.22739999999999999</v>
+      </c>
+      <c r="J808">
+        <v>0.41010000000000002</v>
+      </c>
+      <c r="K808">
+        <v>1.2859</v>
+      </c>
+      <c r="L808">
+        <v>5.1299999999999998E-2</v>
+      </c>
+    </row>
+    <row r="809" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A809" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B809" s="1" t="s">
+        <v>1515</v>
+      </c>
+      <c r="C809" t="s">
+        <v>74</v>
+      </c>
+      <c r="D809" t="s">
+        <v>54</v>
+      </c>
+      <c r="E809" t="s">
+        <v>14</v>
+      </c>
+      <c r="F809">
+        <v>2</v>
+      </c>
+      <c r="G809">
+        <v>0</v>
+      </c>
+      <c r="H809">
+        <v>7995.4573</v>
+      </c>
+      <c r="I809">
+        <v>0.1696</v>
+      </c>
+      <c r="J809">
+        <v>0.21870000000000001</v>
+      </c>
+      <c r="K809">
+        <v>1.3178000000000001</v>
+      </c>
+      <c r="L809">
+        <v>5.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="810" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A810" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B810" s="1" t="s">
+        <v>1516</v>
+      </c>
+      <c r="C810" t="s">
+        <v>74</v>
+      </c>
+      <c r="D810" t="s">
+        <v>54</v>
+      </c>
+      <c r="E810" t="s">
+        <v>14</v>
+      </c>
+      <c r="F810">
+        <v>2</v>
+      </c>
+      <c r="G810">
+        <v>1</v>
+      </c>
+      <c r="H810">
+        <v>5944.34</v>
+      </c>
+      <c r="I810">
+        <v>0.1628</v>
+      </c>
+      <c r="J810">
+        <v>0.1923</v>
+      </c>
+      <c r="K810">
+        <v>1.2635000000000001</v>
+      </c>
+      <c r="L810">
+        <v>4.8099999999999997E-2</v>
+      </c>
+    </row>
+    <row r="811" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A811" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B811" s="1" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C811" t="s">
+        <v>74</v>
+      </c>
+      <c r="D811" t="s">
+        <v>54</v>
+      </c>
+      <c r="E811" t="s">
+        <v>14</v>
+      </c>
+      <c r="F811">
+        <v>2</v>
+      </c>
+      <c r="G811">
+        <v>2</v>
+      </c>
+      <c r="H811">
+        <v>10131.5795</v>
+      </c>
+      <c r="I811">
+        <v>0.17549999999999999</v>
+      </c>
+      <c r="J811">
+        <v>0.19289999999999999</v>
+      </c>
+      <c r="K811">
+        <v>1.2848999999999999</v>
+      </c>
+      <c r="L811">
+        <v>4.9099999999999998E-2</v>
+      </c>
+    </row>
+    <row r="812" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A812" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B812" s="1" t="s">
+        <v>1518</v>
+      </c>
+      <c r="C812" t="s">
+        <v>13</v>
+      </c>
+      <c r="D812" t="s">
+        <v>54</v>
+      </c>
+      <c r="E812" t="s">
+        <v>14</v>
+      </c>
+      <c r="F812">
+        <v>0</v>
+      </c>
+      <c r="G812">
+        <v>0</v>
+      </c>
+      <c r="H812">
+        <v>38128.180800000002</v>
+      </c>
+      <c r="I812">
+        <v>0.15939999999999999</v>
+      </c>
+      <c r="J812">
+        <v>1.6523000000000001</v>
+      </c>
+      <c r="K812">
+        <v>1.5566</v>
+      </c>
+      <c r="L812">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="813" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A813" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B813" s="1" t="s">
+        <v>1519</v>
+      </c>
+      <c r="C813" t="s">
+        <v>13</v>
+      </c>
+      <c r="D813" t="s">
+        <v>54</v>
+      </c>
+      <c r="E813" t="s">
+        <v>14</v>
+      </c>
+      <c r="F813">
+        <v>0</v>
+      </c>
+      <c r="G813">
+        <v>1</v>
+      </c>
+      <c r="H813">
+        <v>7351.4205000000002</v>
+      </c>
+      <c r="I813">
+        <v>7.9399999999999998E-2</v>
+      </c>
+      <c r="J813">
+        <v>4.4200000000000003E-2</v>
+      </c>
+      <c r="K813">
+        <v>1.3087</v>
+      </c>
+      <c r="L813">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="814" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A814" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B814" s="1" t="s">
+        <v>1520</v>
+      </c>
+      <c r="C814" t="s">
+        <v>13</v>
+      </c>
+      <c r="D814" t="s">
+        <v>54</v>
+      </c>
+      <c r="E814" t="s">
+        <v>14</v>
+      </c>
+      <c r="F814">
+        <v>0</v>
+      </c>
+      <c r="G814">
+        <v>2</v>
+      </c>
+      <c r="H814">
+        <v>18820.076400000002</v>
+      </c>
+      <c r="I814">
+        <v>0.2072</v>
+      </c>
+      <c r="J814">
+        <v>2.5392000000000001</v>
+      </c>
+      <c r="K814">
+        <v>1.5397000000000001</v>
+      </c>
+      <c r="L814">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="815" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A815" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B815" s="1" t="s">
+        <v>1521</v>
+      </c>
+      <c r="C815" t="s">
+        <v>13</v>
+      </c>
+      <c r="D815" t="s">
+        <v>54</v>
+      </c>
+      <c r="E815" t="s">
+        <v>14</v>
+      </c>
+      <c r="F815">
+        <v>1</v>
+      </c>
+      <c r="G815">
+        <v>0</v>
+      </c>
+      <c r="H815">
+        <v>15230.8711</v>
+      </c>
+      <c r="I815">
+        <v>0.13980000000000001</v>
+      </c>
+      <c r="J815">
+        <v>4.1075999999999997</v>
+      </c>
+      <c r="K815">
+        <v>2.0196999999999998</v>
+      </c>
+      <c r="L815">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="816" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A816" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B816" s="1" t="s">
+        <v>1522</v>
+      </c>
+      <c r="C816" t="s">
+        <v>13</v>
+      </c>
+      <c r="D816" t="s">
+        <v>54</v>
+      </c>
+      <c r="E816" t="s">
+        <v>14</v>
+      </c>
+      <c r="F816">
+        <v>1</v>
+      </c>
+      <c r="G816">
+        <v>1</v>
+      </c>
+      <c r="H816">
+        <v>13264.7587</v>
+      </c>
+      <c r="I816">
+        <v>6.8699999999999997E-2</v>
+      </c>
+      <c r="J816">
+        <v>4.4463999999999997</v>
+      </c>
+      <c r="K816">
+        <v>1.5441</v>
+      </c>
+      <c r="L816">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="817" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A817" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B817" s="1" t="s">
+        <v>1523</v>
+      </c>
+      <c r="C817" t="s">
+        <v>13</v>
+      </c>
+      <c r="D817" t="s">
+        <v>54</v>
+      </c>
+      <c r="E817" t="s">
+        <v>14</v>
+      </c>
+      <c r="F817">
+        <v>1</v>
+      </c>
+      <c r="G817">
+        <v>2</v>
+      </c>
+      <c r="H817">
+        <v>20347.163799999998</v>
+      </c>
+      <c r="I817">
+        <v>0.16009999999999999</v>
+      </c>
+      <c r="J817">
+        <v>1.6549</v>
+      </c>
+      <c r="K817">
+        <v>1.6860999999999999</v>
+      </c>
+      <c r="L817">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="818" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A818" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B818" s="1" t="s">
+        <v>1524</v>
+      </c>
+      <c r="C818" t="s">
+        <v>13</v>
+      </c>
+      <c r="D818" t="s">
+        <v>54</v>
+      </c>
+      <c r="E818" t="s">
+        <v>14</v>
+      </c>
+      <c r="F818">
+        <v>2</v>
+      </c>
+      <c r="G818">
+        <v>0</v>
+      </c>
+      <c r="H818">
+        <v>12191.6973</v>
+      </c>
+      <c r="I818">
+        <v>8.3500000000000005E-2</v>
+      </c>
+      <c r="J818">
+        <v>4.5696000000000003</v>
+      </c>
+      <c r="K818">
+        <v>1.7293000000000001</v>
+      </c>
+      <c r="L818">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="819" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A819" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B819" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C819" t="s">
+        <v>13</v>
+      </c>
+      <c r="D819" t="s">
+        <v>54</v>
+      </c>
+      <c r="E819" t="s">
+        <v>14</v>
+      </c>
+      <c r="F819">
+        <v>2</v>
+      </c>
+      <c r="G819">
+        <v>1</v>
+      </c>
+      <c r="H819">
+        <v>8607.4923999999992</v>
+      </c>
+      <c r="I819">
+        <v>0.15620000000000001</v>
+      </c>
+      <c r="J819">
+        <v>0.81810000000000005</v>
+      </c>
+      <c r="K819">
+        <v>1.5983000000000001</v>
+      </c>
+      <c r="L819">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="820" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A820" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B820" s="1" t="s">
+        <v>1526</v>
+      </c>
+      <c r="C820" t="s">
+        <v>13</v>
+      </c>
+      <c r="D820" t="s">
+        <v>54</v>
+      </c>
+      <c r="E820" t="s">
+        <v>14</v>
+      </c>
+      <c r="F820">
+        <v>2</v>
+      </c>
+      <c r="G820">
+        <v>2</v>
+      </c>
+      <c r="H820">
+        <v>16055.9184</v>
+      </c>
+      <c r="I820">
+        <v>0</v>
+      </c>
+      <c r="J820">
+        <v>0.95020000000000004</v>
+      </c>
+      <c r="K820">
+        <v>1.8337000000000001</v>
+      </c>
+      <c r="L820">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="821" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A821" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B821" s="1" t="s">
+        <v>1527</v>
+      </c>
+      <c r="C821" t="s">
+        <v>74</v>
+      </c>
+      <c r="D821" t="s">
+        <v>54</v>
+      </c>
+      <c r="E821" t="s">
+        <v>35</v>
+      </c>
+      <c r="F821">
+        <v>0</v>
+      </c>
+      <c r="G821">
+        <v>0</v>
+      </c>
+      <c r="H821">
+        <v>7838.4483</v>
+      </c>
+      <c r="I821">
+        <v>6.13E-2</v>
+      </c>
+      <c r="J821">
+        <v>0.26779999999999998</v>
+      </c>
+      <c r="K821">
+        <v>1.3164</v>
+      </c>
+      <c r="L821">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="822" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A822" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B822" s="1" t="s">
+        <v>1528</v>
+      </c>
+      <c r="C822" t="s">
+        <v>74</v>
+      </c>
+      <c r="D822" t="s">
+        <v>54</v>
+      </c>
+      <c r="E822" t="s">
+        <v>35</v>
+      </c>
+      <c r="F822">
+        <v>0</v>
+      </c>
+      <c r="G822">
+        <v>1</v>
+      </c>
+      <c r="H822">
+        <v>10075.576300000001</v>
+      </c>
+      <c r="I822">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="J822">
+        <v>1.2231000000000001</v>
+      </c>
+      <c r="K822">
+        <v>1.4755</v>
+      </c>
+      <c r="L822">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="823" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A823" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B823" s="1" t="s">
+        <v>1529</v>
+      </c>
+      <c r="C823" t="s">
+        <v>74</v>
+      </c>
+      <c r="D823" t="s">
+        <v>54</v>
+      </c>
+      <c r="E823" t="s">
+        <v>35</v>
+      </c>
+      <c r="F823">
+        <v>0</v>
+      </c>
+      <c r="G823">
+        <v>2</v>
+      </c>
+      <c r="H823">
+        <v>6883.3936999999996</v>
+      </c>
+      <c r="I823">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="J823">
+        <v>3.7528000000000001</v>
+      </c>
+      <c r="K823">
+        <v>1.4965999999999999</v>
+      </c>
+      <c r="L823">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="824" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A824" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B824" s="1" t="s">
+        <v>1530</v>
+      </c>
+      <c r="C824" t="s">
+        <v>74</v>
+      </c>
+      <c r="D824" t="s">
+        <v>54</v>
+      </c>
+      <c r="E824" t="s">
+        <v>35</v>
+      </c>
+      <c r="F824">
+        <v>1</v>
+      </c>
+      <c r="G824">
+        <v>0</v>
+      </c>
+      <c r="H824">
+        <v>6875.3932000000004</v>
+      </c>
+      <c r="I824">
+        <v>6.83E-2</v>
+      </c>
+      <c r="J824">
+        <v>0.23230000000000001</v>
+      </c>
+      <c r="K824">
+        <v>1.5505</v>
+      </c>
+      <c r="L824">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="825" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A825" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B825" s="1" t="s">
+        <v>1531</v>
+      </c>
+      <c r="C825" t="s">
+        <v>74</v>
+      </c>
+      <c r="D825" t="s">
+        <v>54</v>
+      </c>
+      <c r="E825" t="s">
+        <v>35</v>
+      </c>
+      <c r="F825">
+        <v>1</v>
+      </c>
+      <c r="G825">
+        <v>1</v>
+      </c>
+      <c r="H825">
+        <v>3244.1855999999998</v>
+      </c>
+      <c r="I825">
+        <v>0.1159</v>
+      </c>
+      <c r="J825">
+        <v>0.12590000000000001</v>
+      </c>
+      <c r="K825">
+        <v>1.4986999999999999</v>
+      </c>
+      <c r="L825">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="826" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A826" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B826" s="1" t="s">
+        <v>1532</v>
+      </c>
+      <c r="C826" t="s">
+        <v>74</v>
+      </c>
+      <c r="D826" t="s">
+        <v>54</v>
+      </c>
+      <c r="E826" t="s">
+        <v>35</v>
+      </c>
+      <c r="F826">
+        <v>1</v>
+      </c>
+      <c r="G826">
+        <v>2</v>
+      </c>
+      <c r="H826">
+        <v>7387.4225999999999</v>
+      </c>
+      <c r="I826">
+        <v>6.6699999999999995E-2</v>
+      </c>
+      <c r="J826">
+        <v>0.27029999999999998</v>
+      </c>
+      <c r="K826">
+        <v>1.5061</v>
+      </c>
+      <c r="L826">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="827" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A827" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B827" s="1" t="s">
+        <v>1533</v>
+      </c>
+      <c r="C827" t="s">
+        <v>74</v>
+      </c>
+      <c r="D827" t="s">
+        <v>54</v>
+      </c>
+      <c r="E827" t="s">
+        <v>35</v>
+      </c>
+      <c r="F827">
+        <v>2</v>
+      </c>
+      <c r="G827">
+        <v>0</v>
+      </c>
+      <c r="H827">
+        <v>9411.5383999999995</v>
+      </c>
+      <c r="I827">
+        <v>8.09E-2</v>
+      </c>
+      <c r="J827">
+        <v>0.18390000000000001</v>
+      </c>
+      <c r="K827">
+        <v>1.7345999999999999</v>
+      </c>
+      <c r="L827">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="828" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A828" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B828" s="1" t="s">
+        <v>1534</v>
+      </c>
+      <c r="C828" t="s">
+        <v>74</v>
+      </c>
+      <c r="D828" t="s">
+        <v>54</v>
+      </c>
+      <c r="E828" t="s">
+        <v>35</v>
+      </c>
+      <c r="F828">
+        <v>2</v>
+      </c>
+      <c r="G828">
+        <v>1</v>
+      </c>
+      <c r="H828">
+        <v>6536.3738999999996</v>
+      </c>
+      <c r="I828">
+        <v>5.7799999999999997E-2</v>
+      </c>
+      <c r="J828">
+        <v>0.52270000000000005</v>
+      </c>
+      <c r="K828">
+        <v>1.5898000000000001</v>
+      </c>
+      <c r="L828">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="829" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A829" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B829" s="1" t="s">
+        <v>1535</v>
+      </c>
+      <c r="C829" t="s">
+        <v>74</v>
+      </c>
+      <c r="D829" t="s">
+        <v>54</v>
+      </c>
+      <c r="E829" t="s">
+        <v>35</v>
+      </c>
+      <c r="F829">
+        <v>2</v>
+      </c>
+      <c r="G829">
+        <v>2</v>
+      </c>
+      <c r="H829">
+        <v>6823.3903</v>
+      </c>
+      <c r="I829">
+        <v>0.1016</v>
+      </c>
+      <c r="J829">
+        <v>0.13569999999999999</v>
+      </c>
+      <c r="K829">
+        <v>1.5033000000000001</v>
+      </c>
+      <c r="L829">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="830" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A830" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B830" s="1" t="s">
+        <v>1536</v>
+      </c>
+      <c r="C830" t="s">
+        <v>13</v>
+      </c>
+      <c r="D830" t="s">
+        <v>54</v>
+      </c>
+      <c r="E830" t="s">
+        <v>55</v>
+      </c>
+      <c r="F830">
+        <v>0</v>
+      </c>
+      <c r="G830">
+        <v>0</v>
+      </c>
+      <c r="H830">
+        <v>54299.1057</v>
+      </c>
+      <c r="I830">
+        <v>0.433</v>
+      </c>
+      <c r="J830">
+        <v>2.9315000000000002</v>
+      </c>
+      <c r="K830">
+        <v>3.1274000000000002</v>
+      </c>
+      <c r="L830">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="831" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A831" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B831" s="1" t="s">
+        <v>1537</v>
+      </c>
+      <c r="C831" t="s">
+        <v>13</v>
+      </c>
+      <c r="D831" t="s">
+        <v>54</v>
+      </c>
+      <c r="E831" t="s">
+        <v>55</v>
+      </c>
+      <c r="F831">
+        <v>0</v>
+      </c>
+      <c r="G831">
+        <v>1</v>
+      </c>
+      <c r="H831">
+        <v>9639.5512999999992</v>
+      </c>
+      <c r="I831">
+        <v>6.4199999999999993E-2</v>
+      </c>
+      <c r="J831">
+        <v>1.4277</v>
+      </c>
+      <c r="K831">
+        <v>2.2856999999999998</v>
+      </c>
+      <c r="L831">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="832" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A832" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B832" s="1" t="s">
+        <v>1538</v>
+      </c>
+      <c r="C832" t="s">
+        <v>13</v>
+      </c>
+      <c r="D832" t="s">
+        <v>54</v>
+      </c>
+      <c r="E832" t="s">
+        <v>55</v>
+      </c>
+      <c r="F832">
+        <v>0</v>
+      </c>
+      <c r="G832">
+        <v>2</v>
+      </c>
+      <c r="H832">
+        <v>5640.3226000000004</v>
+      </c>
+      <c r="I832">
+        <v>0.1144</v>
+      </c>
+      <c r="J832">
+        <v>1.3</v>
+      </c>
+      <c r="K832">
+        <v>2.2538</v>
+      </c>
+      <c r="L832">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="833" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A833" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B833" s="1" t="s">
+        <v>1539</v>
+      </c>
+      <c r="C833" t="s">
+        <v>13</v>
+      </c>
+      <c r="D833" t="s">
+        <v>54</v>
+      </c>
+      <c r="E833" t="s">
+        <v>55</v>
+      </c>
+      <c r="F833">
+        <v>1</v>
+      </c>
+      <c r="G833">
+        <v>0</v>
+      </c>
+      <c r="H833">
+        <v>9915.5671999999995</v>
+      </c>
+      <c r="I833">
+        <v>0</v>
+      </c>
+      <c r="J833">
+        <v>4.6727999999999996</v>
+      </c>
+      <c r="K833">
+        <v>1.8251999999999999</v>
+      </c>
+      <c r="L833">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="834" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A834" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B834" s="1" t="s">
+        <v>1540</v>
+      </c>
+      <c r="C834" t="s">
+        <v>13</v>
+      </c>
+      <c r="D834" t="s">
+        <v>54</v>
+      </c>
+      <c r="E834" t="s">
+        <v>55</v>
+      </c>
+      <c r="F834">
+        <v>1</v>
+      </c>
+      <c r="G834">
+        <v>1</v>
+      </c>
+      <c r="H834">
+        <v>15043.860500000001</v>
+      </c>
+      <c r="I834">
+        <v>0.30730000000000002</v>
+      </c>
+      <c r="J834">
+        <v>1.6135999999999999</v>
+      </c>
+      <c r="K834">
+        <v>2.4047999999999998</v>
+      </c>
+      <c r="L834">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="835" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A835" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B835" s="1" t="s">
+        <v>1541</v>
+      </c>
+      <c r="C835" t="s">
+        <v>13</v>
+      </c>
+      <c r="D835" t="s">
+        <v>54</v>
+      </c>
+      <c r="E835" t="s">
+        <v>55</v>
+      </c>
+      <c r="F835">
+        <v>1</v>
+      </c>
+      <c r="G835">
+        <v>2</v>
+      </c>
+      <c r="H835">
+        <v>15459.8843</v>
+      </c>
+      <c r="I835">
+        <v>0.26950000000000002</v>
+      </c>
+      <c r="J835">
+        <v>9.2103000000000002</v>
+      </c>
+      <c r="K835">
+        <v>2.5213000000000001</v>
+      </c>
+      <c r="L835">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="836" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A836" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B836" s="1" t="s">
+        <v>1542</v>
+      </c>
+      <c r="C836" t="s">
+        <v>13</v>
+      </c>
+      <c r="D836" t="s">
+        <v>54</v>
+      </c>
+      <c r="E836" t="s">
+        <v>55</v>
+      </c>
+      <c r="F836">
+        <v>2</v>
+      </c>
+      <c r="G836">
+        <v>0</v>
+      </c>
+      <c r="H836">
+        <v>8439.4827000000005</v>
+      </c>
+      <c r="I836">
+        <v>6.7100000000000007E-2</v>
+      </c>
+      <c r="J836">
+        <v>1.2107000000000001</v>
+      </c>
+      <c r="K836">
+        <v>1.772</v>
+      </c>
+      <c r="L836">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="837" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A837" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B837" s="1" t="s">
+        <v>1543</v>
+      </c>
+      <c r="C837" t="s">
+        <v>13</v>
+      </c>
+      <c r="D837" t="s">
+        <v>54</v>
+      </c>
+      <c r="E837" t="s">
+        <v>55</v>
+      </c>
+      <c r="F837">
+        <v>2</v>
+      </c>
+      <c r="G837">
+        <v>1</v>
+      </c>
+      <c r="H837">
+        <v>16654.952600000001</v>
+      </c>
+      <c r="I837">
+        <v>6.4600000000000005E-2</v>
+      </c>
+      <c r="J837">
+        <v>2.9775</v>
+      </c>
+      <c r="K837">
+        <v>1.5184</v>
+      </c>
+      <c r="L837">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="838" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A838" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B838" s="1" t="s">
+        <v>1544</v>
+      </c>
+      <c r="C838" t="s">
+        <v>13</v>
+      </c>
+      <c r="D838" t="s">
+        <v>54</v>
+      </c>
+      <c r="E838" t="s">
+        <v>55</v>
+      </c>
+      <c r="F838">
+        <v>2</v>
+      </c>
+      <c r="G838">
+        <v>2</v>
+      </c>
+      <c r="H838">
+        <v>11470.6561</v>
+      </c>
+      <c r="I838">
+        <v>9.9599999999999994E-2</v>
+      </c>
+      <c r="J838">
+        <v>1.6609</v>
+      </c>
+      <c r="K838">
+        <v>2.0874000000000001</v>
+      </c>
+      <c r="L838">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="839" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A839" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B839" s="1" t="s">
+        <v>1545</v>
+      </c>
+      <c r="C839" t="s">
+        <v>13</v>
+      </c>
+      <c r="D839" t="s">
+        <v>13</v>
+      </c>
+      <c r="E839" t="s">
+        <v>55</v>
+      </c>
+      <c r="F839">
+        <v>0</v>
+      </c>
+      <c r="G839">
+        <v>0</v>
+      </c>
+      <c r="H839">
+        <v>4953.2833000000001</v>
+      </c>
+      <c r="I839">
+        <v>5.11E-2</v>
+      </c>
+      <c r="J839">
+        <v>0.70730000000000004</v>
+      </c>
+      <c r="K839">
+        <v>0</v>
+      </c>
+      <c r="L839">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="840" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A840" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B840" s="1" t="s">
+        <v>1546</v>
+      </c>
+      <c r="C840" t="s">
+        <v>13</v>
+      </c>
+      <c r="D840" t="s">
+        <v>13</v>
+      </c>
+      <c r="E840" t="s">
+        <v>55</v>
+      </c>
+      <c r="F840">
+        <v>0</v>
+      </c>
+      <c r="G840">
+        <v>1</v>
+      </c>
+      <c r="H840">
+        <v>1764.1010000000001</v>
+      </c>
+      <c r="I840">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="J840">
+        <v>0.7117</v>
+      </c>
+      <c r="K840">
+        <v>0</v>
+      </c>
+      <c r="L840">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="841" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A841" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B841" s="1" t="s">
+        <v>1547</v>
+      </c>
+      <c r="C841" t="s">
+        <v>13</v>
+      </c>
+      <c r="D841" t="s">
+        <v>13</v>
+      </c>
+      <c r="E841" t="s">
+        <v>55</v>
+      </c>
+      <c r="F841">
+        <v>0</v>
+      </c>
+      <c r="G841">
+        <v>2</v>
+      </c>
+      <c r="H841">
+        <v>7391.4228000000003</v>
+      </c>
+      <c r="I841">
+        <v>6.6799999999999998E-2</v>
+      </c>
+      <c r="J841">
+        <v>1.9614</v>
+      </c>
+      <c r="K841">
+        <v>0</v>
+      </c>
+      <c r="L841">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="842" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A842" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B842" s="1" t="s">
+        <v>1548</v>
+      </c>
+      <c r="C842" t="s">
+        <v>13</v>
+      </c>
+      <c r="D842" t="s">
+        <v>13</v>
+      </c>
+      <c r="E842" t="s">
+        <v>55</v>
+      </c>
+      <c r="F842">
+        <v>1</v>
+      </c>
+      <c r="G842">
+        <v>0</v>
+      </c>
+      <c r="H842">
+        <v>10075.576300000001</v>
+      </c>
+      <c r="I842">
+        <v>0.2152</v>
+      </c>
+      <c r="J842">
+        <v>0.3745</v>
+      </c>
+      <c r="K842">
+        <v>0</v>
+      </c>
+      <c r="L842">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="843" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A843" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B843" s="1" t="s">
+        <v>1549</v>
+      </c>
+      <c r="C843" t="s">
+        <v>13</v>
+      </c>
+      <c r="D843" t="s">
+        <v>13</v>
+      </c>
+      <c r="E843" t="s">
+        <v>55</v>
+      </c>
+      <c r="F843">
+        <v>1</v>
+      </c>
+      <c r="G843">
+        <v>1</v>
+      </c>
+      <c r="H843">
+        <v>3039.1738</v>
+      </c>
+      <c r="I843">
+        <v>4.36E-2</v>
+      </c>
+      <c r="J843">
+        <v>0.75380000000000003</v>
+      </c>
+      <c r="K843">
+        <v>0</v>
+      </c>
+      <c r="L843">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="844" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A844" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B844" s="1" t="s">
+        <v>1550</v>
+      </c>
+      <c r="C844" t="s">
+        <v>13</v>
+      </c>
+      <c r="D844" t="s">
+        <v>13</v>
+      </c>
+      <c r="E844" t="s">
+        <v>55</v>
+      </c>
+      <c r="F844">
+        <v>1</v>
+      </c>
+      <c r="G844">
+        <v>2</v>
+      </c>
+      <c r="H844">
+        <v>8792.5028999999995</v>
+      </c>
+      <c r="I844">
+        <v>5.7200000000000001E-2</v>
+      </c>
+      <c r="J844">
+        <v>5.8773999999999997</v>
+      </c>
+      <c r="K844">
+        <v>0</v>
+      </c>
+      <c r="L844">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="845" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A845" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B845" s="1" t="s">
+        <v>1551</v>
+      </c>
+      <c r="C845" t="s">
+        <v>13</v>
+      </c>
+      <c r="D845" t="s">
+        <v>13</v>
+      </c>
+      <c r="E845" t="s">
+        <v>55</v>
+      </c>
+      <c r="F845">
+        <v>2</v>
+      </c>
+      <c r="G845">
+        <v>0</v>
+      </c>
+      <c r="H845">
+        <v>2968.1696999999999</v>
+      </c>
+      <c r="I845">
+        <v>0.1018</v>
+      </c>
+      <c r="J845">
+        <v>5.2374999999999998</v>
+      </c>
+      <c r="K845">
+        <v>0</v>
+      </c>
+      <c r="L845">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="846" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A846" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B846" s="1" t="s">
+        <v>1552</v>
+      </c>
+      <c r="C846" t="s">
+        <v>13</v>
+      </c>
+      <c r="D846" t="s">
+        <v>13</v>
+      </c>
+      <c r="E846" t="s">
+        <v>55</v>
+      </c>
+      <c r="F846">
+        <v>2</v>
+      </c>
+      <c r="G846">
+        <v>1</v>
+      </c>
+      <c r="H846">
+        <v>10023.573399999999</v>
+      </c>
+      <c r="I846">
+        <v>0.17760000000000001</v>
+      </c>
+      <c r="J846">
+        <v>7.8532999999999999</v>
+      </c>
+      <c r="K846">
+        <v>0</v>
+      </c>
+      <c r="L846">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="847" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A847" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B847" s="1" t="s">
+        <v>1553</v>
+      </c>
+      <c r="C847" t="s">
+        <v>13</v>
+      </c>
+      <c r="D847" t="s">
+        <v>13</v>
+      </c>
+      <c r="E847" t="s">
+        <v>55</v>
+      </c>
+      <c r="F847">
+        <v>2</v>
+      </c>
+      <c r="G847">
+        <v>2</v>
+      </c>
+      <c r="H847">
+        <v>2485.1421</v>
+      </c>
+      <c r="I847">
+        <v>8.9700000000000002E-2</v>
+      </c>
+      <c r="J847">
+        <v>6.2290000000000001</v>
+      </c>
+      <c r="K847">
+        <v>0</v>
+      </c>
+      <c r="L847">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="848" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A848" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B848" s="1" t="s">
+        <v>1554</v>
+      </c>
+      <c r="C848" t="s">
+        <v>13</v>
+      </c>
+      <c r="D848" t="s">
+        <v>13</v>
+      </c>
+      <c r="E848" t="s">
+        <v>35</v>
+      </c>
+      <c r="F848">
+        <v>0</v>
+      </c>
+      <c r="G848">
+        <v>0</v>
+      </c>
+      <c r="H848">
+        <v>18067.033299999999</v>
+      </c>
+      <c r="I848">
+        <v>0.28770000000000001</v>
+      </c>
+      <c r="J848">
+        <v>1.5967</v>
+      </c>
+      <c r="K848">
+        <v>0</v>
+      </c>
+      <c r="L848">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="849" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A849" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B849" s="1" t="s">
+        <v>1555</v>
+      </c>
+      <c r="C849" t="s">
+        <v>13</v>
+      </c>
+      <c r="D849" t="s">
+        <v>13</v>
+      </c>
+      <c r="E849" t="s">
+        <v>35</v>
+      </c>
+      <c r="F849">
+        <v>0</v>
+      </c>
+      <c r="G849">
+        <v>1</v>
+      </c>
+      <c r="H849">
+        <v>3944.2256000000002</v>
+      </c>
+      <c r="I849">
+        <v>9.01E-2</v>
+      </c>
+      <c r="J849">
+        <v>1.7837000000000001</v>
+      </c>
+      <c r="K849">
+        <v>0</v>
+      </c>
+      <c r="L849">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="850" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A850" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B850" s="1" t="s">
+        <v>1556</v>
+      </c>
+      <c r="C850" t="s">
+        <v>13</v>
+      </c>
+      <c r="D850" t="s">
+        <v>13</v>
+      </c>
+      <c r="E850" t="s">
+        <v>35</v>
+      </c>
+      <c r="F850">
+        <v>0</v>
+      </c>
+      <c r="G850">
+        <v>2</v>
+      </c>
+      <c r="H850">
+        <v>2412.1379999999999</v>
+      </c>
+      <c r="I850">
+        <v>0.54349999999999998</v>
+      </c>
+      <c r="J850">
+        <v>2.4895999999999998</v>
+      </c>
+      <c r="K850">
+        <v>0</v>
+      </c>
+      <c r="L850">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="851" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A851" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B851" s="1" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C851" t="s">
+        <v>13</v>
+      </c>
+      <c r="D851" t="s">
+        <v>13</v>
+      </c>
+      <c r="E851" t="s">
+        <v>35</v>
+      </c>
+      <c r="F851">
+        <v>1</v>
+      </c>
+      <c r="G851">
+        <v>0</v>
+      </c>
+      <c r="H851">
+        <v>2305.1318999999999</v>
+      </c>
+      <c r="I851">
+        <v>0.13650000000000001</v>
+      </c>
+      <c r="J851">
+        <v>0.3049</v>
+      </c>
+      <c r="K851">
+        <v>0</v>
+      </c>
+      <c r="L851">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="852" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A852" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B852" s="1" t="s">
+        <v>1558</v>
+      </c>
+      <c r="C852" t="s">
+        <v>13</v>
+      </c>
+      <c r="D852" t="s">
+        <v>13</v>
+      </c>
+      <c r="E852" t="s">
+        <v>35</v>
+      </c>
+      <c r="F852">
+        <v>1</v>
+      </c>
+      <c r="G852">
+        <v>1</v>
+      </c>
+      <c r="H852">
+        <v>7149.4089000000004</v>
+      </c>
+      <c r="I852">
+        <v>2.9899999999999999E-2</v>
+      </c>
+      <c r="J852">
+        <v>0</v>
+      </c>
+      <c r="K852">
+        <v>0</v>
+      </c>
+      <c r="L852">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="853" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A853" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B853" s="1" t="s">
+        <v>1559</v>
+      </c>
+      <c r="C853" t="s">
+        <v>13</v>
+      </c>
+      <c r="D853" t="s">
+        <v>13</v>
+      </c>
+      <c r="E853" t="s">
+        <v>35</v>
+      </c>
+      <c r="F853">
+        <v>1</v>
+      </c>
+      <c r="G853">
+        <v>2</v>
+      </c>
+      <c r="H853">
+        <v>9359.5352999999996</v>
+      </c>
+      <c r="I853">
+        <v>0.1628</v>
+      </c>
+      <c r="J853">
+        <v>5.0114999999999998</v>
+      </c>
+      <c r="K853">
+        <v>0</v>
+      </c>
+      <c r="L853">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="854" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A854" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B854" s="1" t="s">
+        <v>1560</v>
+      </c>
+      <c r="C854" t="s">
+        <v>13</v>
+      </c>
+      <c r="D854" t="s">
+        <v>13</v>
+      </c>
+      <c r="E854" t="s">
+        <v>35</v>
+      </c>
+      <c r="F854">
+        <v>2</v>
+      </c>
+      <c r="G854">
+        <v>0</v>
+      </c>
+      <c r="H854">
+        <v>2119.1212</v>
+      </c>
+      <c r="I854">
+        <v>0.33069999999999999</v>
+      </c>
+      <c r="J854">
+        <v>4.1181999999999999</v>
+      </c>
+      <c r="K854">
+        <v>0</v>
+      </c>
+      <c r="L854">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="855" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A855" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B855" s="1" t="s">
+        <v>1561</v>
+      </c>
+      <c r="C855" t="s">
+        <v>13</v>
+      </c>
+      <c r="D855" t="s">
+        <v>13</v>
+      </c>
+      <c r="E855" t="s">
+        <v>35</v>
+      </c>
+      <c r="F855">
+        <v>2</v>
+      </c>
+      <c r="G855">
+        <v>1</v>
+      </c>
+      <c r="H855">
+        <v>7775.4448000000002</v>
+      </c>
+      <c r="I855">
+        <v>0.18140000000000001</v>
+      </c>
+      <c r="J855">
+        <v>3.4197000000000002</v>
+      </c>
+      <c r="K855">
+        <v>0</v>
+      </c>
+      <c r="L855">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="856" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A856" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B856" s="1" t="s">
+        <v>1562</v>
+      </c>
+      <c r="C856" t="s">
+        <v>13</v>
+      </c>
+      <c r="D856" t="s">
+        <v>13</v>
+      </c>
+      <c r="E856" t="s">
+        <v>35</v>
+      </c>
+      <c r="F856">
+        <v>2</v>
+      </c>
+      <c r="G856">
+        <v>2</v>
+      </c>
+      <c r="H856">
+        <v>1640.0938000000001</v>
+      </c>
+      <c r="I856">
+        <v>0.2044</v>
+      </c>
+      <c r="J856">
+        <v>2.6063000000000001</v>
+      </c>
+      <c r="K856">
+        <v>0</v>
+      </c>
+      <c r="L856">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="857" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A857" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B857" s="1" t="s">
+        <v>1563</v>
+      </c>
+      <c r="C857" t="s">
+        <v>13</v>
+      </c>
+      <c r="D857" t="s">
+        <v>13</v>
+      </c>
+      <c r="E857" t="s">
+        <v>14</v>
+      </c>
+      <c r="F857">
+        <v>0</v>
+      </c>
+      <c r="G857">
+        <v>0</v>
+      </c>
+      <c r="H857">
+        <v>14642.8375</v>
+      </c>
+      <c r="I857">
+        <v>0.2117</v>
+      </c>
+      <c r="J857">
+        <v>0.7994</v>
+      </c>
+      <c r="K857">
+        <v>0</v>
+      </c>
+      <c r="L857">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="858" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A858" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B858" s="1" t="s">
+        <v>1564</v>
+      </c>
+      <c r="C858" t="s">
+        <v>13</v>
+      </c>
+      <c r="D858" t="s">
+        <v>13</v>
+      </c>
+      <c r="E858" t="s">
+        <v>14</v>
+      </c>
+      <c r="F858">
+        <v>0</v>
+      </c>
+      <c r="G858">
+        <v>1</v>
+      </c>
+      <c r="H858">
+        <v>10433.596799999999</v>
+      </c>
+      <c r="I858">
+        <v>0.2336</v>
+      </c>
+      <c r="J858">
+        <v>0.3165</v>
+      </c>
+      <c r="K858">
+        <v>0</v>
+      </c>
+      <c r="L858">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="859" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A859" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B859" s="1" t="s">
+        <v>1565</v>
+      </c>
+      <c r="C859" t="s">
+        <v>13</v>
+      </c>
+      <c r="D859" t="s">
+        <v>13</v>
+      </c>
+      <c r="E859" t="s">
+        <v>14</v>
+      </c>
+      <c r="F859">
+        <v>0</v>
+      </c>
+      <c r="G859">
+        <v>2</v>
+      </c>
+      <c r="H859">
+        <v>9759.5581999999995</v>
+      </c>
+      <c r="I859">
+        <v>0.1222</v>
+      </c>
+      <c r="J859">
+        <v>2.2395</v>
+      </c>
+      <c r="K859">
+        <v>0</v>
+      </c>
+      <c r="L859">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="860" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A860" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B860" s="1" t="s">
+        <v>1566</v>
+      </c>
+      <c r="C860" t="s">
+        <v>13</v>
+      </c>
+      <c r="D860" t="s">
+        <v>13</v>
+      </c>
+      <c r="E860" t="s">
+        <v>14</v>
+      </c>
+      <c r="F860">
+        <v>1</v>
+      </c>
+      <c r="G860">
+        <v>0</v>
+      </c>
+      <c r="H860">
+        <v>4627.2646999999997</v>
+      </c>
+      <c r="I860">
+        <v>0.40129999999999999</v>
+      </c>
+      <c r="J860">
+        <v>1.5008999999999999</v>
+      </c>
+      <c r="K860">
+        <v>0</v>
+      </c>
+      <c r="L860">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="861" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A861" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B861" s="1" t="s">
+        <v>1567</v>
+      </c>
+      <c r="C861" t="s">
+        <v>13</v>
+      </c>
+      <c r="D861" t="s">
+        <v>13</v>
+      </c>
+      <c r="E861" t="s">
+        <v>14</v>
+      </c>
+      <c r="F861">
+        <v>1</v>
+      </c>
+      <c r="G861">
+        <v>1</v>
+      </c>
+      <c r="H861">
+        <v>1304.0745999999999</v>
+      </c>
+      <c r="I861">
+        <v>0.30130000000000001</v>
+      </c>
+      <c r="J861">
+        <v>2.1299000000000001</v>
+      </c>
+      <c r="K861">
+        <v>0</v>
+      </c>
+      <c r="L861">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="862" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A862" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B862" s="1" t="s">
+        <v>1568</v>
+      </c>
+      <c r="C862" t="s">
+        <v>13</v>
+      </c>
+      <c r="D862" t="s">
+        <v>13</v>
+      </c>
+      <c r="E862" t="s">
+        <v>14</v>
+      </c>
+      <c r="F862">
+        <v>1</v>
+      </c>
+      <c r="G862">
+        <v>2</v>
+      </c>
+      <c r="H862">
+        <v>6103.3491000000004</v>
+      </c>
+      <c r="I862">
+        <v>0.10050000000000001</v>
+      </c>
+      <c r="J862">
+        <v>4.3432000000000004</v>
+      </c>
+      <c r="K862">
+        <v>0</v>
+      </c>
+      <c r="L862">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="863" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A863" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B863" s="1" t="s">
+        <v>1569</v>
+      </c>
+      <c r="C863" t="s">
+        <v>13</v>
+      </c>
+      <c r="D863" t="s">
+        <v>13</v>
+      </c>
+      <c r="E863" t="s">
+        <v>14</v>
+      </c>
+      <c r="F863">
+        <v>2</v>
+      </c>
+      <c r="G863">
+        <v>0</v>
+      </c>
+      <c r="H863">
+        <v>4239.2424000000001</v>
+      </c>
+      <c r="I863">
+        <v>0.36409999999999998</v>
+      </c>
+      <c r="J863">
+        <v>1.9902</v>
+      </c>
+      <c r="K863">
+        <v>0</v>
+      </c>
+      <c r="L863">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="864" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A864" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B864" s="1" t="s">
+        <v>1570</v>
+      </c>
+      <c r="C864" t="s">
+        <v>13</v>
+      </c>
+      <c r="D864" t="s">
+        <v>13</v>
+      </c>
+      <c r="E864" t="s">
+        <v>14</v>
+      </c>
+      <c r="F864">
+        <v>2</v>
+      </c>
+      <c r="G864">
+        <v>1</v>
+      </c>
+      <c r="H864">
+        <v>1446.0826999999999</v>
+      </c>
+      <c r="I864">
+        <v>0.42309999999999998</v>
+      </c>
+      <c r="J864">
+        <v>1.4625999999999999</v>
+      </c>
+      <c r="K864">
+        <v>0</v>
+      </c>
+      <c r="L864">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="865" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A865" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B865" s="1" t="s">
+        <v>1571</v>
+      </c>
+      <c r="C865" t="s">
+        <v>13</v>
+      </c>
+      <c r="D865" t="s">
+        <v>13</v>
+      </c>
+      <c r="E865" t="s">
+        <v>14</v>
+      </c>
+      <c r="F865">
+        <v>2</v>
+      </c>
+      <c r="G865">
+        <v>2</v>
+      </c>
+      <c r="H865">
+        <v>5146.2942999999996</v>
+      </c>
+      <c r="I865">
+        <v>0.21360000000000001</v>
+      </c>
+      <c r="J865">
+        <v>3.4283999999999999</v>
+      </c>
+      <c r="K865">
+        <v>0</v>
+      </c>
+      <c r="L865">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
All data + tagging for P11
</commit_message>
<xml_diff>
--- a/Data/exp2-consolidated.xlsx
+++ b/Data/exp2-consolidated.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7139" uniqueCount="1791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7679" uniqueCount="1900">
   <si>
     <t>Ticks</t>
   </si>
@@ -5389,6 +5389,333 @@
   </si>
   <si>
     <t>P10</t>
+  </si>
+  <si>
+    <t>P11</t>
+  </si>
+  <si>
+    <t>635145988741703640</t>
+  </si>
+  <si>
+    <t>635145988867780851</t>
+  </si>
+  <si>
+    <t>635145988957906006</t>
+  </si>
+  <si>
+    <t>635145989096343924</t>
+  </si>
+  <si>
+    <t>635145989280464455</t>
+  </si>
+  <si>
+    <t>635145989351298507</t>
+  </si>
+  <si>
+    <t>635145989460304742</t>
+  </si>
+  <si>
+    <t>635145989562460585</t>
+  </si>
+  <si>
+    <t>635145989665976505</t>
+  </si>
+  <si>
+    <t>635145989805294474</t>
+  </si>
+  <si>
+    <t>635145989850017032</t>
+  </si>
+  <si>
+    <t>635145989942972349</t>
+  </si>
+  <si>
+    <t>635145990047138306</t>
+  </si>
+  <si>
+    <t>635145990136773433</t>
+  </si>
+  <si>
+    <t>635145990209257579</t>
+  </si>
+  <si>
+    <t>635145990283811843</t>
+  </si>
+  <si>
+    <t>635145990387407769</t>
+  </si>
+  <si>
+    <t>635145990438820709</t>
+  </si>
+  <si>
+    <t>635145990556777456</t>
+  </si>
+  <si>
+    <t>635145990639652196</t>
+  </si>
+  <si>
+    <t>635145990759729064</t>
+  </si>
+  <si>
+    <t>635145990887136352</t>
+  </si>
+  <si>
+    <t>635145991017813826</t>
+  </si>
+  <si>
+    <t>635145991096888349</t>
+  </si>
+  <si>
+    <t>635145991181893211</t>
+  </si>
+  <si>
+    <t>635145991267908131</t>
+  </si>
+  <si>
+    <t>635145991326651490</t>
+  </si>
+  <si>
+    <t>635145991877683008</t>
+  </si>
+  <si>
+    <t>635145992133677650</t>
+  </si>
+  <si>
+    <t>635145992339679432</t>
+  </si>
+  <si>
+    <t>635145992504638867</t>
+  </si>
+  <si>
+    <t>635145992668198223</t>
+  </si>
+  <si>
+    <t>635145992775474358</t>
+  </si>
+  <si>
+    <t>635145992902351615</t>
+  </si>
+  <si>
+    <t>635145992992516773</t>
+  </si>
+  <si>
+    <t>635145993030918969</t>
+  </si>
+  <si>
+    <t>635145993672315655</t>
+  </si>
+  <si>
+    <t>635145993768071132</t>
+  </si>
+  <si>
+    <t>635145993839565221</t>
+  </si>
+  <si>
+    <t>635145993894148343</t>
+  </si>
+  <si>
+    <t>635145993938750894</t>
+  </si>
+  <si>
+    <t>635145994010264984</t>
+  </si>
+  <si>
+    <t>635145994085829306</t>
+  </si>
+  <si>
+    <t>635145994167503978</t>
+  </si>
+  <si>
+    <t>635145994251908806</t>
+  </si>
+  <si>
+    <t>635145994663902370</t>
+  </si>
+  <si>
+    <t>635145994844862721</t>
+  </si>
+  <si>
+    <t>635145994983620657</t>
+  </si>
+  <si>
+    <t>635145995019702721</t>
+  </si>
+  <si>
+    <t>635145995052504597</t>
+  </si>
+  <si>
+    <t>635145995144699870</t>
+  </si>
+  <si>
+    <t>635145995189742447</t>
+  </si>
+  <si>
+    <t>635145995302938921</t>
+  </si>
+  <si>
+    <t>635145995338860976</t>
+  </si>
+  <si>
+    <t>635145995739173872</t>
+  </si>
+  <si>
+    <t>635145995827658933</t>
+  </si>
+  <si>
+    <t>635145995919174168</t>
+  </si>
+  <si>
+    <t>635145995999058737</t>
+  </si>
+  <si>
+    <t>635145996084193606</t>
+  </si>
+  <si>
+    <t>635145996164618206</t>
+  </si>
+  <si>
+    <t>635145996201490315</t>
+  </si>
+  <si>
+    <t>635145996227251789</t>
+  </si>
+  <si>
+    <t>635145996353008982</t>
+  </si>
+  <si>
+    <t>635145996866048326</t>
+  </si>
+  <si>
+    <t>635145996929371948</t>
+  </si>
+  <si>
+    <t>635145997155804899</t>
+  </si>
+  <si>
+    <t>635145997203447624</t>
+  </si>
+  <si>
+    <t>635145997290162584</t>
+  </si>
+  <si>
+    <t>635145997350086011</t>
+  </si>
+  <si>
+    <t>635145997429040527</t>
+  </si>
+  <si>
+    <t>635145997454721996</t>
+  </si>
+  <si>
+    <t>635145997537286718</t>
+  </si>
+  <si>
+    <t>635145997943639961</t>
+  </si>
+  <si>
+    <t>635145997971721567</t>
+  </si>
+  <si>
+    <t>635145997992102732</t>
+  </si>
+  <si>
+    <t>635145998018124221</t>
+  </si>
+  <si>
+    <t>635145998083197943</t>
+  </si>
+  <si>
+    <t>635145998147521622</t>
+  </si>
+  <si>
+    <t>635145998206194978</t>
+  </si>
+  <si>
+    <t>635145998279919195</t>
+  </si>
+  <si>
+    <t>635145998301040403</t>
+  </si>
+  <si>
+    <t>635145998802189067</t>
+  </si>
+  <si>
+    <t>635145999028712023</t>
+  </si>
+  <si>
+    <t>635145999132187942</t>
+  </si>
+  <si>
+    <t>635145999297387390</t>
+  </si>
+  <si>
+    <t>635145999485988178</t>
+  </si>
+  <si>
+    <t>635145999663428327</t>
+  </si>
+  <si>
+    <t>635145999876150494</t>
+  </si>
+  <si>
+    <t>635146000046070213</t>
+  </si>
+  <si>
+    <t>635146000201349094</t>
+  </si>
+  <si>
+    <t>635146000528617813</t>
+  </si>
+  <si>
+    <t>635146000783542394</t>
+  </si>
+  <si>
+    <t>635146000906019399</t>
+  </si>
+  <si>
+    <t>635146001102300626</t>
+  </si>
+  <si>
+    <t>635146001183575274</t>
+  </si>
+  <si>
+    <t>635146001248779004</t>
+  </si>
+  <si>
+    <t>635146001323013250</t>
+  </si>
+  <si>
+    <t>635146001389457050</t>
+  </si>
+  <si>
+    <t>635146001541415742</t>
+  </si>
+  <si>
+    <t>635146001738617021</t>
+  </si>
+  <si>
+    <t>635146001831012306</t>
+  </si>
+  <si>
+    <t>635146002084086781</t>
+  </si>
+  <si>
+    <t>635146002239535672</t>
+  </si>
+  <si>
+    <t>635146002407405273</t>
+  </si>
+  <si>
+    <t>635146002515811474</t>
+  </si>
+  <si>
+    <t>635146002660329740</t>
+  </si>
+  <si>
+    <t>635146002799567704</t>
+  </si>
+  <si>
+    <t>635146002888392784</t>
   </si>
 </sst>
 </file>
@@ -5736,10 +6063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1081"/>
+  <dimension ref="A1:L1189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1078" workbookViewId="0">
-      <selection activeCell="B1083" sqref="B1083"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46826,6 +47153,4110 @@
         <v>2.3317000000000001</v>
       </c>
       <c r="L1081">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1082" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1082" s="1" t="s">
+        <v>1792</v>
+      </c>
+      <c r="C1082" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1082" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1082" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1082">
+        <v>0</v>
+      </c>
+      <c r="G1082">
+        <v>0</v>
+      </c>
+      <c r="H1082">
+        <v>24158.381799999999</v>
+      </c>
+      <c r="I1082">
+        <v>0.1249</v>
+      </c>
+      <c r="J1082">
+        <v>0.57310000000000005</v>
+      </c>
+      <c r="K1082">
+        <v>1.6328</v>
+      </c>
+      <c r="L1082">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1083" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1083" s="1" t="s">
+        <v>1793</v>
+      </c>
+      <c r="C1083" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1083" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1083" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1083">
+        <v>0</v>
+      </c>
+      <c r="G1083">
+        <v>1</v>
+      </c>
+      <c r="H1083">
+        <v>63514598886778.102</v>
+      </c>
+      <c r="I1083">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="J1083">
+        <v>2.0874999999999999</v>
+      </c>
+      <c r="K1083">
+        <v>1.6653</v>
+      </c>
+      <c r="L1083">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1084" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1084" s="1" t="s">
+        <v>1794</v>
+      </c>
+      <c r="C1084" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1084" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1084" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1084">
+        <v>0</v>
+      </c>
+      <c r="G1084">
+        <v>2</v>
+      </c>
+      <c r="H1084">
+        <v>7755.4435999999996</v>
+      </c>
+      <c r="I1084">
+        <v>9.0899999999999995E-2</v>
+      </c>
+      <c r="J1084">
+        <v>3.7376</v>
+      </c>
+      <c r="K1084">
+        <v>1.7493000000000001</v>
+      </c>
+      <c r="L1084">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1085" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1085" s="1" t="s">
+        <v>1795</v>
+      </c>
+      <c r="C1085" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1085" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1085" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1085">
+        <v>1</v>
+      </c>
+      <c r="G1085">
+        <v>0</v>
+      </c>
+      <c r="H1085">
+        <v>12879.736699999999</v>
+      </c>
+      <c r="I1085">
+        <v>0.126</v>
+      </c>
+      <c r="J1085">
+        <v>2.0735999999999999</v>
+      </c>
+      <c r="K1085">
+        <v>1.8643000000000001</v>
+      </c>
+      <c r="L1085">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1086" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1086" s="1" t="s">
+        <v>1796</v>
+      </c>
+      <c r="C1086" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1086" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1086" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1086">
+        <v>1</v>
+      </c>
+      <c r="G1086">
+        <v>1</v>
+      </c>
+      <c r="H1086">
+        <v>17508.001400000001</v>
+      </c>
+      <c r="I1086">
+        <v>6.3399999999999998E-2</v>
+      </c>
+      <c r="J1086">
+        <v>2.4780000000000002</v>
+      </c>
+      <c r="K1086">
+        <v>1.6941999999999999</v>
+      </c>
+      <c r="L1086">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1087" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1087" s="1" t="s">
+        <v>1797</v>
+      </c>
+      <c r="C1087" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1087" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1087" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1087">
+        <v>1</v>
+      </c>
+      <c r="G1087">
+        <v>2</v>
+      </c>
+      <c r="H1087">
+        <v>6007.3436000000002</v>
+      </c>
+      <c r="I1087">
+        <v>5.4600000000000003E-2</v>
+      </c>
+      <c r="J1087">
+        <v>0.22140000000000001</v>
+      </c>
+      <c r="K1087">
+        <v>1.8576999999999999</v>
+      </c>
+      <c r="L1087">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1088" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1088" s="1" t="s">
+        <v>1798</v>
+      </c>
+      <c r="C1088" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1088" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1088" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1088">
+        <v>2</v>
+      </c>
+      <c r="G1088">
+        <v>0</v>
+      </c>
+      <c r="H1088">
+        <v>9844.5630999999994</v>
+      </c>
+      <c r="I1088">
+        <v>7.6799999999999993E-2</v>
+      </c>
+      <c r="J1088">
+        <v>1.1753</v>
+      </c>
+      <c r="K1088">
+        <v>1.7928999999999999</v>
+      </c>
+      <c r="L1088">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1089" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1089" s="1" t="s">
+        <v>1799</v>
+      </c>
+      <c r="C1089" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1089" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1089" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1089">
+        <v>2</v>
+      </c>
+      <c r="G1089">
+        <v>1</v>
+      </c>
+      <c r="H1089">
+        <v>9343.5344999999998</v>
+      </c>
+      <c r="I1089">
+        <v>7.4899999999999994E-2</v>
+      </c>
+      <c r="J1089">
+        <v>0.32340000000000002</v>
+      </c>
+      <c r="K1089">
+        <v>2.1387</v>
+      </c>
+      <c r="L1089">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1090" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1090" s="1" t="s">
+        <v>1800</v>
+      </c>
+      <c r="C1090" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1090" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1090" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1090">
+        <v>2</v>
+      </c>
+      <c r="G1090">
+        <v>2</v>
+      </c>
+      <c r="H1090">
+        <v>9531.5450999999994</v>
+      </c>
+      <c r="I1090">
+        <v>7.3400000000000007E-2</v>
+      </c>
+      <c r="J1090">
+        <v>1.2209000000000001</v>
+      </c>
+      <c r="K1090">
+        <v>1.6251</v>
+      </c>
+      <c r="L1090">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1091" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1091" s="1" t="s">
+        <v>1801</v>
+      </c>
+      <c r="C1091" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1091" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1091" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1091">
+        <v>0</v>
+      </c>
+      <c r="G1091">
+        <v>0</v>
+      </c>
+      <c r="H1091">
+        <v>13062.7472</v>
+      </c>
+      <c r="I1091">
+        <v>0.13</v>
+      </c>
+      <c r="J1091">
+        <v>0.57020000000000004</v>
+      </c>
+      <c r="K1091">
+        <v>1.5951</v>
+      </c>
+      <c r="L1091">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1092" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1092" s="1" t="s">
+        <v>1802</v>
+      </c>
+      <c r="C1092" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1092" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1092" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1092">
+        <v>0</v>
+      </c>
+      <c r="G1092">
+        <v>1</v>
+      </c>
+      <c r="H1092">
+        <v>3387.1938</v>
+      </c>
+      <c r="I1092">
+        <v>7.6300000000000007E-2</v>
+      </c>
+      <c r="J1092">
+        <v>1.278</v>
+      </c>
+      <c r="K1092">
+        <v>1.4791000000000001</v>
+      </c>
+      <c r="L1092">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1093" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1093" s="1" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C1093" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1093" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1093" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1093">
+        <v>0</v>
+      </c>
+      <c r="G1093">
+        <v>2</v>
+      </c>
+      <c r="H1093">
+        <v>8455.4837000000007</v>
+      </c>
+      <c r="I1093">
+        <v>0.1229</v>
+      </c>
+      <c r="J1093">
+        <v>1.8988</v>
+      </c>
+      <c r="K1093">
+        <v>1.8622000000000001</v>
+      </c>
+      <c r="L1093">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1094" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1094" s="1" t="s">
+        <v>1804</v>
+      </c>
+      <c r="C1094" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1094" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1094" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1094">
+        <v>1</v>
+      </c>
+      <c r="G1094">
+        <v>0</v>
+      </c>
+      <c r="H1094">
+        <v>9359.5352999999996</v>
+      </c>
+      <c r="I1094">
+        <v>5.4399999999999997E-2</v>
+      </c>
+      <c r="J1094">
+        <v>0.36449999999999999</v>
+      </c>
+      <c r="K1094">
+        <v>1.5949</v>
+      </c>
+      <c r="L1094">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1095" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1095" s="1" t="s">
+        <v>1805</v>
+      </c>
+      <c r="C1095" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1095" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1095" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1095">
+        <v>1</v>
+      </c>
+      <c r="G1095">
+        <v>1</v>
+      </c>
+      <c r="H1095">
+        <v>8231.4707999999991</v>
+      </c>
+      <c r="I1095">
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="J1095">
+        <v>1.4032</v>
+      </c>
+      <c r="K1095">
+        <v>1.4892000000000001</v>
+      </c>
+      <c r="L1095">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1096" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1096" s="1" t="s">
+        <v>1806</v>
+      </c>
+      <c r="C1096" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1096" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1096" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1096">
+        <v>1</v>
+      </c>
+      <c r="G1096">
+        <v>2</v>
+      </c>
+      <c r="H1096">
+        <v>6260.3581000000004</v>
+      </c>
+      <c r="I1096">
+        <v>5.6800000000000003E-2</v>
+      </c>
+      <c r="J1096">
+        <v>1.2042999999999999</v>
+      </c>
+      <c r="K1096">
+        <v>1.5818000000000001</v>
+      </c>
+      <c r="L1096">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1097" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1097" s="1" t="s">
+        <v>1807</v>
+      </c>
+      <c r="C1097" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1097" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1097" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1097">
+        <v>2</v>
+      </c>
+      <c r="G1097">
+        <v>0</v>
+      </c>
+      <c r="H1097">
+        <v>6539.3739999999998</v>
+      </c>
+      <c r="I1097">
+        <v>0</v>
+      </c>
+      <c r="J1097">
+        <v>2.1676000000000002</v>
+      </c>
+      <c r="K1097">
+        <v>1.5601</v>
+      </c>
+      <c r="L1097">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1098" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1098" s="1" t="s">
+        <v>1808</v>
+      </c>
+      <c r="C1098" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1098" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1098" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1098">
+        <v>2</v>
+      </c>
+      <c r="G1098">
+        <v>1</v>
+      </c>
+      <c r="H1098">
+        <v>9338.5342000000001</v>
+      </c>
+      <c r="I1098">
+        <v>0.1118</v>
+      </c>
+      <c r="J1098">
+        <v>1.9366000000000001</v>
+      </c>
+      <c r="K1098">
+        <v>1.6928000000000001</v>
+      </c>
+      <c r="L1098">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1099" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1099" s="1" t="s">
+        <v>1809</v>
+      </c>
+      <c r="C1099" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1099" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1099" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1099">
+        <v>2</v>
+      </c>
+      <c r="G1099">
+        <v>2</v>
+      </c>
+      <c r="H1099">
+        <v>4552.2602999999999</v>
+      </c>
+      <c r="I1099">
+        <v>0.10920000000000001</v>
+      </c>
+      <c r="J1099">
+        <v>2.2509999999999999</v>
+      </c>
+      <c r="K1099">
+        <v>1.8429</v>
+      </c>
+      <c r="L1099">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1100" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1100" s="1" t="s">
+        <v>1810</v>
+      </c>
+      <c r="C1100" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1100" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1100" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1100">
+        <v>0</v>
+      </c>
+      <c r="G1100">
+        <v>0</v>
+      </c>
+      <c r="H1100">
+        <v>10683.611000000001</v>
+      </c>
+      <c r="I1100">
+        <v>5.74E-2</v>
+      </c>
+      <c r="J1100">
+        <v>0.2079</v>
+      </c>
+      <c r="K1100">
+        <v>2.7902999999999998</v>
+      </c>
+      <c r="L1100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1101" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1101" s="1" t="s">
+        <v>1811</v>
+      </c>
+      <c r="C1101" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1101" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1101" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1101">
+        <v>0</v>
+      </c>
+      <c r="G1101">
+        <v>1</v>
+      </c>
+      <c r="H1101">
+        <v>7463.4268000000002</v>
+      </c>
+      <c r="I1101">
+        <v>7.3300000000000004E-2</v>
+      </c>
+      <c r="J1101">
+        <v>3.5552999999999999</v>
+      </c>
+      <c r="K1101">
+        <v>3.1644999999999999</v>
+      </c>
+      <c r="L1101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1102" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1102" s="1" t="s">
+        <v>1812</v>
+      </c>
+      <c r="C1102" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1102" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1102" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1102">
+        <v>0</v>
+      </c>
+      <c r="G1102">
+        <v>2</v>
+      </c>
+      <c r="H1102">
+        <v>9855.5637000000006</v>
+      </c>
+      <c r="I1102">
+        <v>0.18540000000000001</v>
+      </c>
+      <c r="J1102">
+        <v>3.9125000000000001</v>
+      </c>
+      <c r="K1102">
+        <v>2.7431000000000001</v>
+      </c>
+      <c r="L1102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1103" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1103" s="1" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C1103" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1103" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1103" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1103">
+        <v>1</v>
+      </c>
+      <c r="G1103">
+        <v>0</v>
+      </c>
+      <c r="H1103">
+        <v>11828.676600000001</v>
+      </c>
+      <c r="I1103">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="J1103">
+        <v>2.5750000000000002</v>
+      </c>
+      <c r="K1103">
+        <v>2.0222000000000002</v>
+      </c>
+      <c r="L1103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1104" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1104" s="1" t="s">
+        <v>1814</v>
+      </c>
+      <c r="C1104" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1104" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1104" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1104">
+        <v>1</v>
+      </c>
+      <c r="G1104">
+        <v>1</v>
+      </c>
+      <c r="H1104">
+        <v>12375.707899999999</v>
+      </c>
+      <c r="I1104">
+        <v>0.10050000000000001</v>
+      </c>
+      <c r="J1104">
+        <v>4.3327999999999998</v>
+      </c>
+      <c r="K1104">
+        <v>2.1034999999999999</v>
+      </c>
+      <c r="L1104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1105" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1105" s="1" t="s">
+        <v>1815</v>
+      </c>
+      <c r="C1105" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1105" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1105" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1105">
+        <v>1</v>
+      </c>
+      <c r="G1105">
+        <v>2</v>
+      </c>
+      <c r="H1105">
+        <v>5847.3344999999999</v>
+      </c>
+      <c r="I1105">
+        <v>0.1028</v>
+      </c>
+      <c r="J1105">
+        <v>2.0539999999999998</v>
+      </c>
+      <c r="K1105">
+        <v>2.3003</v>
+      </c>
+      <c r="L1105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1106" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1106" s="1" t="s">
+        <v>1816</v>
+      </c>
+      <c r="C1106" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1106" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1106" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1106">
+        <v>2</v>
+      </c>
+      <c r="G1106">
+        <v>0</v>
+      </c>
+      <c r="H1106">
+        <v>7320.4187000000002</v>
+      </c>
+      <c r="I1106">
+        <v>8.5699999999999998E-2</v>
+      </c>
+      <c r="J1106">
+        <v>2.2557999999999998</v>
+      </c>
+      <c r="K1106">
+        <v>2.2652000000000001</v>
+      </c>
+      <c r="L1106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1107" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1107" s="1" t="s">
+        <v>1817</v>
+      </c>
+      <c r="C1107" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1107" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1107" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1107">
+        <v>2</v>
+      </c>
+      <c r="G1107">
+        <v>1</v>
+      </c>
+      <c r="H1107">
+        <v>7921.4530999999997</v>
+      </c>
+      <c r="I1107">
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="J1107">
+        <v>2.7749999999999999</v>
+      </c>
+      <c r="K1107">
+        <v>2.1004</v>
+      </c>
+      <c r="L1107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1108" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1108" s="1" t="s">
+        <v>1818</v>
+      </c>
+      <c r="C1108" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1108" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1108" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1108">
+        <v>2</v>
+      </c>
+      <c r="G1108">
+        <v>2</v>
+      </c>
+      <c r="H1108">
+        <v>5176.2960000000003</v>
+      </c>
+      <c r="I1108">
+        <v>0.21179999999999999</v>
+      </c>
+      <c r="J1108">
+        <v>3.6798999999999999</v>
+      </c>
+      <c r="K1108">
+        <v>2.3081</v>
+      </c>
+      <c r="L1108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1109" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1109" s="1" t="s">
+        <v>1819</v>
+      </c>
+      <c r="C1109" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1109" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1109" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1109">
+        <v>0</v>
+      </c>
+      <c r="G1109">
+        <v>0</v>
+      </c>
+      <c r="H1109">
+        <v>54251.103000000003</v>
+      </c>
+      <c r="I1109">
+        <v>6.3700000000000007E-2</v>
+      </c>
+      <c r="J1109">
+        <v>1.4879</v>
+      </c>
+      <c r="K1109">
+        <v>0</v>
+      </c>
+      <c r="L1109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1110" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1110" s="1" t="s">
+        <v>1820</v>
+      </c>
+      <c r="C1110" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1110" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1110" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1110">
+        <v>0</v>
+      </c>
+      <c r="G1110">
+        <v>1</v>
+      </c>
+      <c r="H1110">
+        <v>23843.363799999999</v>
+      </c>
+      <c r="I1110">
+        <v>7.3300000000000004E-2</v>
+      </c>
+      <c r="J1110">
+        <v>1.9581</v>
+      </c>
+      <c r="K1110">
+        <v>0</v>
+      </c>
+      <c r="L1110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1111" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1111" s="1" t="s">
+        <v>1821</v>
+      </c>
+      <c r="C1111" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1111" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1111" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1111">
+        <v>0</v>
+      </c>
+      <c r="G1111">
+        <v>2</v>
+      </c>
+      <c r="H1111">
+        <v>19039.088899999999</v>
+      </c>
+      <c r="I1111">
+        <v>9.2700000000000005E-2</v>
+      </c>
+      <c r="J1111">
+        <v>0</v>
+      </c>
+      <c r="K1111">
+        <v>0</v>
+      </c>
+      <c r="L1111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1112" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1112" s="1" t="s">
+        <v>1822</v>
+      </c>
+      <c r="C1112" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1112" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1112" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1112">
+        <v>1</v>
+      </c>
+      <c r="G1112">
+        <v>0</v>
+      </c>
+      <c r="H1112">
+        <v>15503.886699999999</v>
+      </c>
+      <c r="I1112">
+        <v>0.43380000000000002</v>
+      </c>
+      <c r="J1112">
+        <v>1.1935</v>
+      </c>
+      <c r="K1112">
+        <v>0</v>
+      </c>
+      <c r="L1112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1113" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1113" s="1" t="s">
+        <v>1823</v>
+      </c>
+      <c r="C1113" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1113" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1113" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1113">
+        <v>1</v>
+      </c>
+      <c r="G1113">
+        <v>1</v>
+      </c>
+      <c r="H1113">
+        <v>15135.8658</v>
+      </c>
+      <c r="I1113">
+        <v>0.2712</v>
+      </c>
+      <c r="J1113">
+        <v>0.63660000000000005</v>
+      </c>
+      <c r="K1113">
+        <v>0</v>
+      </c>
+      <c r="L1113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1114" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1114" s="1" t="s">
+        <v>1824</v>
+      </c>
+      <c r="C1114" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1114" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1114" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1114">
+        <v>1</v>
+      </c>
+      <c r="G1114">
+        <v>2</v>
+      </c>
+      <c r="H1114">
+        <v>9419.5386999999992</v>
+      </c>
+      <c r="I1114">
+        <v>0.42309999999999998</v>
+      </c>
+      <c r="J1114">
+        <v>0.68210000000000004</v>
+      </c>
+      <c r="K1114">
+        <v>0</v>
+      </c>
+      <c r="L1114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1115" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1115" s="1" t="s">
+        <v>1825</v>
+      </c>
+      <c r="C1115" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1115" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1115" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1115">
+        <v>2</v>
+      </c>
+      <c r="G1115">
+        <v>0</v>
+      </c>
+      <c r="H1115">
+        <v>11391.6515</v>
+      </c>
+      <c r="I1115">
+        <v>9.6199999999999994E-2</v>
+      </c>
+      <c r="J1115">
+        <v>1.3322000000000001</v>
+      </c>
+      <c r="K1115">
+        <v>0</v>
+      </c>
+      <c r="L1115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1116" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1116" s="1" t="s">
+        <v>1826</v>
+      </c>
+      <c r="C1116" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1116" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1116" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1116">
+        <v>2</v>
+      </c>
+      <c r="G1116">
+        <v>1</v>
+      </c>
+      <c r="H1116">
+        <v>8191.4686000000002</v>
+      </c>
+      <c r="I1116">
+        <v>0.1648</v>
+      </c>
+      <c r="J1116">
+        <v>4.3986999999999998</v>
+      </c>
+      <c r="K1116">
+        <v>0</v>
+      </c>
+      <c r="L1116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1117" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1117" s="1" t="s">
+        <v>1827</v>
+      </c>
+      <c r="C1117" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1117" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1117" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1117">
+        <v>2</v>
+      </c>
+      <c r="G1117">
+        <v>2</v>
+      </c>
+      <c r="H1117">
+        <v>3052.1745999999998</v>
+      </c>
+      <c r="I1117">
+        <v>7.7700000000000005E-2</v>
+      </c>
+      <c r="J1117">
+        <v>3.0448</v>
+      </c>
+      <c r="K1117">
+        <v>0</v>
+      </c>
+      <c r="L1117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1118" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1118" s="1" t="s">
+        <v>1828</v>
+      </c>
+      <c r="C1118" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1118" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1118" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1118">
+        <v>0</v>
+      </c>
+      <c r="G1118">
+        <v>0</v>
+      </c>
+      <c r="H1118">
+        <v>63355.623800000001</v>
+      </c>
+      <c r="I1118">
+        <v>7.3599999999999999E-2</v>
+      </c>
+      <c r="J1118">
+        <v>2.92E-2</v>
+      </c>
+      <c r="K1118">
+        <v>0</v>
+      </c>
+      <c r="L1118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1119" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1119" s="1" t="s">
+        <v>1829</v>
+      </c>
+      <c r="C1119" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1119" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1119" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1119">
+        <v>0</v>
+      </c>
+      <c r="G1119">
+        <v>1</v>
+      </c>
+      <c r="H1119">
+        <v>8571.4902999999995</v>
+      </c>
+      <c r="I1119">
+        <v>0.14630000000000001</v>
+      </c>
+      <c r="J1119">
+        <v>0.44390000000000002</v>
+      </c>
+      <c r="K1119">
+        <v>0</v>
+      </c>
+      <c r="L1119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1120" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1120" s="1" t="s">
+        <v>1830</v>
+      </c>
+      <c r="C1120" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1120" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1120" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1120">
+        <v>0</v>
+      </c>
+      <c r="G1120">
+        <v>2</v>
+      </c>
+      <c r="H1120">
+        <v>6165.3526000000002</v>
+      </c>
+      <c r="I1120">
+        <v>0.18149999999999999</v>
+      </c>
+      <c r="J1120">
+        <v>0.58460000000000001</v>
+      </c>
+      <c r="K1120">
+        <v>0</v>
+      </c>
+      <c r="L1120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1121" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1121" s="1" t="s">
+        <v>1831</v>
+      </c>
+      <c r="C1121" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1121" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1121" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1121">
+        <v>1</v>
+      </c>
+      <c r="G1121">
+        <v>0</v>
+      </c>
+      <c r="H1121">
+        <v>4719.2699000000002</v>
+      </c>
+      <c r="I1121">
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="J1121">
+        <v>1.2777000000000001</v>
+      </c>
+      <c r="K1121">
+        <v>0</v>
+      </c>
+      <c r="L1121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1122" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1122" s="1" t="s">
+        <v>1832</v>
+      </c>
+      <c r="C1122" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1122" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1122" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1122">
+        <v>1</v>
+      </c>
+      <c r="G1122">
+        <v>1</v>
+      </c>
+      <c r="H1122">
+        <v>3552.2031999999999</v>
+      </c>
+      <c r="I1122">
+        <v>0.1148</v>
+      </c>
+      <c r="J1122">
+        <v>1.4715</v>
+      </c>
+      <c r="K1122">
+        <v>0</v>
+      </c>
+      <c r="L1122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1123" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1123" s="1" t="s">
+        <v>1833</v>
+      </c>
+      <c r="C1123" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1123" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1123" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1123">
+        <v>1</v>
+      </c>
+      <c r="G1123">
+        <v>2</v>
+      </c>
+      <c r="H1123">
+        <v>6183.3536000000004</v>
+      </c>
+      <c r="I1123">
+        <v>0.1283</v>
+      </c>
+      <c r="J1123">
+        <v>1.0416000000000001</v>
+      </c>
+      <c r="K1123">
+        <v>0</v>
+      </c>
+      <c r="L1123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1124" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1124" s="1" t="s">
+        <v>1834</v>
+      </c>
+      <c r="C1124" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1124" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1124" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1124">
+        <v>2</v>
+      </c>
+      <c r="G1124">
+        <v>0</v>
+      </c>
+      <c r="H1124">
+        <v>6859.3923000000004</v>
+      </c>
+      <c r="I1124">
+        <v>7.46E-2</v>
+      </c>
+      <c r="J1124">
+        <v>0.65649999999999997</v>
+      </c>
+      <c r="K1124">
+        <v>0</v>
+      </c>
+      <c r="L1124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1125" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1125" s="1" t="s">
+        <v>1835</v>
+      </c>
+      <c r="C1125" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1125" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1125" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1125">
+        <v>2</v>
+      </c>
+      <c r="G1125">
+        <v>1</v>
+      </c>
+      <c r="H1125">
+        <v>7315.4183999999996</v>
+      </c>
+      <c r="I1125">
+        <v>5.4300000000000001E-2</v>
+      </c>
+      <c r="J1125">
+        <v>0.58919999999999995</v>
+      </c>
+      <c r="K1125">
+        <v>0</v>
+      </c>
+      <c r="L1125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1126" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1126" s="1" t="s">
+        <v>1836</v>
+      </c>
+      <c r="C1126" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1126" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1126" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1126">
+        <v>2</v>
+      </c>
+      <c r="G1126">
+        <v>2</v>
+      </c>
+      <c r="H1126">
+        <v>7647.4373999999998</v>
+      </c>
+      <c r="I1126">
+        <v>7.6200000000000004E-2</v>
+      </c>
+      <c r="J1126">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="K1126">
+        <v>0</v>
+      </c>
+      <c r="L1126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1127" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1127" s="1" t="s">
+        <v>1837</v>
+      </c>
+      <c r="C1127" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1127" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1127" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1127">
+        <v>0</v>
+      </c>
+      <c r="G1127">
+        <v>0</v>
+      </c>
+      <c r="H1127">
+        <v>40450.313600000001</v>
+      </c>
+      <c r="I1127">
+        <v>0.2334</v>
+      </c>
+      <c r="J1127">
+        <v>1.7594000000000001</v>
+      </c>
+      <c r="K1127">
+        <v>0</v>
+      </c>
+      <c r="L1127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1128" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1128" s="1" t="s">
+        <v>1838</v>
+      </c>
+      <c r="C1128" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1128" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1128" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1128">
+        <v>0</v>
+      </c>
+      <c r="G1128">
+        <v>1</v>
+      </c>
+      <c r="H1128">
+        <v>16775.959599999998</v>
+      </c>
+      <c r="I1128">
+        <v>9.0200000000000002E-2</v>
+      </c>
+      <c r="J1128">
+        <v>0.89480000000000004</v>
+      </c>
+      <c r="K1128">
+        <v>0</v>
+      </c>
+      <c r="L1128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1129" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1129" s="1" t="s">
+        <v>1839</v>
+      </c>
+      <c r="C1129" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1129" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1129" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1129">
+        <v>0</v>
+      </c>
+      <c r="G1129">
+        <v>2</v>
+      </c>
+      <c r="H1129">
+        <v>13071.747600000001</v>
+      </c>
+      <c r="I1129">
+        <v>0.1696</v>
+      </c>
+      <c r="J1129">
+        <v>1.4528000000000001</v>
+      </c>
+      <c r="K1129">
+        <v>0</v>
+      </c>
+      <c r="L1129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1130" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1130" s="1" t="s">
+        <v>1840</v>
+      </c>
+      <c r="C1130" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1130" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1130" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1130">
+        <v>1</v>
+      </c>
+      <c r="G1130">
+        <v>0</v>
+      </c>
+      <c r="H1130">
+        <v>2572.1471000000001</v>
+      </c>
+      <c r="I1130">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="J1130">
+        <v>2.3243999999999998</v>
+      </c>
+      <c r="K1130">
+        <v>0</v>
+      </c>
+      <c r="L1130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1131" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1131" s="1" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C1131" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1131" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1131" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1131">
+        <v>1</v>
+      </c>
+      <c r="G1131">
+        <v>1</v>
+      </c>
+      <c r="H1131">
+        <v>2588.1480000000001</v>
+      </c>
+      <c r="I1131">
+        <v>0.20250000000000001</v>
+      </c>
+      <c r="J1131">
+        <v>0.72829999999999995</v>
+      </c>
+      <c r="K1131">
+        <v>0</v>
+      </c>
+      <c r="L1131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1132" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1132" s="1" t="s">
+        <v>1842</v>
+      </c>
+      <c r="C1132" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1132" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1132" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1132">
+        <v>1</v>
+      </c>
+      <c r="G1132">
+        <v>2</v>
+      </c>
+      <c r="H1132">
+        <v>8459.4838</v>
+      </c>
+      <c r="I1132">
+        <v>0.24560000000000001</v>
+      </c>
+      <c r="J1132">
+        <v>3.4681999999999999</v>
+      </c>
+      <c r="K1132">
+        <v>0</v>
+      </c>
+      <c r="L1132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1133" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1133" s="1" t="s">
+        <v>1843</v>
+      </c>
+      <c r="C1133" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1133" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1133" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1133">
+        <v>2</v>
+      </c>
+      <c r="G1133">
+        <v>0</v>
+      </c>
+      <c r="H1133">
+        <v>3776.2159999999999</v>
+      </c>
+      <c r="I1133">
+        <v>0.16950000000000001</v>
+      </c>
+      <c r="J1133">
+        <v>4.0856000000000003</v>
+      </c>
+      <c r="K1133">
+        <v>0</v>
+      </c>
+      <c r="L1133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1134" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1134" s="1" t="s">
+        <v>1844</v>
+      </c>
+      <c r="C1134" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1134" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1134" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1134">
+        <v>2</v>
+      </c>
+      <c r="G1134">
+        <v>1</v>
+      </c>
+      <c r="H1134">
+        <v>10555.6037</v>
+      </c>
+      <c r="I1134">
+        <v>4.7300000000000002E-2</v>
+      </c>
+      <c r="J1134">
+        <v>0.74409999999999998</v>
+      </c>
+      <c r="K1134">
+        <v>0</v>
+      </c>
+      <c r="L1134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1135" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1135" s="1" t="s">
+        <v>1845</v>
+      </c>
+      <c r="C1135" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1135" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1135" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1135">
+        <v>2</v>
+      </c>
+      <c r="G1135">
+        <v>2</v>
+      </c>
+      <c r="H1135">
+        <v>2696.1541999999999</v>
+      </c>
+      <c r="I1135">
+        <v>0.1376</v>
+      </c>
+      <c r="J1135">
+        <v>1.7508999999999999</v>
+      </c>
+      <c r="K1135">
+        <v>0</v>
+      </c>
+      <c r="L1135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1136" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1136" s="1" t="s">
+        <v>1846</v>
+      </c>
+      <c r="C1136" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1136" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1136" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1136">
+        <v>0</v>
+      </c>
+      <c r="G1136">
+        <v>0</v>
+      </c>
+      <c r="H1136">
+        <v>39370.251799999998</v>
+      </c>
+      <c r="I1136">
+        <v>0.1116</v>
+      </c>
+      <c r="J1136">
+        <v>0.69850000000000001</v>
+      </c>
+      <c r="K1136">
+        <v>0</v>
+      </c>
+      <c r="L1136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1137" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1137" s="1" t="s">
+        <v>1847</v>
+      </c>
+      <c r="C1137" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1137" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1137" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1137">
+        <v>0</v>
+      </c>
+      <c r="G1137">
+        <v>1</v>
+      </c>
+      <c r="H1137">
+        <v>8160.4666999999999</v>
+      </c>
+      <c r="I1137">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="J1137">
+        <v>6.3299999999999995E-2</v>
+      </c>
+      <c r="K1137">
+        <v>0</v>
+      </c>
+      <c r="L1137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1138" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1138" s="1" t="s">
+        <v>1848</v>
+      </c>
+      <c r="C1138" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1138" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1138" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1138">
+        <v>0</v>
+      </c>
+      <c r="G1138">
+        <v>2</v>
+      </c>
+      <c r="H1138">
+        <v>8383.4794999999995</v>
+      </c>
+      <c r="I1138">
+        <v>5.16E-2</v>
+      </c>
+      <c r="J1138">
+        <v>0.1237</v>
+      </c>
+      <c r="K1138">
+        <v>0</v>
+      </c>
+      <c r="L1138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1139" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1139" s="1" t="s">
+        <v>1849</v>
+      </c>
+      <c r="C1139" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1139" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1139" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1139">
+        <v>1</v>
+      </c>
+      <c r="G1139">
+        <v>0</v>
+      </c>
+      <c r="H1139">
+        <v>7280.4164000000001</v>
+      </c>
+      <c r="I1139">
+        <v>7.46E-2</v>
+      </c>
+      <c r="J1139">
+        <v>4.4499999999999998E-2</v>
+      </c>
+      <c r="K1139">
+        <v>0</v>
+      </c>
+      <c r="L1139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1140" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1140" s="1" t="s">
+        <v>1850</v>
+      </c>
+      <c r="C1140" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1140" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1140" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1140">
+        <v>1</v>
+      </c>
+      <c r="G1140">
+        <v>1</v>
+      </c>
+      <c r="H1140">
+        <v>7649.4375</v>
+      </c>
+      <c r="I1140">
+        <v>2.7713000000000001</v>
+      </c>
+      <c r="J1140">
+        <v>0.72840000000000005</v>
+      </c>
+      <c r="K1140">
+        <v>0</v>
+      </c>
+      <c r="L1140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1141" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1141" s="1" t="s">
+        <v>1851</v>
+      </c>
+      <c r="C1141" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1141" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1141" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1141">
+        <v>1</v>
+      </c>
+      <c r="G1141">
+        <v>2</v>
+      </c>
+      <c r="H1141">
+        <v>6960.3981000000003</v>
+      </c>
+      <c r="I1141">
+        <v>0.1651</v>
+      </c>
+      <c r="J1141">
+        <v>9.2100000000000001E-2</v>
+      </c>
+      <c r="K1141">
+        <v>0</v>
+      </c>
+      <c r="L1141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1142" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1142" s="1" t="s">
+        <v>1852</v>
+      </c>
+      <c r="C1142" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1142" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1142" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1142">
+        <v>2</v>
+      </c>
+      <c r="G1142">
+        <v>0</v>
+      </c>
+      <c r="H1142">
+        <v>2749.1572000000001</v>
+      </c>
+      <c r="I1142">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="J1142">
+        <v>0.95089999999999997</v>
+      </c>
+      <c r="K1142">
+        <v>0</v>
+      </c>
+      <c r="L1142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1143" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1143" s="1" t="s">
+        <v>1853</v>
+      </c>
+      <c r="C1143" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1143" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1143" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1143">
+        <v>2</v>
+      </c>
+      <c r="G1143">
+        <v>1</v>
+      </c>
+      <c r="H1143">
+        <v>1868.1069</v>
+      </c>
+      <c r="I1143">
+        <v>0.15529999999999999</v>
+      </c>
+      <c r="J1143">
+        <v>2.4504999999999999</v>
+      </c>
+      <c r="K1143">
+        <v>0</v>
+      </c>
+      <c r="L1143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1144" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1144" s="1" t="s">
+        <v>1854</v>
+      </c>
+      <c r="C1144" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1144" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1144" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1144">
+        <v>2</v>
+      </c>
+      <c r="G1144">
+        <v>2</v>
+      </c>
+      <c r="H1144">
+        <v>63514599635300.898</v>
+      </c>
+      <c r="I1144">
+        <v>0.1045</v>
+      </c>
+      <c r="J1144">
+        <v>1.0350999999999999</v>
+      </c>
+      <c r="K1144">
+        <v>0</v>
+      </c>
+      <c r="L1144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1145" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1145" s="1" t="s">
+        <v>1855</v>
+      </c>
+      <c r="C1145" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1145" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1145" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1145">
+        <v>0</v>
+      </c>
+      <c r="G1145">
+        <v>0</v>
+      </c>
+      <c r="H1145">
+        <v>63514599686604.797</v>
+      </c>
+      <c r="I1145">
+        <v>0.12039999999999999</v>
+      </c>
+      <c r="J1145">
+        <v>1.3849</v>
+      </c>
+      <c r="K1145">
+        <v>0</v>
+      </c>
+      <c r="L1145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1146" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1146" s="1" t="s">
+        <v>1856</v>
+      </c>
+      <c r="C1146" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1146" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1146" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1146">
+        <v>0</v>
+      </c>
+      <c r="G1146">
+        <v>1</v>
+      </c>
+      <c r="H1146">
+        <v>5168.2956000000004</v>
+      </c>
+      <c r="I1146">
+        <v>0.1048</v>
+      </c>
+      <c r="J1146">
+        <v>1.0407999999999999</v>
+      </c>
+      <c r="K1146">
+        <v>0</v>
+      </c>
+      <c r="L1146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1147" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1147" s="1" t="s">
+        <v>1857</v>
+      </c>
+      <c r="C1147" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1147" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1147" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1147">
+        <v>0</v>
+      </c>
+      <c r="G1147">
+        <v>2</v>
+      </c>
+      <c r="H1147">
+        <v>11667.6674</v>
+      </c>
+      <c r="I1147">
+        <v>0.52969999999999995</v>
+      </c>
+      <c r="J1147">
+        <v>0.38979999999999998</v>
+      </c>
+      <c r="K1147">
+        <v>0</v>
+      </c>
+      <c r="L1147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1148" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1148" s="1" t="s">
+        <v>1858</v>
+      </c>
+      <c r="C1148" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1148" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1148" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1148">
+        <v>1</v>
+      </c>
+      <c r="G1148">
+        <v>0</v>
+      </c>
+      <c r="H1148">
+        <v>3972.2271999999998</v>
+      </c>
+      <c r="I1148">
+        <v>5.2600000000000001E-2</v>
+      </c>
+      <c r="J1148">
+        <v>0.1842</v>
+      </c>
+      <c r="K1148">
+        <v>0</v>
+      </c>
+      <c r="L1148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1149" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1149" s="1" t="s">
+        <v>1859</v>
+      </c>
+      <c r="C1149" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1149" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1149" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1149">
+        <v>1</v>
+      </c>
+      <c r="G1149">
+        <v>1</v>
+      </c>
+      <c r="H1149">
+        <v>7899.4517999999998</v>
+      </c>
+      <c r="I1149">
+        <v>0.24790000000000001</v>
+      </c>
+      <c r="J1149">
+        <v>1.0769</v>
+      </c>
+      <c r="K1149">
+        <v>0</v>
+      </c>
+      <c r="L1149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1150" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1150" s="1" t="s">
+        <v>1860</v>
+      </c>
+      <c r="C1150" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1150" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1150" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1150">
+        <v>1</v>
+      </c>
+      <c r="G1150">
+        <v>2</v>
+      </c>
+      <c r="H1150">
+        <v>5220.2986000000001</v>
+      </c>
+      <c r="I1150">
+        <v>0.21640000000000001</v>
+      </c>
+      <c r="J1150">
+        <v>0.20250000000000001</v>
+      </c>
+      <c r="K1150">
+        <v>0</v>
+      </c>
+      <c r="L1150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1151" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1151" s="1" t="s">
+        <v>1861</v>
+      </c>
+      <c r="C1151" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1151" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1151" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1151">
+        <v>2</v>
+      </c>
+      <c r="G1151">
+        <v>0</v>
+      </c>
+      <c r="H1151">
+        <v>6947.3973999999998</v>
+      </c>
+      <c r="I1151">
+        <v>0.36459999999999998</v>
+      </c>
+      <c r="J1151">
+        <v>0.97540000000000004</v>
+      </c>
+      <c r="K1151">
+        <v>0</v>
+      </c>
+      <c r="L1151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1152" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1152" s="1" t="s">
+        <v>1862</v>
+      </c>
+      <c r="C1152" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1152" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1152" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1152">
+        <v>2</v>
+      </c>
+      <c r="G1152">
+        <v>1</v>
+      </c>
+      <c r="H1152">
+        <v>1688.0965000000001</v>
+      </c>
+      <c r="I1152">
+        <v>0.2656</v>
+      </c>
+      <c r="J1152">
+        <v>1.5812999999999999</v>
+      </c>
+      <c r="K1152">
+        <v>0</v>
+      </c>
+      <c r="L1152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1153" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1153" s="1" t="s">
+        <v>1863</v>
+      </c>
+      <c r="C1153" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1153" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1153" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1153">
+        <v>2</v>
+      </c>
+      <c r="G1153">
+        <v>2</v>
+      </c>
+      <c r="H1153">
+        <v>7476.4276</v>
+      </c>
+      <c r="I1153">
+        <v>0.4829</v>
+      </c>
+      <c r="J1153">
+        <v>0.57869999999999999</v>
+      </c>
+      <c r="K1153">
+        <v>0</v>
+      </c>
+      <c r="L1153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1154" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1154" s="1" t="s">
+        <v>1864</v>
+      </c>
+      <c r="C1154" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1154" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1154" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1154">
+        <v>0</v>
+      </c>
+      <c r="G1154">
+        <v>0</v>
+      </c>
+      <c r="H1154">
+        <v>39699.270700000001</v>
+      </c>
+      <c r="I1154">
+        <v>0.14480000000000001</v>
+      </c>
+      <c r="J1154">
+        <v>0.39650000000000002</v>
+      </c>
+      <c r="K1154">
+        <v>0</v>
+      </c>
+      <c r="L1154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1155" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1155" s="1" t="s">
+        <v>1865</v>
+      </c>
+      <c r="C1155" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1155" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1155" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1155">
+        <v>0</v>
+      </c>
+      <c r="G1155">
+        <v>1</v>
+      </c>
+      <c r="H1155">
+        <v>2016.1152999999999</v>
+      </c>
+      <c r="I1155">
+        <v>0.16109999999999999</v>
+      </c>
+      <c r="J1155">
+        <v>1.6273</v>
+      </c>
+      <c r="K1155">
+        <v>0</v>
+      </c>
+      <c r="L1155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1156" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1156" s="1" t="s">
+        <v>1866</v>
+      </c>
+      <c r="C1156" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1156" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1156" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1156">
+        <v>0</v>
+      </c>
+      <c r="G1156">
+        <v>2</v>
+      </c>
+      <c r="H1156">
+        <v>1394.0797</v>
+      </c>
+      <c r="I1156">
+        <v>0.16259999999999999</v>
+      </c>
+      <c r="J1156">
+        <v>0.78480000000000005</v>
+      </c>
+      <c r="K1156">
+        <v>0</v>
+      </c>
+      <c r="L1156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1157" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1157" s="1" t="s">
+        <v>1867</v>
+      </c>
+      <c r="C1157" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1157" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1157" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1157">
+        <v>1</v>
+      </c>
+      <c r="G1157">
+        <v>0</v>
+      </c>
+      <c r="H1157">
+        <v>2028.116</v>
+      </c>
+      <c r="I1157">
+        <v>0.1638</v>
+      </c>
+      <c r="J1157">
+        <v>0.94389999999999996</v>
+      </c>
+      <c r="K1157">
+        <v>0</v>
+      </c>
+      <c r="L1157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1158" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1158" s="1" t="s">
+        <v>1868</v>
+      </c>
+      <c r="C1158" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1158" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1158" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1158">
+        <v>1</v>
+      </c>
+      <c r="G1158">
+        <v>1</v>
+      </c>
+      <c r="H1158">
+        <v>5943.34</v>
+      </c>
+      <c r="I1158">
+        <v>0.19839999999999999</v>
+      </c>
+      <c r="J1158">
+        <v>0.3982</v>
+      </c>
+      <c r="K1158">
+        <v>0</v>
+      </c>
+      <c r="L1158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1159" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1159" s="1" t="s">
+        <v>1869</v>
+      </c>
+      <c r="C1159" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1159" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1159" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1159">
+        <v>1</v>
+      </c>
+      <c r="G1159">
+        <v>2</v>
+      </c>
+      <c r="H1159">
+        <v>5856.335</v>
+      </c>
+      <c r="I1159">
+        <v>0.17549999999999999</v>
+      </c>
+      <c r="J1159">
+        <v>0.15890000000000001</v>
+      </c>
+      <c r="K1159">
+        <v>0</v>
+      </c>
+      <c r="L1159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1160" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1160" s="1" t="s">
+        <v>1870</v>
+      </c>
+      <c r="C1160" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1160" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1160" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1160">
+        <v>2</v>
+      </c>
+      <c r="G1160">
+        <v>0</v>
+      </c>
+      <c r="H1160">
+        <v>5163.2952999999998</v>
+      </c>
+      <c r="I1160">
+        <v>0.1648</v>
+      </c>
+      <c r="J1160">
+        <v>1.6686000000000001</v>
+      </c>
+      <c r="K1160">
+        <v>0</v>
+      </c>
+      <c r="L1160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1161" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1161" s="1" t="s">
+        <v>1871</v>
+      </c>
+      <c r="C1161" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1161" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1161" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1161">
+        <v>2</v>
+      </c>
+      <c r="G1161">
+        <v>1</v>
+      </c>
+      <c r="H1161">
+        <v>6731.3851000000004</v>
+      </c>
+      <c r="I1161">
+        <v>0.1217</v>
+      </c>
+      <c r="J1161">
+        <v>1.4767999999999999</v>
+      </c>
+      <c r="K1161">
+        <v>0</v>
+      </c>
+      <c r="L1161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1162" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1162" s="1" t="s">
+        <v>1872</v>
+      </c>
+      <c r="C1162" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1162" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1162" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1162">
+        <v>2</v>
+      </c>
+      <c r="G1162">
+        <v>2</v>
+      </c>
+      <c r="H1162">
+        <v>1484.0849000000001</v>
+      </c>
+      <c r="I1162">
+        <v>8.9800000000000005E-2</v>
+      </c>
+      <c r="J1162">
+        <v>0.39269999999999999</v>
+      </c>
+      <c r="K1162">
+        <v>0</v>
+      </c>
+      <c r="L1162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1163" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1163" s="1" t="s">
+        <v>1873</v>
+      </c>
+      <c r="C1163" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1163" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1163" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1163">
+        <v>0</v>
+      </c>
+      <c r="G1163">
+        <v>0</v>
+      </c>
+      <c r="H1163">
+        <v>49058.805999999997</v>
+      </c>
+      <c r="I1163">
+        <v>6.54E-2</v>
+      </c>
+      <c r="J1163">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="K1163">
+        <v>2.0533000000000001</v>
+      </c>
+      <c r="L1163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1164" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1164" s="1" t="s">
+        <v>1874</v>
+      </c>
+      <c r="C1164" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1164" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1164" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1164">
+        <v>0</v>
+      </c>
+      <c r="G1164">
+        <v>1</v>
+      </c>
+      <c r="H1164">
+        <v>21431.2258</v>
+      </c>
+      <c r="I1164">
+        <v>0.04</v>
+      </c>
+      <c r="J1164">
+        <v>0.13009999999999999</v>
+      </c>
+      <c r="K1164">
+        <v>2.387</v>
+      </c>
+      <c r="L1164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1165" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1165" s="1" t="s">
+        <v>1875</v>
+      </c>
+      <c r="C1165" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1165" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1165" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1165">
+        <v>0</v>
+      </c>
+      <c r="G1165">
+        <v>2</v>
+      </c>
+      <c r="H1165">
+        <v>9371.5360999999994</v>
+      </c>
+      <c r="I1165">
+        <v>9.3399999999999997E-2</v>
+      </c>
+      <c r="J1165">
+        <v>1.0324</v>
+      </c>
+      <c r="K1165">
+        <v>2.4087999999999998</v>
+      </c>
+      <c r="L1165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1166" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1166" s="1" t="s">
+        <v>1876</v>
+      </c>
+      <c r="C1166" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1166" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1166" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1166">
+        <v>1</v>
+      </c>
+      <c r="G1166">
+        <v>0</v>
+      </c>
+      <c r="H1166">
+        <v>15294.8748</v>
+      </c>
+      <c r="I1166">
+        <v>0.19589999999999999</v>
+      </c>
+      <c r="J1166">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="K1166">
+        <v>1.9801</v>
+      </c>
+      <c r="L1166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1167" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1167" s="1" t="s">
+        <v>1877</v>
+      </c>
+      <c r="C1167" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1167" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1167" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1167">
+        <v>1</v>
+      </c>
+      <c r="G1167">
+        <v>1</v>
+      </c>
+      <c r="H1167">
+        <v>17975.0281</v>
+      </c>
+      <c r="I1167">
+        <v>0.113</v>
+      </c>
+      <c r="J1167">
+        <v>4.2672999999999996</v>
+      </c>
+      <c r="K1167">
+        <v>2.1246</v>
+      </c>
+      <c r="L1167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1168" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1168" s="1" t="s">
+        <v>1878</v>
+      </c>
+      <c r="C1168" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1168" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1168" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1168">
+        <v>1</v>
+      </c>
+      <c r="G1168">
+        <v>2</v>
+      </c>
+      <c r="H1168">
+        <v>16651.952499999999</v>
+      </c>
+      <c r="I1168">
+        <v>0</v>
+      </c>
+      <c r="J1168">
+        <v>0.54830000000000001</v>
+      </c>
+      <c r="K1168">
+        <v>1.8923000000000001</v>
+      </c>
+      <c r="L1168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1169" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1169" s="1" t="s">
+        <v>1879</v>
+      </c>
+      <c r="C1169" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1169" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1169" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1169">
+        <v>2</v>
+      </c>
+      <c r="G1169">
+        <v>0</v>
+      </c>
+      <c r="H1169">
+        <v>19932.140100000001</v>
+      </c>
+      <c r="I1169">
+        <v>2.9600000000000001E-2</v>
+      </c>
+      <c r="J1169">
+        <v>0.19489999999999999</v>
+      </c>
+      <c r="K1169">
+        <v>1.8755999999999999</v>
+      </c>
+      <c r="L1169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1170" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1170" s="1" t="s">
+        <v>1880</v>
+      </c>
+      <c r="C1170" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1170" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1170" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1170">
+        <v>2</v>
+      </c>
+      <c r="G1170">
+        <v>1</v>
+      </c>
+      <c r="H1170">
+        <v>15591.891799999999</v>
+      </c>
+      <c r="I1170">
+        <v>6.4399999999999999E-2</v>
+      </c>
+      <c r="J1170">
+        <v>0.69820000000000004</v>
+      </c>
+      <c r="K1170">
+        <v>1.7923</v>
+      </c>
+      <c r="L1170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1171" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1171" s="1" t="s">
+        <v>1881</v>
+      </c>
+      <c r="C1171" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1171" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1171" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1171">
+        <v>2</v>
+      </c>
+      <c r="G1171">
+        <v>2</v>
+      </c>
+      <c r="H1171">
+        <v>13331.762500000001</v>
+      </c>
+      <c r="I1171">
+        <v>7.5499999999999998E-2</v>
+      </c>
+      <c r="J1171">
+        <v>1.5657000000000001</v>
+      </c>
+      <c r="K1171">
+        <v>2.2284000000000002</v>
+      </c>
+      <c r="L1171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1172" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1172" s="1" t="s">
+        <v>1882</v>
+      </c>
+      <c r="C1172" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1172" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1172" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1172">
+        <v>0</v>
+      </c>
+      <c r="G1172">
+        <v>0</v>
+      </c>
+      <c r="H1172">
+        <v>30850.764599999999</v>
+      </c>
+      <c r="I1172">
+        <v>0.31359999999999999</v>
+      </c>
+      <c r="J1172">
+        <v>1.0989</v>
+      </c>
+      <c r="K1172">
+        <v>1.8066</v>
+      </c>
+      <c r="L1172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1173" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1173" s="1" t="s">
+        <v>1883</v>
+      </c>
+      <c r="C1173" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1173" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1173" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1173">
+        <v>0</v>
+      </c>
+      <c r="G1173">
+        <v>1</v>
+      </c>
+      <c r="H1173">
+        <v>24427.397199999999</v>
+      </c>
+      <c r="I1173">
+        <v>9.35E-2</v>
+      </c>
+      <c r="J1173">
+        <v>2.5817000000000001</v>
+      </c>
+      <c r="K1173">
+        <v>1.4041999999999999</v>
+      </c>
+      <c r="L1173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1174" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1174" s="1" t="s">
+        <v>1884</v>
+      </c>
+      <c r="C1174" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1174" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1174" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1174">
+        <v>0</v>
+      </c>
+      <c r="G1174">
+        <v>2</v>
+      </c>
+      <c r="H1174">
+        <v>10935.6255</v>
+      </c>
+      <c r="I1174">
+        <v>0.55959999999999999</v>
+      </c>
+      <c r="J1174">
+        <v>2.1598000000000002</v>
+      </c>
+      <c r="K1174">
+        <v>1.9094</v>
+      </c>
+      <c r="L1174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1175" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1175" s="1" t="s">
+        <v>1885</v>
+      </c>
+      <c r="C1175" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1175" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1175" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1175">
+        <v>1</v>
+      </c>
+      <c r="G1175">
+        <v>0</v>
+      </c>
+      <c r="H1175">
+        <v>18437.054599999999</v>
+      </c>
+      <c r="I1175">
+        <v>0.32819999999999999</v>
+      </c>
+      <c r="J1175">
+        <v>1.4955000000000001</v>
+      </c>
+      <c r="K1175">
+        <v>1.8138000000000001</v>
+      </c>
+      <c r="L1175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1176" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1176" s="1" t="s">
+        <v>1886</v>
+      </c>
+      <c r="C1176" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1176" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1176" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1176">
+        <v>1</v>
+      </c>
+      <c r="G1176">
+        <v>1</v>
+      </c>
+      <c r="H1176">
+        <v>7179.4106000000002</v>
+      </c>
+      <c r="I1176">
+        <v>0.221</v>
+      </c>
+      <c r="J1176">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="K1176">
+        <v>1.5224</v>
+      </c>
+      <c r="L1176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1177" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1177" s="1" t="s">
+        <v>1887</v>
+      </c>
+      <c r="C1177" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1177" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1177" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1177">
+        <v>1</v>
+      </c>
+      <c r="G1177">
+        <v>2</v>
+      </c>
+      <c r="H1177">
+        <v>5643.3227999999999</v>
+      </c>
+      <c r="I1177">
+        <v>0.33160000000000001</v>
+      </c>
+      <c r="J1177">
+        <v>1.4698</v>
+      </c>
+      <c r="K1177">
+        <v>1.5650999999999999</v>
+      </c>
+      <c r="L1177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1178" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1178" s="1" t="s">
+        <v>1888</v>
+      </c>
+      <c r="C1178" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1178" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1178" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1178">
+        <v>2</v>
+      </c>
+      <c r="G1178">
+        <v>0</v>
+      </c>
+      <c r="H1178">
+        <v>6563.3753999999999</v>
+      </c>
+      <c r="I1178">
+        <v>0.26529999999999998</v>
+      </c>
+      <c r="J1178">
+        <v>1.5189999999999999</v>
+      </c>
+      <c r="K1178">
+        <v>1.6500999999999999</v>
+      </c>
+      <c r="L1178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1179" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1179" s="1" t="s">
+        <v>1889</v>
+      </c>
+      <c r="C1179" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1179" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1179" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1179">
+        <v>2</v>
+      </c>
+      <c r="G1179">
+        <v>1</v>
+      </c>
+      <c r="H1179">
+        <v>5851.3347000000003</v>
+      </c>
+      <c r="I1179">
+        <v>0.26050000000000001</v>
+      </c>
+      <c r="J1179">
+        <v>2.6818</v>
+      </c>
+      <c r="K1179">
+        <v>1.7289000000000001</v>
+      </c>
+      <c r="L1179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1180" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1180" s="1" t="s">
+        <v>1890</v>
+      </c>
+      <c r="C1180" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1180" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1180" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1180">
+        <v>2</v>
+      </c>
+      <c r="G1180">
+        <v>2</v>
+      </c>
+      <c r="H1180">
+        <v>14287.817300000001</v>
+      </c>
+      <c r="I1180">
+        <v>0.1953</v>
+      </c>
+      <c r="J1180">
+        <v>1.1308</v>
+      </c>
+      <c r="K1180">
+        <v>1.4472</v>
+      </c>
+      <c r="L1180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1181" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1181" s="1" t="s">
+        <v>1891</v>
+      </c>
+      <c r="C1181" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1181" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1181" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1181">
+        <v>0</v>
+      </c>
+      <c r="G1181">
+        <v>0</v>
+      </c>
+      <c r="H1181">
+        <v>17976.028200000001</v>
+      </c>
+      <c r="I1181">
+        <v>0.18840000000000001</v>
+      </c>
+      <c r="J1181">
+        <v>2.1355</v>
+      </c>
+      <c r="K1181">
+        <v>2.0266999999999999</v>
+      </c>
+      <c r="L1181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1182" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1182" s="1" t="s">
+        <v>1892</v>
+      </c>
+      <c r="C1182" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1182" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1182" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1182">
+        <v>0</v>
+      </c>
+      <c r="G1182">
+        <v>1</v>
+      </c>
+      <c r="H1182">
+        <v>8011.4583000000002</v>
+      </c>
+      <c r="I1182">
+        <v>0.6774</v>
+      </c>
+      <c r="J1182">
+        <v>1.3396999999999999</v>
+      </c>
+      <c r="K1182">
+        <v>2.3287</v>
+      </c>
+      <c r="L1182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1183" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1183" s="1" t="s">
+        <v>1893</v>
+      </c>
+      <c r="C1183" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1183" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1183" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1183">
+        <v>0</v>
+      </c>
+      <c r="G1183">
+        <v>2</v>
+      </c>
+      <c r="H1183">
+        <v>24447.398399999998</v>
+      </c>
+      <c r="I1183">
+        <v>0.31690000000000002</v>
+      </c>
+      <c r="J1183">
+        <v>0.79569999999999996</v>
+      </c>
+      <c r="K1183">
+        <v>1.4804999999999999</v>
+      </c>
+      <c r="L1183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1184" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1184" s="1" t="s">
+        <v>1894</v>
+      </c>
+      <c r="C1184" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1184" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1184" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1184">
+        <v>1</v>
+      </c>
+      <c r="G1184">
+        <v>0</v>
+      </c>
+      <c r="H1184">
+        <v>14356.8212</v>
+      </c>
+      <c r="I1184">
+        <v>9.2100000000000001E-2</v>
+      </c>
+      <c r="J1184">
+        <v>2.4127000000000001</v>
+      </c>
+      <c r="K1184">
+        <v>1.9744999999999999</v>
+      </c>
+      <c r="L1184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1185" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1185" s="1" t="s">
+        <v>1895</v>
+      </c>
+      <c r="C1185" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1185" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1185" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1185">
+        <v>1</v>
+      </c>
+      <c r="G1185">
+        <v>1</v>
+      </c>
+      <c r="H1185">
+        <v>15446.8835</v>
+      </c>
+      <c r="I1185">
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="J1185">
+        <v>4.3510999999999997</v>
+      </c>
+      <c r="K1185">
+        <v>1.7978000000000001</v>
+      </c>
+      <c r="L1185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1186" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1186" s="1" t="s">
+        <v>1896</v>
+      </c>
+      <c r="C1186" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1186" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1186" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1186">
+        <v>1</v>
+      </c>
+      <c r="G1186">
+        <v>2</v>
+      </c>
+      <c r="H1186">
+        <v>5620.3215</v>
+      </c>
+      <c r="I1186">
+        <v>4.7300000000000002E-2</v>
+      </c>
+      <c r="J1186">
+        <v>1.0818000000000001</v>
+      </c>
+      <c r="K1186">
+        <v>1.8125</v>
+      </c>
+      <c r="L1186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1187" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1187" s="1" t="s">
+        <v>1897</v>
+      </c>
+      <c r="C1187" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1187" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1187" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1187">
+        <v>2</v>
+      </c>
+      <c r="G1187">
+        <v>0</v>
+      </c>
+      <c r="H1187">
+        <v>13407.766900000001</v>
+      </c>
+      <c r="I1187">
+        <v>9.6600000000000005E-2</v>
+      </c>
+      <c r="J1187">
+        <v>0.1055</v>
+      </c>
+      <c r="K1187">
+        <v>1.6762999999999999</v>
+      </c>
+      <c r="L1187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1188" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1188" s="1" t="s">
+        <v>1898</v>
+      </c>
+      <c r="C1188" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1188" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1188" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1188">
+        <v>2</v>
+      </c>
+      <c r="G1188">
+        <v>1</v>
+      </c>
+      <c r="H1188">
+        <v>12635.7227</v>
+      </c>
+      <c r="I1188">
+        <v>9.1300000000000006E-2</v>
+      </c>
+      <c r="J1188">
+        <v>3.1884999999999999</v>
+      </c>
+      <c r="K1188">
+        <v>1.5885</v>
+      </c>
+      <c r="L1188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1189" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1189" s="1" t="s">
+        <v>1899</v>
+      </c>
+      <c r="C1189" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1189" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1189" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1189">
+        <v>2</v>
+      </c>
+      <c r="G1189">
+        <v>2</v>
+      </c>
+      <c r="H1189">
+        <v>7776.4448000000002</v>
+      </c>
+      <c r="I1189">
+        <v>0.1595</v>
+      </c>
+      <c r="J1189">
+        <v>1.7444</v>
+      </c>
+      <c r="K1189">
+        <v>1.8008999999999999</v>
+      </c>
+      <c r="L1189">
         <v>0</v>
       </c>
     </row>

</xml_diff>